<commit_message>
about to mess with enrollment to try and clean it up.
</commit_message>
<xml_diff>
--- a/Local Historic Crosswalk.xlsx
+++ b/Local Historic Crosswalk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasontheisen/Documents/Advance Illinois/Historic Report Card/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA87F33-D734-C548-B949-91281C3A6CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF73BFB7-98ED-8A4A-8BA9-0AB2FD030F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="77">
   <si>
     <t>Year</t>
   </si>
@@ -321,6 +321,141 @@
   </si>
   <si>
     <t>DISTRICT TYPE NAME</t>
+  </si>
+  <si>
+    <t>Total Teacher FTE</t>
+  </si>
+  <si>
+    <t>TOTAL TEACH FTE COUNT- DISTRICT</t>
+  </si>
+  <si>
+    <t>TOTAL TEACH FTE COUNT- DISTRICT - Coming Soon</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Disaggregation follows format: "% Teachers - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>demo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Disaggregation follows format: "% of Teachers - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>demo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Disaggregation follows format: "% </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TEACHER - DISTRICT"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Disaggregation follows format: "% </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TEACH - DISTRICT"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Disaggregation follows format: "% </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEMO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TEACHER - DISTRICT - Coming Soon"</t>
+    </r>
+  </si>
+  <si>
+    <t>Teacher Retention Rate</t>
+  </si>
+  <si>
+    <t>TEACHER RETENTION RATE (SCHOOL)</t>
   </si>
 </sst>
 </file>
@@ -456,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -471,11 +606,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="25">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -531,6 +670,20 @@
           <color theme="4" tint="0.39997558519241921"/>
         </right>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -793,43 +946,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}" name="Table1" displayName="Table1" ref="A1:M18" totalsRowShown="0" dataDxfId="22">
-  <autoFilter ref="A1:M18" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{6DA6945B-9D7D-0142-A374-7C4A97BBBBAB}" name="Year" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{1617EDAF-51CD-413F-9022-F6E4C97C233F}" name="RCDTS" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{A67D85A4-5303-744E-B7CD-31ECBC6CE0A7}" name="Type" dataDxfId="19"/>
-    <tableColumn id="13" xr3:uid="{C8F50192-B0A1-D84D-96D9-819955E9CE26}" name="District Type" dataDxfId="18"/>
-    <tableColumn id="14" xr3:uid="{A7661728-A363-9840-8182-CBC0352B14C6}" name="School Type" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{94336B41-A312-184A-9F00-C5E1720E28AF}" name="School Name" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{7516DA0D-E868-1941-B0D3-80B0E523A018}" name="District Name" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{DCD59F4B-C55C-2846-9070-7F8CC6CA2F51}" name="City" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{AB642454-853E-F049-84B7-745455B992F3}" name="County" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{5B5F7B45-CEFB-EE48-90E0-380BD11BD347}" name="Student Enrollment" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{DC5BC21C-5B26-D441-96D3-64D606494C9A}" name="Student Attendance Rate" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{16C5B399-2D53-AF41-815C-1F7C3259622D}" name="Chronic Truancy Rate" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{E3173650-9CBD-2046-9561-EC76593F21A4}" name="Chronic Absenteeism" dataDxfId="9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}" name="Table1" displayName="Table1" ref="A1:O18" totalsRowShown="0" dataDxfId="24">
+  <autoFilter ref="A1:O18" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O18">
+    <sortCondition ref="A1:A18"/>
+  </sortState>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{6DA6945B-9D7D-0142-A374-7C4A97BBBBAB}" name="Year" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{1617EDAF-51CD-413F-9022-F6E4C97C233F}" name="RCDTS" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{A67D85A4-5303-744E-B7CD-31ECBC6CE0A7}" name="Type" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{C8F50192-B0A1-D84D-96D9-819955E9CE26}" name="District Type" dataDxfId="20"/>
+    <tableColumn id="14" xr3:uid="{A7661728-A363-9840-8182-CBC0352B14C6}" name="School Type" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{94336B41-A312-184A-9F00-C5E1720E28AF}" name="School Name" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{7516DA0D-E868-1941-B0D3-80B0E523A018}" name="District Name" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{DCD59F4B-C55C-2846-9070-7F8CC6CA2F51}" name="City" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{AB642454-853E-F049-84B7-745455B992F3}" name="County" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{5B5F7B45-CEFB-EE48-90E0-380BD11BD347}" name="Student Enrollment" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{DC5BC21C-5B26-D441-96D3-64D606494C9A}" name="Student Attendance Rate" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{16C5B399-2D53-AF41-815C-1F7C3259622D}" name="Chronic Truancy Rate" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{E3173650-9CBD-2046-9561-EC76593F21A4}" name="Chronic Absenteeism" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{A5C89E32-E6C7-354A-AD94-8B9E7BF5BEAF}" name="Total Teacher FTE" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{91CEEB72-10AD-5347-AD91-C2EA26951FFD}" name="Teacher Retention Rate" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{07EA3C7D-22C7-3142-BED0-4051FC9CF2E2}" name="Table4" displayName="Table4" ref="A1:G173" totalsRowShown="0" dataDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="A1:G173" xr:uid="{07EA3C7D-22C7-3142-BED0-4051FC9CF2E2}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="District Type"/>
-        <filter val="DISTRICT TYPE NAME"/>
-        <filter val="School Type"/>
-        <filter val="SCHOOL TYPE NAME"/>
-        <filter val="Type"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:G173">
-    <sortCondition ref="A1:A173"/>
-  </sortState>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{07EA3C7D-22C7-3142-BED0-4051FC9CF2E2}" name="Table4" displayName="Table4" ref="A1:G199" totalsRowShown="0" dataDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A1:G199" xr:uid="{07EA3C7D-22C7-3142-BED0-4051FC9CF2E2}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{DD0B638C-4311-0744-95CB-52513DBACE2D}" name="Year" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{26FE4BE8-2ADC-0040-8E5B-EA972212A95A}" name="Metric" dataDxfId="5"/>
@@ -1473,11 +1618,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K2" sqref="K2"/>
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1495,9 +1640,11 @@
     <col min="11" max="11" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="28.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1537,256 +1684,250 @@
       <c r="M1" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2023</v>
+        <v>2008</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>64</v>
+        <v>28</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J2" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="K2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2022</v>
+        <v>2009</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>64</v>
+        <v>28</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J3" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="K3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="N3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2021</v>
+        <v>2010</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>64</v>
+        <v>28</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J4" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="N4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2020</v>
+        <v>2011</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>64</v>
+        <v>28</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J5" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="N5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2019</v>
+        <v>2012</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>64</v>
+        <v>28</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J6" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="K6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L6" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="N6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>64</v>
+        <v>28</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I7" t="s">
-        <v>62</v>
-      </c>
-      <c r="J7" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="K7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="N7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>28</v>
@@ -1819,10 +1960,16 @@
       <c r="L8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>28</v>
@@ -1855,10 +2002,16 @@
       <c r="L9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" t="s">
+        <v>68</v>
+      </c>
+      <c r="O9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>28</v>
@@ -1891,10 +2044,16 @@
       <c r="L10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" t="s">
+        <v>68</v>
+      </c>
+      <c r="O10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>28</v>
@@ -1927,224 +2086,296 @@
       <c r="L11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" t="s">
+        <v>68</v>
+      </c>
+      <c r="O11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2013</v>
+        <v>2018</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>65</v>
+        <v>23</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
+      </c>
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" t="s">
+        <v>48</v>
       </c>
       <c r="K12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="M12" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" t="s">
+        <v>67</v>
+      </c>
+      <c r="O12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2012</v>
+        <v>2019</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>65</v>
+        <v>23</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
+      </c>
+      <c r="G13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" t="s">
+        <v>50</v>
       </c>
       <c r="K13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="M13" t="s">
+        <v>25</v>
+      </c>
+      <c r="N13" t="s">
+        <v>67</v>
+      </c>
+      <c r="O13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2011</v>
+        <v>2020</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>65</v>
+        <v>23</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
+      </c>
+      <c r="G14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" t="s">
+        <v>50</v>
       </c>
       <c r="K14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="M14" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" t="s">
+        <v>67</v>
+      </c>
+      <c r="O14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>2010</v>
+        <v>2021</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>65</v>
+        <v>23</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
+      </c>
+      <c r="G15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" t="s">
+        <v>62</v>
+      </c>
+      <c r="J15" t="s">
+        <v>50</v>
       </c>
       <c r="K15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="M15" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" t="s">
+        <v>67</v>
+      </c>
+      <c r="O15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>2009</v>
+        <v>2022</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>65</v>
+        <v>23</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
+      </c>
+      <c r="G16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J16" t="s">
+        <v>50</v>
       </c>
       <c r="K16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="M16" t="s">
+        <v>25</v>
+      </c>
+      <c r="N16" t="s">
+        <v>67</v>
+      </c>
+      <c r="O16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>2008</v>
+        <v>2023</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>65</v>
+        <v>23</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
+      </c>
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" t="s">
+        <v>50</v>
       </c>
       <c r="K17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="M17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N17" t="s">
+        <v>67</v>
+      </c>
+      <c r="O17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -2166,15 +2397,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249B090D-D7BB-374A-9D81-FFCE8C0599DD}">
-  <dimension ref="A1:G173"/>
+  <dimension ref="A1:G199"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="167" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A158" zoomScale="150" zoomScaleNormal="167" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A162" sqref="A162"/>
+      <selection pane="topRight" activeCell="C179" sqref="C179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="52.6640625" customWidth="1"/>
@@ -2204,7 +2437,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2008</v>
       </c>
@@ -2221,7 +2454,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2008</v>
       </c>
@@ -2235,7 +2468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2008</v>
       </c>
@@ -2250,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2008</v>
       </c>
@@ -2264,7 +2497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2008</v>
       </c>
@@ -2292,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2008</v>
       </c>
@@ -2315,7 +2548,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2008</v>
       </c>
@@ -2329,7 +2562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2008</v>
       </c>
@@ -2357,7 +2590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2009</v>
       </c>
@@ -2374,7 +2607,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2009</v>
       </c>
@@ -2388,7 +2621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2009</v>
       </c>
@@ -2403,7 +2636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2009</v>
       </c>
@@ -2417,7 +2650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2009</v>
       </c>
@@ -2445,7 +2678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2009</v>
       </c>
@@ -2468,7 +2701,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2009</v>
       </c>
@@ -2482,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2009</v>
       </c>
@@ -2510,7 +2743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2010</v>
       </c>
@@ -2527,7 +2760,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2010</v>
       </c>
@@ -2541,7 +2774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2010</v>
       </c>
@@ -2556,7 +2789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2010</v>
       </c>
@@ -2570,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2010</v>
       </c>
@@ -2598,7 +2831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2010</v>
       </c>
@@ -2621,7 +2854,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2010</v>
       </c>
@@ -2635,7 +2868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2010</v>
       </c>
@@ -2663,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2011</v>
       </c>
@@ -2680,7 +2913,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2011</v>
       </c>
@@ -2694,7 +2927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2011</v>
       </c>
@@ -2709,7 +2942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2011</v>
       </c>
@@ -2723,7 +2956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2011</v>
       </c>
@@ -2751,7 +2984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2011</v>
       </c>
@@ -2774,7 +3007,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2011</v>
       </c>
@@ -2788,7 +3021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2011</v>
       </c>
@@ -2816,7 +3049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2012</v>
       </c>
@@ -2833,7 +3066,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2012</v>
       </c>
@@ -2847,7 +3080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2012</v>
       </c>
@@ -2862,7 +3095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2012</v>
       </c>
@@ -2876,7 +3109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2012</v>
       </c>
@@ -2904,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2012</v>
       </c>
@@ -2927,7 +3160,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2012</v>
       </c>
@@ -2941,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2012</v>
       </c>
@@ -2969,7 +3202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2013</v>
       </c>
@@ -2986,7 +3219,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2013</v>
       </c>
@@ -3000,7 +3233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2013</v>
       </c>
@@ -3015,7 +3248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2013</v>
       </c>
@@ -3029,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2013</v>
       </c>
@@ -3057,7 +3290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2013</v>
       </c>
@@ -3080,7 +3313,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2013</v>
       </c>
@@ -3094,7 +3327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2013</v>
       </c>
@@ -3122,7 +3355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2014</v>
       </c>
@@ -3139,7 +3372,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2014</v>
       </c>
@@ -3153,7 +3386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2014</v>
       </c>
@@ -3168,7 +3401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2014</v>
       </c>
@@ -3182,7 +3415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2014</v>
       </c>
@@ -3210,7 +3443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2014</v>
       </c>
@@ -3233,7 +3466,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2014</v>
       </c>
@@ -3247,7 +3480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2014</v>
       </c>
@@ -3275,7 +3508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2015</v>
       </c>
@@ -3292,7 +3525,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2015</v>
       </c>
@@ -3306,7 +3539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2015</v>
       </c>
@@ -3321,7 +3554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2015</v>
       </c>
@@ -3335,7 +3568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2015</v>
       </c>
@@ -3363,7 +3596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>2015</v>
       </c>
@@ -3386,7 +3619,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>2015</v>
       </c>
@@ -3400,7 +3633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>2015</v>
       </c>
@@ -3428,7 +3661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>2016</v>
       </c>
@@ -3445,7 +3678,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>2016</v>
       </c>
@@ -3459,7 +3692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>2016</v>
       </c>
@@ -3474,7 +3707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>2016</v>
       </c>
@@ -3488,7 +3721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>2016</v>
       </c>
@@ -3516,7 +3749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>2016</v>
       </c>
@@ -3539,7 +3772,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>2016</v>
       </c>
@@ -3553,7 +3786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>2016</v>
       </c>
@@ -3581,7 +3814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>2017</v>
       </c>
@@ -3598,7 +3831,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>2017</v>
       </c>
@@ -3612,7 +3845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>2017</v>
       </c>
@@ -3627,7 +3860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>2017</v>
       </c>
@@ -3641,7 +3874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>2017</v>
       </c>
@@ -3669,7 +3902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>2017</v>
       </c>
@@ -3692,7 +3925,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2017</v>
       </c>
@@ -3706,7 +3939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>2017</v>
       </c>
@@ -3734,7 +3967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>2018</v>
       </c>
@@ -3751,7 +3984,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>2018</v>
       </c>
@@ -3765,7 +3998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>2018</v>
       </c>
@@ -3779,7 +4012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>2018</v>
       </c>
@@ -3793,7 +4026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>2018</v>
       </c>
@@ -3821,7 +4054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>2018</v>
       </c>
@@ -3835,7 +4068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>2018</v>
       </c>
@@ -3849,7 +4082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>2018</v>
       </c>
@@ -3866,7 +4099,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>2018</v>
       </c>
@@ -3903,7 +4136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>2019</v>
       </c>
@@ -3923,7 +4156,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>2019</v>
       </c>
@@ -3940,7 +4173,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>2019</v>
       </c>
@@ -3954,7 +4187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>2019</v>
       </c>
@@ -3968,7 +4201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>2019</v>
       </c>
@@ -3982,7 +4215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>2019</v>
       </c>
@@ -4010,7 +4243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>2019</v>
       </c>
@@ -4024,7 +4257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>2019</v>
       </c>
@@ -4038,7 +4271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>2019</v>
       </c>
@@ -4066,7 +4299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>2020</v>
       </c>
@@ -4086,7 +4319,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>2020</v>
       </c>
@@ -4103,7 +4336,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>2020</v>
       </c>
@@ -4117,7 +4350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>2020</v>
       </c>
@@ -4131,7 +4364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>2020</v>
       </c>
@@ -4145,7 +4378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>2020</v>
       </c>
@@ -4173,7 +4406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>2020</v>
       </c>
@@ -4187,7 +4420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>2020</v>
       </c>
@@ -4201,7 +4434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>2020</v>
       </c>
@@ -4229,7 +4462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>2021</v>
       </c>
@@ -4249,7 +4482,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>2021</v>
       </c>
@@ -4266,7 +4499,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>2021</v>
       </c>
@@ -4280,7 +4513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>2021</v>
       </c>
@@ -4294,7 +4527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>2021</v>
       </c>
@@ -4308,7 +4541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>2021</v>
       </c>
@@ -4336,7 +4569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>2021</v>
       </c>
@@ -4350,7 +4583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>2021</v>
       </c>
@@ -4364,7 +4597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>2021</v>
       </c>
@@ -4392,7 +4625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>2022</v>
       </c>
@@ -4412,7 +4645,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>2022</v>
       </c>
@@ -4429,7 +4662,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>2022</v>
       </c>
@@ -4443,7 +4676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>2022</v>
       </c>
@@ -4457,7 +4690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>2022</v>
       </c>
@@ -4471,7 +4704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>2022</v>
       </c>
@@ -4499,7 +4732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>2022</v>
       </c>
@@ -4513,7 +4746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>2022</v>
       </c>
@@ -4527,7 +4760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>2022</v>
       </c>
@@ -4555,7 +4788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>2023</v>
       </c>
@@ -4575,7 +4808,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>2023</v>
       </c>
@@ -4592,7 +4825,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>2023</v>
       </c>
@@ -4606,7 +4839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>2023</v>
       </c>
@@ -4620,7 +4853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>2023</v>
       </c>
@@ -4634,7 +4867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>2023</v>
       </c>
@@ -4648,7 +4881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>2021</v>
       </c>
@@ -4662,7 +4895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>2023</v>
       </c>
@@ -4676,7 +4909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>2023</v>
       </c>
@@ -4690,7 +4923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>2023</v>
       </c>
@@ -4704,7 +4937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>2021</v>
       </c>
@@ -4718,7 +4951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" s="7">
         <v>2022</v>
       </c>
@@ -4732,7 +4965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" s="7">
         <v>2022</v>
       </c>
@@ -4746,7 +4979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" s="7">
         <v>2022</v>
       </c>
@@ -4760,7 +4993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" s="7">
         <v>2023</v>
       </c>
@@ -4774,7 +5007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" s="7">
         <v>2023</v>
       </c>
@@ -4788,7 +5021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" s="9">
         <v>2023</v>
       </c>
@@ -4799,6 +5032,467 @@
         <v>35</v>
       </c>
       <c r="E173" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>2008</v>
+      </c>
+      <c r="B174" t="s">
+        <v>68</v>
+      </c>
+      <c r="D174" t="s">
+        <v>38</v>
+      </c>
+      <c r="E174" t="b">
+        <v>1</v>
+      </c>
+      <c r="F174" t="s">
+        <v>54</v>
+      </c>
+      <c r="G174" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>2009</v>
+      </c>
+      <c r="B175" t="s">
+        <v>68</v>
+      </c>
+      <c r="D175" t="s">
+        <v>38</v>
+      </c>
+      <c r="E175" t="b">
+        <v>1</v>
+      </c>
+      <c r="F175" t="s">
+        <v>54</v>
+      </c>
+      <c r="G175" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>2010</v>
+      </c>
+      <c r="B176" t="s">
+        <v>68</v>
+      </c>
+      <c r="D176" t="s">
+        <v>38</v>
+      </c>
+      <c r="E176" t="b">
+        <v>1</v>
+      </c>
+      <c r="F176" t="s">
+        <v>54</v>
+      </c>
+      <c r="G176" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>2011</v>
+      </c>
+      <c r="B177" t="s">
+        <v>68</v>
+      </c>
+      <c r="D177" t="s">
+        <v>38</v>
+      </c>
+      <c r="E177" t="b">
+        <v>1</v>
+      </c>
+      <c r="F177" t="s">
+        <v>54</v>
+      </c>
+      <c r="G177" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>2012</v>
+      </c>
+      <c r="B178" t="s">
+        <v>68</v>
+      </c>
+      <c r="D178" t="s">
+        <v>38</v>
+      </c>
+      <c r="E178" t="b">
+        <v>1</v>
+      </c>
+      <c r="F178" t="s">
+        <v>54</v>
+      </c>
+      <c r="G178" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>2013</v>
+      </c>
+      <c r="B179" t="s">
+        <v>69</v>
+      </c>
+      <c r="C179" s="13"/>
+      <c r="D179" t="s">
+        <v>38</v>
+      </c>
+      <c r="E179" t="b">
+        <v>1</v>
+      </c>
+      <c r="F179" t="s">
+        <v>54</v>
+      </c>
+      <c r="G179" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>2014</v>
+      </c>
+      <c r="B180" t="s">
+        <v>68</v>
+      </c>
+      <c r="D180" t="s">
+        <v>38</v>
+      </c>
+      <c r="E180" t="b">
+        <v>1</v>
+      </c>
+      <c r="F180" t="s">
+        <v>54</v>
+      </c>
+      <c r="G180" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>2015</v>
+      </c>
+      <c r="B181" t="s">
+        <v>68</v>
+      </c>
+      <c r="D181" t="s">
+        <v>38</v>
+      </c>
+      <c r="E181" t="b">
+        <v>1</v>
+      </c>
+      <c r="F181" t="s">
+        <v>54</v>
+      </c>
+      <c r="G181" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>2016</v>
+      </c>
+      <c r="B182" t="s">
+        <v>68</v>
+      </c>
+      <c r="D182" t="s">
+        <v>38</v>
+      </c>
+      <c r="E182" t="b">
+        <v>1</v>
+      </c>
+      <c r="F182" t="s">
+        <v>54</v>
+      </c>
+      <c r="G182" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>2017</v>
+      </c>
+      <c r="B183" t="s">
+        <v>68</v>
+      </c>
+      <c r="D183" t="s">
+        <v>38</v>
+      </c>
+      <c r="E183" t="b">
+        <v>1</v>
+      </c>
+      <c r="F183" t="s">
+        <v>54</v>
+      </c>
+      <c r="G183" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>2018</v>
+      </c>
+      <c r="B184" t="s">
+        <v>67</v>
+      </c>
+      <c r="D184" t="s">
+        <v>35</v>
+      </c>
+      <c r="E184" t="b">
+        <v>1</v>
+      </c>
+      <c r="F184" t="s">
+        <v>54</v>
+      </c>
+      <c r="G184" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>2019</v>
+      </c>
+      <c r="B185" t="s">
+        <v>67</v>
+      </c>
+      <c r="D185" t="s">
+        <v>35</v>
+      </c>
+      <c r="E185" t="b">
+        <v>1</v>
+      </c>
+      <c r="F185" t="s">
+        <v>54</v>
+      </c>
+      <c r="G185" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>2020</v>
+      </c>
+      <c r="B186" t="s">
+        <v>67</v>
+      </c>
+      <c r="D186" t="s">
+        <v>35</v>
+      </c>
+      <c r="E186" t="b">
+        <v>1</v>
+      </c>
+      <c r="F186" t="s">
+        <v>54</v>
+      </c>
+      <c r="G186" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>2021</v>
+      </c>
+      <c r="B187" t="s">
+        <v>67</v>
+      </c>
+      <c r="D187" t="s">
+        <v>35</v>
+      </c>
+      <c r="E187" t="b">
+        <v>1</v>
+      </c>
+      <c r="F187" t="s">
+        <v>54</v>
+      </c>
+      <c r="G187" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>2022</v>
+      </c>
+      <c r="B188" t="s">
+        <v>67</v>
+      </c>
+      <c r="D188" t="s">
+        <v>35</v>
+      </c>
+      <c r="E188" t="b">
+        <v>1</v>
+      </c>
+      <c r="F188" t="s">
+        <v>54</v>
+      </c>
+      <c r="G188" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>2023</v>
+      </c>
+      <c r="B189" t="s">
+        <v>67</v>
+      </c>
+      <c r="D189" t="s">
+        <v>35</v>
+      </c>
+      <c r="E189" t="b">
+        <v>1</v>
+      </c>
+      <c r="F189" t="s">
+        <v>54</v>
+      </c>
+      <c r="G189" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>2014</v>
+      </c>
+      <c r="B190" t="s">
+        <v>76</v>
+      </c>
+      <c r="D190" t="s">
+        <v>35</v>
+      </c>
+      <c r="E190" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>2015</v>
+      </c>
+      <c r="B191" t="s">
+        <v>76</v>
+      </c>
+      <c r="D191" t="s">
+        <v>35</v>
+      </c>
+      <c r="E191" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>2016</v>
+      </c>
+      <c r="B192" t="s">
+        <v>76</v>
+      </c>
+      <c r="D192" t="s">
+        <v>35</v>
+      </c>
+      <c r="E192" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>2017</v>
+      </c>
+      <c r="B193" t="s">
+        <v>76</v>
+      </c>
+      <c r="D193" t="s">
+        <v>35</v>
+      </c>
+      <c r="E193" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>2018</v>
+      </c>
+      <c r="B194" t="s">
+        <v>75</v>
+      </c>
+      <c r="D194" t="s">
+        <v>35</v>
+      </c>
+      <c r="E194" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>2019</v>
+      </c>
+      <c r="B195" t="s">
+        <v>75</v>
+      </c>
+      <c r="D195" t="s">
+        <v>35</v>
+      </c>
+      <c r="E195" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>2020</v>
+      </c>
+      <c r="B196" t="s">
+        <v>75</v>
+      </c>
+      <c r="D196" t="s">
+        <v>35</v>
+      </c>
+      <c r="E196" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>2021</v>
+      </c>
+      <c r="B197" t="s">
+        <v>75</v>
+      </c>
+      <c r="D197" t="s">
+        <v>35</v>
+      </c>
+      <c r="E197" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>2022</v>
+      </c>
+      <c r="B198" t="s">
+        <v>75</v>
+      </c>
+      <c r="D198" t="s">
+        <v>35</v>
+      </c>
+      <c r="E198" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>2023</v>
+      </c>
+      <c r="B199" t="s">
+        <v>75</v>
+      </c>
+      <c r="D199" t="s">
+        <v>35</v>
+      </c>
+      <c r="E199" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4820,17 +5514,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d5cc9fc5-cf59-440a-a506-890d57680064">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B598B773ED9FC644B8B740EB3205C8DA" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6cfe95817d5870f6c066b2c32ab5fb2a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xmlns:ns3="d5cc9fc5-cf59-440a-a506-890d57680064" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a231614a4bf4996e6f4146316e2aaf8" ns2:_="" ns3:_="">
     <xsd:import namespace="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
@@ -5093,6 +5776,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d5cc9fc5-cf59-440a-a506-890d57680064">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3FAF407-B1B6-4FB8-B534-293B9E1D533A}">
   <ds:schemaRefs>
@@ -5102,23 +5796,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA6725D-5CB1-4E78-9F97-F79E79C18DA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d5cc9fc5-cf59-440a-a506-890d57680064"/>
-    <ds:schemaRef ds:uri="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B298AB6-2F6D-497E-AD9E-0F97ABEC8463}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5135,4 +5812,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA6725D-5CB1-4E78-9F97-F79E79C18DA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="d5cc9fc5-cf59-440a-a506-890d57680064"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added 3 smaller metrics
</commit_message>
<xml_diff>
--- a/Local Historic Crosswalk.xlsx
+++ b/Local Historic Crosswalk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasontheisen/Documents/Advance Illinois/Historic Report Card/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51755A17-8C52-5840-86F4-D118F73F1D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8976DDEB-18C3-304F-B737-AEA4E73D517E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20560" yWindow="880" windowWidth="20560" windowHeight="25700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report Card Metadata" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="100">
   <si>
     <t>Year</t>
   </si>
@@ -497,6 +497,72 @@
   </si>
   <si>
     <t>PUPIL-TEACHER RATIO -ELEM DISTRICT - Coming Soon</t>
+  </si>
+  <si>
+    <t>% Novice Teachers</t>
+  </si>
+  <si>
+    <t>% 8th Grade Passing Algebra 1</t>
+  </si>
+  <si>
+    <t>% 8TH GRADERS PASSING ALGEBRA I - SCHOOL</t>
+  </si>
+  <si>
+    <t>%8th Grade Passing Algebra 1</t>
+  </si>
+  <si>
+    <t>% FRESHMAN ON TRACK - SCHOOL</t>
+  </si>
+  <si>
+    <t>9th Grade on Track</t>
+  </si>
+  <si>
+    <t>% 9th Grade on Track</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">9th Grade on Track - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>demo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">% 9th Grade on Track - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>demo</t>
+    </r>
+  </si>
+  <si>
+    <t>% Novice Teachers - High Poverty Schools</t>
+  </si>
+  <si>
+    <t>% Novice Teachers - Low Poverty Schools</t>
+  </si>
+  <si>
+    <t>Novice Teachers - Low Poverty Schools</t>
+  </si>
+  <si>
+    <t>Novice Teachers - High Poverty Schools</t>
+  </si>
+  <si>
+    <t># 9th Grade on Track</t>
   </si>
 </sst>
 </file>
@@ -632,7 +698,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -650,12 +716,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="33">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -721,6 +809,27 @@
           <color theme="4" tint="0.39997558519241921"/>
         </right>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -997,49 +1106,55 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}" name="Table1" displayName="Table1" ref="A1:Q17" totalsRowShown="0" dataDxfId="26">
-  <autoFilter ref="A1:Q17" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}" name="Table1" displayName="Table1" ref="A1:W17" totalsRowShown="0" dataDxfId="32">
+  <autoFilter ref="A1:W17" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O17">
     <sortCondition ref="A1:A17"/>
   </sortState>
-  <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{6DA6945B-9D7D-0142-A374-7C4A97BBBBAB}" name="Year" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{1617EDAF-51CD-413F-9022-F6E4C97C233F}" name="RCDTS" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{A67D85A4-5303-744E-B7CD-31ECBC6CE0A7}" name="Type" dataDxfId="23"/>
-    <tableColumn id="13" xr3:uid="{C8F50192-B0A1-D84D-96D9-819955E9CE26}" name="District Type" dataDxfId="22"/>
-    <tableColumn id="14" xr3:uid="{A7661728-A363-9840-8182-CBC0352B14C6}" name="School Type" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{94336B41-A312-184A-9F00-C5E1720E28AF}" name="School Name" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{7516DA0D-E868-1941-B0D3-80B0E523A018}" name="District Name" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{DCD59F4B-C55C-2846-9070-7F8CC6CA2F51}" name="City" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{AB642454-853E-F049-84B7-745455B992F3}" name="County" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{5B5F7B45-CEFB-EE48-90E0-380BD11BD347}" name="Student Enrollment" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{DC5BC21C-5B26-D441-96D3-64D606494C9A}" name="Student Attendance Rate" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{16C5B399-2D53-AF41-815C-1F7C3259622D}" name="Student Chronic Truancy Rate" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{E3173650-9CBD-2046-9561-EC76593F21A4}" name="Chronic Absenteeism" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{A5C89E32-E6C7-354A-AD94-8B9E7BF5BEAF}" name="Total Teacher FTE" dataDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{91CEEB72-10AD-5347-AD91-C2EA26951FFD}" name="Teacher Retention Rate" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{B95926A8-CE9E-5E4C-8517-F53E1DD6BB12}" name="Pupil Teacher Ratio - Elementary" dataDxfId="1"/>
-    <tableColumn id="17" xr3:uid="{66E6EF1B-5F71-724F-BE1B-2EAE768FA6E4}" name="Pupil Teacher Ratio - High School" dataDxfId="0"/>
+  <tableColumns count="23">
+    <tableColumn id="1" xr3:uid="{6DA6945B-9D7D-0142-A374-7C4A97BBBBAB}" name="Year" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{1617EDAF-51CD-413F-9022-F6E4C97C233F}" name="RCDTS" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{A67D85A4-5303-744E-B7CD-31ECBC6CE0A7}" name="Type" dataDxfId="29"/>
+    <tableColumn id="13" xr3:uid="{C8F50192-B0A1-D84D-96D9-819955E9CE26}" name="District Type" dataDxfId="28"/>
+    <tableColumn id="14" xr3:uid="{A7661728-A363-9840-8182-CBC0352B14C6}" name="School Type" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{94336B41-A312-184A-9F00-C5E1720E28AF}" name="School Name" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{7516DA0D-E868-1941-B0D3-80B0E523A018}" name="District Name" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{DCD59F4B-C55C-2846-9070-7F8CC6CA2F51}" name="City" dataDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{AB642454-853E-F049-84B7-745455B992F3}" name="County" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{5B5F7B45-CEFB-EE48-90E0-380BD11BD347}" name="Student Enrollment" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{DC5BC21C-5B26-D441-96D3-64D606494C9A}" name="Student Attendance Rate" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{16C5B399-2D53-AF41-815C-1F7C3259622D}" name="Student Chronic Truancy Rate" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{E3173650-9CBD-2046-9561-EC76593F21A4}" name="Chronic Absenteeism" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{A5C89E32-E6C7-354A-AD94-8B9E7BF5BEAF}" name="Total Teacher FTE" dataDxfId="18"/>
+    <tableColumn id="15" xr3:uid="{91CEEB72-10AD-5347-AD91-C2EA26951FFD}" name="Teacher Retention Rate" dataDxfId="17"/>
+    <tableColumn id="16" xr3:uid="{B95926A8-CE9E-5E4C-8517-F53E1DD6BB12}" name="Pupil Teacher Ratio - Elementary" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{66E6EF1B-5F71-724F-BE1B-2EAE768FA6E4}" name="Pupil Teacher Ratio - High School" dataDxfId="15"/>
+    <tableColumn id="18" xr3:uid="{FF7C5CB9-8A3F-654A-AAC2-F90DDD57691C}" name="% Novice Teachers" dataDxfId="14"/>
+    <tableColumn id="21" xr3:uid="{14F53AE3-04FD-0049-9CD6-2E8BE716335E}" name="% Novice Teachers - High Poverty Schools" dataDxfId="4"/>
+    <tableColumn id="22" xr3:uid="{1A89C2C1-D5B1-D84E-AF9A-AFFF73A90C04}" name="% Novice Teachers - Low Poverty Schools" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{31BB3C4C-CD8A-9848-85A3-6A3A4A977857}" name="% 8th Grade Passing Algebra 1" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{7DC2CAA5-3B64-9C42-8E87-31C44668510E}" name="% 9th Grade on Track" dataDxfId="1"/>
+    <tableColumn id="23" xr3:uid="{AD3426F6-72EB-7A4F-BA71-66C2A3294CCF}" name="# 9th Grade on Track" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}" name="Table44" displayName="Table44" ref="A1:H231" totalsRowShown="0" dataDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="A1:H231" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}" name="Table44" displayName="Table44" ref="A1:H272" totalsRowShown="0" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A1:H272" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H231">
     <sortCondition ref="B1:B231"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{CF003222-4DDE-BB47-A657-1775812A7CF9}" name="Year" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{75198FC7-15E7-C749-9856-FF87007012FD}" name="Metric" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{250849D7-E98C-6047-AD29-C748E7E94296}" name="Original Metric" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{2B055042-83EA-3F40-9F97-2E2C80BE4FCE}" name="Sheet" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{FCF3CEDF-90EF-DD4A-BD7C-2C3BB2D372C6}" name="Disaggregated" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{E905735F-4B71-1A4E-AA00-10B4AAD2B5F6}" name="Disaggregation Details" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{CF003222-4DDE-BB47-A657-1775812A7CF9}" name="Year" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{75198FC7-15E7-C749-9856-FF87007012FD}" name="Metric" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{250849D7-E98C-6047-AD29-C748E7E94296}" name="Original Metric" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{2B055042-83EA-3F40-9F97-2E2C80BE4FCE}" name="Sheet" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{FCF3CEDF-90EF-DD4A-BD7C-2C3BB2D372C6}" name="Disaggregated" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{E905735F-4B71-1A4E-AA00-10B4AAD2B5F6}" name="Disaggregation Details" dataDxfId="6"/>
     <tableColumn id="7" xr3:uid="{6FC8DE02-1AAB-8248-8E52-B299C7FFB44A}" name="Disaggregation Format"/>
-    <tableColumn id="6" xr3:uid="{89643796-F484-D048-862D-B85A1B6BB907}" name="Special Format" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{89643796-F484-D048-862D-B85A1B6BB907}" name="Special Format" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1675,11 +1790,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q2" activeCellId="1" sqref="A2:A17 Q2:Q17"/>
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W12" activeCellId="2" sqref="A12:A17 S12:T17 W12:W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1693,17 +1808,24 @@
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="28.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="40.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="30" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="42.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1755,8 +1877,26 @@
       <c r="Q1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R1" t="s">
+        <v>86</v>
+      </c>
+      <c r="S1" t="s">
+        <v>95</v>
+      </c>
+      <c r="T1" t="s">
+        <v>96</v>
+      </c>
+      <c r="U1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2008</v>
       </c>
@@ -1794,14 +1934,17 @@
       <c r="N2" t="s">
         <v>61</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" t="s">
         <v>82</v>
       </c>
-      <c r="Q2" s="14" t="s">
+      <c r="Q2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="W2" s="14"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2009</v>
       </c>
@@ -1839,14 +1982,17 @@
       <c r="N3" t="s">
         <v>61</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" t="s">
         <v>82</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="W3" s="14"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2010</v>
       </c>
@@ -1884,14 +2030,17 @@
       <c r="N4" t="s">
         <v>61</v>
       </c>
-      <c r="P4" s="14" t="s">
+      <c r="P4" t="s">
         <v>82</v>
       </c>
-      <c r="Q4" s="14" t="s">
+      <c r="Q4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="W4" s="14"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2011</v>
       </c>
@@ -1929,14 +2078,17 @@
       <c r="N5" t="s">
         <v>61</v>
       </c>
-      <c r="P5" s="14" t="s">
+      <c r="P5" t="s">
         <v>82</v>
       </c>
-      <c r="Q5" s="14" t="s">
+      <c r="Q5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="W5" s="14"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2012</v>
       </c>
@@ -1974,14 +2126,17 @@
       <c r="N6" t="s">
         <v>61</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" t="s">
         <v>82</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="W6" s="14"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2013</v>
       </c>
@@ -2019,14 +2174,17 @@
       <c r="N7" t="s">
         <v>62</v>
       </c>
-      <c r="P7" s="14" t="s">
+      <c r="P7" t="s">
         <v>85</v>
       </c>
-      <c r="Q7" s="14" t="s">
+      <c r="Q7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="W7" s="14"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2014</v>
       </c>
@@ -2067,14 +2225,20 @@
       <c r="O8" t="s">
         <v>64</v>
       </c>
-      <c r="P8" s="14" t="s">
+      <c r="P8" t="s">
         <v>82</v>
       </c>
-      <c r="Q8" s="14" t="s">
+      <c r="Q8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="V8" t="s">
+        <v>90</v>
+      </c>
+      <c r="W8" s="14"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2015</v>
       </c>
@@ -2115,14 +2279,23 @@
       <c r="O9" t="s">
         <v>64</v>
       </c>
-      <c r="P9" s="14" t="s">
+      <c r="P9" t="s">
         <v>82</v>
       </c>
-      <c r="Q9" s="14" t="s">
+      <c r="Q9" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" t="s">
+        <v>88</v>
+      </c>
+      <c r="V9" t="s">
+        <v>90</v>
+      </c>
+      <c r="W9" s="14"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2016</v>
       </c>
@@ -2163,14 +2336,23 @@
       <c r="O10" t="s">
         <v>64</v>
       </c>
-      <c r="P10" s="14" t="s">
+      <c r="P10" t="s">
         <v>82</v>
       </c>
-      <c r="Q10" s="14" t="s">
+      <c r="Q10" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" t="s">
+        <v>88</v>
+      </c>
+      <c r="V10" t="s">
+        <v>90</v>
+      </c>
+      <c r="W10" s="14"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2017</v>
       </c>
@@ -2211,14 +2393,23 @@
       <c r="O11" t="s">
         <v>64</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="P11" t="s">
         <v>82</v>
       </c>
-      <c r="Q11" s="14" t="s">
+      <c r="Q11" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" t="s">
+        <v>88</v>
+      </c>
+      <c r="V11" t="s">
+        <v>90</v>
+      </c>
+      <c r="W11" s="14"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -2264,14 +2455,27 @@
       <c r="O12" t="s">
         <v>63</v>
       </c>
-      <c r="P12" s="14" t="s">
+      <c r="P12" t="s">
         <v>80</v>
       </c>
-      <c r="Q12" s="14" t="s">
+      <c r="Q12" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S12" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="T12" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="U12" t="s">
+        <v>89</v>
+      </c>
+      <c r="V12" t="s">
+        <v>91</v>
+      </c>
+      <c r="W12" s="14"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2019</v>
       </c>
@@ -2317,14 +2521,32 @@
       <c r="O13" t="s">
         <v>63</v>
       </c>
-      <c r="P13" s="14" t="s">
+      <c r="P13" t="s">
         <v>80</v>
       </c>
-      <c r="Q13" s="14" t="s">
+      <c r="Q13" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R13" t="s">
+        <v>86</v>
+      </c>
+      <c r="S13" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="T13" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="U13" t="s">
+        <v>87</v>
+      </c>
+      <c r="V13" t="s">
+        <v>92</v>
+      </c>
+      <c r="W13" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2020</v>
       </c>
@@ -2370,14 +2592,32 @@
       <c r="O14" t="s">
         <v>63</v>
       </c>
-      <c r="P14" s="14" t="s">
+      <c r="P14" t="s">
         <v>80</v>
       </c>
-      <c r="Q14" s="14" t="s">
+      <c r="Q14" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R14" t="s">
+        <v>86</v>
+      </c>
+      <c r="S14" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="T14" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="U14" t="s">
+        <v>87</v>
+      </c>
+      <c r="V14" t="s">
+        <v>92</v>
+      </c>
+      <c r="W14" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2021</v>
       </c>
@@ -2423,14 +2663,32 @@
       <c r="O15" t="s">
         <v>63</v>
       </c>
-      <c r="P15" s="14" t="s">
+      <c r="P15" t="s">
         <v>80</v>
       </c>
-      <c r="Q15" s="14" t="s">
+      <c r="Q15" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R15" t="s">
+        <v>86</v>
+      </c>
+      <c r="S15" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="T15" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="U15" t="s">
+        <v>87</v>
+      </c>
+      <c r="V15" t="s">
+        <v>92</v>
+      </c>
+      <c r="W15" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2022</v>
       </c>
@@ -2476,14 +2734,32 @@
       <c r="O16" t="s">
         <v>63</v>
       </c>
-      <c r="P16" s="14" t="s">
+      <c r="P16" t="s">
         <v>80</v>
       </c>
-      <c r="Q16" s="14" t="s">
+      <c r="Q16" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R16" t="s">
+        <v>86</v>
+      </c>
+      <c r="S16" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="T16" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="U16" t="s">
+        <v>87</v>
+      </c>
+      <c r="V16" t="s">
+        <v>92</v>
+      </c>
+      <c r="W16" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2023</v>
       </c>
@@ -2529,11 +2805,29 @@
       <c r="O17" t="s">
         <v>63</v>
       </c>
-      <c r="P17" s="14" t="s">
+      <c r="P17" t="s">
         <v>80</v>
       </c>
-      <c r="Q17" s="14" t="s">
+      <c r="Q17" t="s">
         <v>81</v>
+      </c>
+      <c r="R17" t="s">
+        <v>86</v>
+      </c>
+      <c r="S17" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="T17" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="U17" t="s">
+        <v>87</v>
+      </c>
+      <c r="V17" t="s">
+        <v>92</v>
+      </c>
+      <c r="W17" s="14" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2548,12 +2842,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249B090D-D7BB-374A-9D81-FFCE8C0599DD}">
-  <dimension ref="A1:H231"/>
+  <dimension ref="A1:H272"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A240" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A162" sqref="A162"/>
-      <selection pane="topRight" activeCell="B10" sqref="B10"/>
+      <selection pane="topRight" activeCell="E256" sqref="E256:E272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3701,7 +3995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2017</v>
       </c>
@@ -3718,7 +4012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2018</v>
       </c>
@@ -3735,7 +4029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2019</v>
       </c>
@@ -3752,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2020</v>
       </c>
@@ -3769,7 +4063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2021</v>
       </c>
@@ -3786,7 +4080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2022</v>
       </c>
@@ -3803,7 +4097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2023</v>
       </c>
@@ -3820,615 +4114,551 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="14">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72">
         <v>2008</v>
       </c>
-      <c r="B72" s="14" t="s">
+      <c r="B72" t="s">
         <v>80</v>
       </c>
-      <c r="C72" s="14" t="s">
+      <c r="C72" t="s">
         <v>82</v>
       </c>
-      <c r="D72" s="14" t="s">
+      <c r="D72" t="s">
         <v>37</v>
       </c>
       <c r="E72" t="b">
         <v>0</v>
       </c>
-      <c r="F72" s="14"/>
-      <c r="H72" s="14"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="14">
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73">
         <v>2009</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B73" t="s">
         <v>80</v>
       </c>
-      <c r="C73" s="14" t="s">
+      <c r="C73" t="s">
         <v>82</v>
       </c>
-      <c r="D73" s="14" t="s">
+      <c r="D73" t="s">
         <v>37</v>
       </c>
       <c r="E73" t="b">
         <v>0</v>
       </c>
-      <c r="F73" s="14"/>
-      <c r="H73" s="14"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="14">
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74">
         <v>2010</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B74" t="s">
         <v>80</v>
       </c>
-      <c r="C74" s="14" t="s">
+      <c r="C74" t="s">
         <v>82</v>
       </c>
-      <c r="D74" s="14" t="s">
+      <c r="D74" t="s">
         <v>37</v>
       </c>
       <c r="E74" t="b">
         <v>0</v>
       </c>
-      <c r="F74" s="14"/>
-      <c r="H74" s="14"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="14">
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75">
         <v>2011</v>
       </c>
-      <c r="B75" s="14" t="s">
+      <c r="B75" t="s">
         <v>80</v>
       </c>
-      <c r="C75" s="14" t="s">
+      <c r="C75" t="s">
         <v>82</v>
       </c>
-      <c r="D75" s="14" t="s">
+      <c r="D75" t="s">
         <v>37</v>
       </c>
       <c r="E75" t="b">
         <v>0</v>
       </c>
-      <c r="F75" s="14"/>
-      <c r="H75" s="14"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="14">
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76">
         <v>2012</v>
       </c>
-      <c r="B76" s="14" t="s">
+      <c r="B76" t="s">
         <v>80</v>
       </c>
-      <c r="C76" s="14" t="s">
+      <c r="C76" t="s">
         <v>82</v>
       </c>
-      <c r="D76" s="14" t="s">
+      <c r="D76" t="s">
         <v>37</v>
       </c>
       <c r="E76" t="b">
         <v>0</v>
       </c>
-      <c r="F76" s="14"/>
-      <c r="H76" s="14"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="14">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77">
         <v>2013</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B77" t="s">
         <v>80</v>
       </c>
-      <c r="C77" s="14" t="s">
+      <c r="C77" t="s">
         <v>85</v>
       </c>
-      <c r="D77" s="14" t="s">
+      <c r="D77" t="s">
         <v>37</v>
       </c>
       <c r="E77" t="b">
         <v>0</v>
       </c>
-      <c r="F77" s="14"/>
-      <c r="H77" s="14"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="14">
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78">
         <v>2014</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B78" t="s">
         <v>80</v>
       </c>
-      <c r="C78" s="14" t="s">
+      <c r="C78" t="s">
         <v>82</v>
       </c>
-      <c r="D78" s="14" t="s">
+      <c r="D78" t="s">
         <v>37</v>
       </c>
       <c r="E78" t="b">
         <v>0</v>
       </c>
-      <c r="F78" s="14"/>
-      <c r="H78" s="14"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="14">
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79">
         <v>2015</v>
       </c>
-      <c r="B79" s="14" t="s">
+      <c r="B79" t="s">
         <v>80</v>
       </c>
-      <c r="C79" s="14" t="s">
+      <c r="C79" t="s">
         <v>82</v>
       </c>
-      <c r="D79" s="14" t="s">
+      <c r="D79" t="s">
         <v>37</v>
       </c>
       <c r="E79" t="b">
         <v>0</v>
       </c>
-      <c r="F79" s="14"/>
-      <c r="H79" s="14"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="14">
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80">
         <v>2016</v>
       </c>
-      <c r="B80" s="14" t="s">
+      <c r="B80" t="s">
         <v>80</v>
       </c>
-      <c r="C80" s="14" t="s">
+      <c r="C80" t="s">
         <v>82</v>
       </c>
-      <c r="D80" s="14" t="s">
+      <c r="D80" t="s">
         <v>37</v>
       </c>
       <c r="E80" t="b">
         <v>0</v>
       </c>
-      <c r="F80" s="14"/>
-      <c r="H80" s="14"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="14">
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81">
         <v>2017</v>
       </c>
-      <c r="B81" s="14" t="s">
+      <c r="B81" t="s">
         <v>80</v>
       </c>
-      <c r="C81" s="14" t="s">
+      <c r="C81" t="s">
         <v>82</v>
       </c>
-      <c r="D81" s="14" t="s">
+      <c r="D81" t="s">
         <v>37</v>
       </c>
       <c r="E81" t="b">
         <v>0</v>
       </c>
-      <c r="F81" s="14"/>
-      <c r="H81" s="14"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="14">
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82">
         <v>2018</v>
       </c>
-      <c r="B82" s="14" t="s">
+      <c r="B82" t="s">
         <v>80</v>
       </c>
-      <c r="C82" s="14" t="s">
+      <c r="C82" t="s">
         <v>80</v>
       </c>
-      <c r="D82" s="14" t="s">
+      <c r="D82" t="s">
         <v>34</v>
       </c>
       <c r="E82" t="b">
         <v>0</v>
       </c>
-      <c r="F82" s="14"/>
-      <c r="H82" s="14"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="14">
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83">
         <v>2019</v>
       </c>
-      <c r="B83" s="14" t="s">
+      <c r="B83" t="s">
         <v>80</v>
       </c>
-      <c r="C83" s="14" t="s">
+      <c r="C83" t="s">
         <v>80</v>
       </c>
-      <c r="D83" s="14" t="s">
+      <c r="D83" t="s">
         <v>34</v>
       </c>
       <c r="E83" t="b">
         <v>0</v>
       </c>
-      <c r="F83" s="14"/>
-      <c r="H83" s="14"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="14">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84">
         <v>2020</v>
       </c>
-      <c r="B84" s="14" t="s">
+      <c r="B84" t="s">
         <v>80</v>
       </c>
-      <c r="C84" s="14" t="s">
+      <c r="C84" t="s">
         <v>80</v>
       </c>
-      <c r="D84" s="14" t="s">
+      <c r="D84" t="s">
         <v>34</v>
       </c>
       <c r="E84" t="b">
         <v>0</v>
       </c>
-      <c r="F84" s="14"/>
-      <c r="H84" s="14"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="14">
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85">
         <v>2021</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B85" t="s">
         <v>80</v>
       </c>
-      <c r="C85" s="14" t="s">
+      <c r="C85" t="s">
         <v>80</v>
       </c>
-      <c r="D85" s="14" t="s">
+      <c r="D85" t="s">
         <v>34</v>
       </c>
       <c r="E85" t="b">
         <v>0</v>
       </c>
-      <c r="F85" s="14"/>
-      <c r="H85" s="14"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="14">
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86">
         <v>2022</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B86" t="s">
         <v>80</v>
       </c>
-      <c r="C86" s="14" t="s">
+      <c r="C86" t="s">
         <v>80</v>
       </c>
-      <c r="D86" s="14" t="s">
+      <c r="D86" t="s">
         <v>34</v>
       </c>
       <c r="E86" t="b">
         <v>0</v>
       </c>
-      <c r="F86" s="14"/>
-      <c r="H86" s="14"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="14">
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87">
         <v>2023</v>
       </c>
-      <c r="B87" s="14" t="s">
+      <c r="B87" t="s">
         <v>80</v>
       </c>
-      <c r="C87" s="14" t="s">
+      <c r="C87" t="s">
         <v>80</v>
       </c>
-      <c r="D87" s="14" t="s">
+      <c r="D87" t="s">
         <v>34</v>
       </c>
       <c r="E87" t="b">
         <v>0</v>
       </c>
-      <c r="F87" s="14"/>
-      <c r="H87" s="14"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="14">
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88">
         <v>2008</v>
       </c>
-      <c r="B88" s="14" t="s">
+      <c r="B88" t="s">
         <v>81</v>
       </c>
-      <c r="C88" s="14" t="s">
+      <c r="C88" t="s">
         <v>83</v>
       </c>
-      <c r="D88" s="14" t="s">
+      <c r="D88" t="s">
         <v>37</v>
       </c>
       <c r="E88" t="b">
         <v>0</v>
       </c>
-      <c r="F88" s="14"/>
-      <c r="H88" s="14"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="14">
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89">
         <v>2009</v>
       </c>
-      <c r="B89" s="14" t="s">
+      <c r="B89" t="s">
         <v>81</v>
       </c>
-      <c r="C89" s="14" t="s">
+      <c r="C89" t="s">
         <v>83</v>
       </c>
-      <c r="D89" s="14" t="s">
+      <c r="D89" t="s">
         <v>37</v>
       </c>
       <c r="E89" t="b">
         <v>0</v>
       </c>
-      <c r="F89" s="14"/>
-      <c r="H89" s="14"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" s="14">
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90">
         <v>2010</v>
       </c>
-      <c r="B90" s="14" t="s">
+      <c r="B90" t="s">
         <v>81</v>
       </c>
-      <c r="C90" s="14" t="s">
+      <c r="C90" t="s">
         <v>83</v>
       </c>
-      <c r="D90" s="14" t="s">
+      <c r="D90" t="s">
         <v>37</v>
       </c>
       <c r="E90" t="b">
         <v>0</v>
       </c>
-      <c r="F90" s="14"/>
-      <c r="H90" s="14"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="14">
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91">
         <v>2011</v>
       </c>
-      <c r="B91" s="14" t="s">
+      <c r="B91" t="s">
         <v>81</v>
       </c>
-      <c r="C91" s="14" t="s">
+      <c r="C91" t="s">
         <v>83</v>
       </c>
-      <c r="D91" s="14" t="s">
+      <c r="D91" t="s">
         <v>37</v>
       </c>
       <c r="E91" t="b">
         <v>0</v>
       </c>
-      <c r="F91" s="14"/>
-      <c r="H91" s="14"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="14">
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92">
         <v>2012</v>
       </c>
-      <c r="B92" s="14" t="s">
+      <c r="B92" t="s">
         <v>81</v>
       </c>
-      <c r="C92" s="14" t="s">
+      <c r="C92" t="s">
         <v>83</v>
       </c>
-      <c r="D92" s="14" t="s">
+      <c r="D92" t="s">
         <v>37</v>
       </c>
       <c r="E92" t="b">
         <v>0</v>
       </c>
-      <c r="F92" s="14"/>
-      <c r="H92" s="14"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="14">
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93">
         <v>2013</v>
       </c>
-      <c r="B93" s="14" t="s">
+      <c r="B93" t="s">
         <v>81</v>
       </c>
-      <c r="C93" s="14" t="s">
+      <c r="C93" t="s">
         <v>84</v>
       </c>
-      <c r="D93" s="14" t="s">
+      <c r="D93" t="s">
         <v>37</v>
       </c>
       <c r="E93" t="b">
         <v>0</v>
       </c>
-      <c r="F93" s="14"/>
-      <c r="H93" s="14"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="14">
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94">
         <v>2014</v>
       </c>
-      <c r="B94" s="14" t="s">
+      <c r="B94" t="s">
         <v>81</v>
       </c>
-      <c r="C94" s="14" t="s">
+      <c r="C94" t="s">
         <v>83</v>
       </c>
-      <c r="D94" s="14" t="s">
+      <c r="D94" t="s">
         <v>37</v>
       </c>
       <c r="E94" t="b">
         <v>0</v>
       </c>
-      <c r="F94" s="14"/>
-      <c r="H94" s="14"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="14">
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95">
         <v>2015</v>
       </c>
-      <c r="B95" s="14" t="s">
+      <c r="B95" t="s">
         <v>81</v>
       </c>
-      <c r="C95" s="14" t="s">
+      <c r="C95" t="s">
         <v>83</v>
       </c>
-      <c r="D95" s="14" t="s">
+      <c r="D95" t="s">
         <v>37</v>
       </c>
       <c r="E95" t="b">
         <v>0</v>
       </c>
-      <c r="F95" s="14"/>
-      <c r="H95" s="14"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="14">
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96">
         <v>2016</v>
       </c>
-      <c r="B96" s="14" t="s">
+      <c r="B96" t="s">
         <v>81</v>
       </c>
-      <c r="C96" s="14" t="s">
+      <c r="C96" t="s">
         <v>83</v>
       </c>
-      <c r="D96" s="14" t="s">
+      <c r="D96" t="s">
         <v>37</v>
       </c>
       <c r="E96" t="b">
         <v>0</v>
       </c>
-      <c r="F96" s="14"/>
-      <c r="H96" s="14"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="14">
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97">
         <v>2017</v>
       </c>
-      <c r="B97" s="14" t="s">
+      <c r="B97" t="s">
         <v>81</v>
       </c>
-      <c r="C97" s="14" t="s">
+      <c r="C97" t="s">
         <v>83</v>
       </c>
-      <c r="D97" s="14" t="s">
+      <c r="D97" t="s">
         <v>37</v>
       </c>
       <c r="E97" t="b">
         <v>0</v>
       </c>
-      <c r="F97" s="14"/>
-      <c r="H97" s="14"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="14">
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98">
         <v>2018</v>
       </c>
-      <c r="B98" s="14" t="s">
+      <c r="B98" t="s">
         <v>81</v>
       </c>
-      <c r="C98" s="14" t="s">
+      <c r="C98" t="s">
         <v>81</v>
       </c>
-      <c r="D98" s="14" t="s">
+      <c r="D98" t="s">
         <v>34</v>
       </c>
       <c r="E98" t="b">
         <v>0</v>
       </c>
-      <c r="F98" s="14"/>
-      <c r="H98" s="14"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="14">
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99">
         <v>2019</v>
       </c>
-      <c r="B99" s="14" t="s">
+      <c r="B99" t="s">
         <v>81</v>
       </c>
-      <c r="C99" s="14" t="s">
+      <c r="C99" t="s">
         <v>81</v>
       </c>
-      <c r="D99" s="14" t="s">
+      <c r="D99" t="s">
         <v>34</v>
       </c>
       <c r="E99" t="b">
         <v>0</v>
       </c>
-      <c r="F99" s="14"/>
-      <c r="H99" s="14"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="14">
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100">
         <v>2020</v>
       </c>
-      <c r="B100" s="14" t="s">
+      <c r="B100" t="s">
         <v>81</v>
       </c>
-      <c r="C100" s="14" t="s">
+      <c r="C100" t="s">
         <v>81</v>
       </c>
-      <c r="D100" s="14" t="s">
+      <c r="D100" t="s">
         <v>34</v>
       </c>
       <c r="E100" t="b">
         <v>0</v>
       </c>
-      <c r="F100" s="14"/>
-      <c r="H100" s="14"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="14">
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101">
         <v>2021</v>
       </c>
-      <c r="B101" s="14" t="s">
+      <c r="B101" t="s">
         <v>81</v>
       </c>
-      <c r="C101" s="14" t="s">
+      <c r="C101" t="s">
         <v>81</v>
       </c>
-      <c r="D101" s="14" t="s">
+      <c r="D101" t="s">
         <v>34</v>
       </c>
       <c r="E101" t="b">
         <v>0</v>
       </c>
-      <c r="F101" s="14"/>
-      <c r="H101" s="14"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="14">
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102">
         <v>2022</v>
       </c>
-      <c r="B102" s="14" t="s">
+      <c r="B102" t="s">
         <v>81</v>
       </c>
-      <c r="C102" s="14" t="s">
+      <c r="C102" t="s">
         <v>81</v>
       </c>
-      <c r="D102" s="14" t="s">
+      <c r="D102" t="s">
         <v>34</v>
       </c>
       <c r="E102" t="b">
         <v>0</v>
       </c>
-      <c r="F102" s="14"/>
-      <c r="H102" s="14"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="14">
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103">
         <v>2023</v>
       </c>
-      <c r="B103" s="14" t="s">
+      <c r="B103" t="s">
         <v>81</v>
       </c>
-      <c r="C103" s="14" t="s">
+      <c r="C103" t="s">
         <v>81</v>
       </c>
-      <c r="D103" s="14" t="s">
+      <c r="D103" t="s">
         <v>34</v>
       </c>
       <c r="E103" t="b">
         <v>0</v>
       </c>
-      <c r="F103" s="14"/>
-      <c r="H103" s="14"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>2008</v>
       </c>
@@ -4445,7 +4675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>2009</v>
       </c>
@@ -4462,7 +4692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>2010</v>
       </c>
@@ -4479,7 +4709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>2011</v>
       </c>
@@ -4496,7 +4726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>2012</v>
       </c>
@@ -4513,7 +4743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>2013</v>
       </c>
@@ -4530,7 +4760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>2014</v>
       </c>
@@ -4547,7 +4777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>2015</v>
       </c>
@@ -4564,7 +4794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>2016</v>
       </c>
@@ -5359,7 +5589,7 @@
       <c r="B158" t="s">
         <v>25</v>
       </c>
-      <c r="C158" s="15" t="s">
+      <c r="C158" t="s">
         <v>28</v>
       </c>
       <c r="D158" t="s">
@@ -6253,13 +6483,13 @@
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A200" s="15">
+      <c r="A200">
         <v>2014</v>
       </c>
       <c r="B200" t="s">
         <v>63</v>
       </c>
-      <c r="C200" s="15" t="s">
+      <c r="C200" t="s">
         <v>64</v>
       </c>
       <c r="D200" t="s">
@@ -6270,13 +6500,13 @@
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A201" s="15">
+      <c r="A201">
         <v>2015</v>
       </c>
       <c r="B201" t="s">
         <v>63</v>
       </c>
-      <c r="C201" s="15" t="s">
+      <c r="C201" t="s">
         <v>64</v>
       </c>
       <c r="D201" t="s">
@@ -6287,13 +6517,13 @@
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A202" s="15">
+      <c r="A202">
         <v>2016</v>
       </c>
       <c r="B202" t="s">
         <v>63</v>
       </c>
-      <c r="C202" s="15" t="s">
+      <c r="C202" t="s">
         <v>64</v>
       </c>
       <c r="D202" t="s">
@@ -6304,13 +6534,13 @@
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A203" s="15">
+      <c r="A203">
         <v>2017</v>
       </c>
       <c r="B203" t="s">
         <v>63</v>
       </c>
-      <c r="C203" s="15" t="s">
+      <c r="C203" t="s">
         <v>64</v>
       </c>
       <c r="D203" t="s">
@@ -6321,13 +6551,13 @@
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A204" s="15">
+      <c r="A204">
         <v>2018</v>
       </c>
       <c r="B204" t="s">
         <v>63</v>
       </c>
-      <c r="C204" s="15" t="s">
+      <c r="C204" t="s">
         <v>63</v>
       </c>
       <c r="D204" t="s">
@@ -6338,13 +6568,13 @@
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A205" s="15">
+      <c r="A205">
         <v>2019</v>
       </c>
       <c r="B205" t="s">
         <v>63</v>
       </c>
-      <c r="C205" s="15" t="s">
+      <c r="C205" t="s">
         <v>63</v>
       </c>
       <c r="D205" t="s">
@@ -6891,6 +7121,755 @@
       <c r="E231" t="b">
         <v>0</v>
       </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A232">
+        <v>2015</v>
+      </c>
+      <c r="B232" t="s">
+        <v>87</v>
+      </c>
+      <c r="C232" t="s">
+        <v>88</v>
+      </c>
+      <c r="D232" t="s">
+        <v>37</v>
+      </c>
+      <c r="E232" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <v>2016</v>
+      </c>
+      <c r="B233" t="s">
+        <v>87</v>
+      </c>
+      <c r="C233" t="s">
+        <v>88</v>
+      </c>
+      <c r="D233" t="s">
+        <v>37</v>
+      </c>
+      <c r="E233" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <v>2017</v>
+      </c>
+      <c r="B234" t="s">
+        <v>87</v>
+      </c>
+      <c r="C234" t="s">
+        <v>88</v>
+      </c>
+      <c r="D234" t="s">
+        <v>37</v>
+      </c>
+      <c r="E234" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>2018</v>
+      </c>
+      <c r="B235" t="s">
+        <v>87</v>
+      </c>
+      <c r="C235" t="s">
+        <v>89</v>
+      </c>
+      <c r="D235" t="s">
+        <v>34</v>
+      </c>
+      <c r="E235" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>2019</v>
+      </c>
+      <c r="B236" t="s">
+        <v>87</v>
+      </c>
+      <c r="C236" t="s">
+        <v>87</v>
+      </c>
+      <c r="D236" t="s">
+        <v>34</v>
+      </c>
+      <c r="E236" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>2020</v>
+      </c>
+      <c r="B237" t="s">
+        <v>87</v>
+      </c>
+      <c r="C237" t="s">
+        <v>87</v>
+      </c>
+      <c r="D237" t="s">
+        <v>34</v>
+      </c>
+      <c r="E237" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>2021</v>
+      </c>
+      <c r="B238" t="s">
+        <v>87</v>
+      </c>
+      <c r="C238" t="s">
+        <v>87</v>
+      </c>
+      <c r="D238" t="s">
+        <v>34</v>
+      </c>
+      <c r="E238" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>2022</v>
+      </c>
+      <c r="B239" t="s">
+        <v>87</v>
+      </c>
+      <c r="C239" t="s">
+        <v>87</v>
+      </c>
+      <c r="D239" t="s">
+        <v>34</v>
+      </c>
+      <c r="E239" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>2023</v>
+      </c>
+      <c r="B240" t="s">
+        <v>87</v>
+      </c>
+      <c r="C240" t="s">
+        <v>87</v>
+      </c>
+      <c r="D240" t="s">
+        <v>34</v>
+      </c>
+      <c r="E240" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>2019</v>
+      </c>
+      <c r="B241" t="s">
+        <v>86</v>
+      </c>
+      <c r="C241" t="s">
+        <v>86</v>
+      </c>
+      <c r="D241" t="s">
+        <v>34</v>
+      </c>
+      <c r="E241" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>2020</v>
+      </c>
+      <c r="B242" t="s">
+        <v>86</v>
+      </c>
+      <c r="C242" t="s">
+        <v>86</v>
+      </c>
+      <c r="D242" t="s">
+        <v>34</v>
+      </c>
+      <c r="E242" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>2021</v>
+      </c>
+      <c r="B243" t="s">
+        <v>86</v>
+      </c>
+      <c r="C243" t="s">
+        <v>86</v>
+      </c>
+      <c r="D243" t="s">
+        <v>34</v>
+      </c>
+      <c r="E243" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>2022</v>
+      </c>
+      <c r="B244" t="s">
+        <v>86</v>
+      </c>
+      <c r="C244" t="s">
+        <v>86</v>
+      </c>
+      <c r="D244" t="s">
+        <v>34</v>
+      </c>
+      <c r="E244" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>2023</v>
+      </c>
+      <c r="B245" t="s">
+        <v>86</v>
+      </c>
+      <c r="C245" t="s">
+        <v>86</v>
+      </c>
+      <c r="D245" t="s">
+        <v>34</v>
+      </c>
+      <c r="E245" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>2014</v>
+      </c>
+      <c r="B246" t="s">
+        <v>92</v>
+      </c>
+      <c r="C246" t="s">
+        <v>90</v>
+      </c>
+      <c r="D246" t="s">
+        <v>37</v>
+      </c>
+      <c r="E246" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>2015</v>
+      </c>
+      <c r="B247" t="s">
+        <v>92</v>
+      </c>
+      <c r="C247" t="s">
+        <v>90</v>
+      </c>
+      <c r="D247" t="s">
+        <v>37</v>
+      </c>
+      <c r="E247" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>2016</v>
+      </c>
+      <c r="B248" t="s">
+        <v>92</v>
+      </c>
+      <c r="C248" t="s">
+        <v>90</v>
+      </c>
+      <c r="D248" t="s">
+        <v>37</v>
+      </c>
+      <c r="E248" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>2017</v>
+      </c>
+      <c r="B249" t="s">
+        <v>92</v>
+      </c>
+      <c r="C249" t="s">
+        <v>90</v>
+      </c>
+      <c r="D249" t="s">
+        <v>37</v>
+      </c>
+      <c r="E249" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>2018</v>
+      </c>
+      <c r="B250" t="s">
+        <v>92</v>
+      </c>
+      <c r="C250" t="s">
+        <v>91</v>
+      </c>
+      <c r="D250" t="s">
+        <v>34</v>
+      </c>
+      <c r="E250" t="b">
+        <v>1</v>
+      </c>
+      <c r="G250" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>2019</v>
+      </c>
+      <c r="B251" t="s">
+        <v>92</v>
+      </c>
+      <c r="C251" t="s">
+        <v>92</v>
+      </c>
+      <c r="D251" t="s">
+        <v>34</v>
+      </c>
+      <c r="E251" t="b">
+        <v>1</v>
+      </c>
+      <c r="G251" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>2020</v>
+      </c>
+      <c r="B252" t="s">
+        <v>92</v>
+      </c>
+      <c r="C252" t="s">
+        <v>92</v>
+      </c>
+      <c r="D252" t="s">
+        <v>34</v>
+      </c>
+      <c r="E252" t="b">
+        <v>1</v>
+      </c>
+      <c r="G252" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>2021</v>
+      </c>
+      <c r="B253" t="s">
+        <v>92</v>
+      </c>
+      <c r="C253" t="s">
+        <v>92</v>
+      </c>
+      <c r="D253" t="s">
+        <v>34</v>
+      </c>
+      <c r="E253" t="b">
+        <v>1</v>
+      </c>
+      <c r="G253" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>2022</v>
+      </c>
+      <c r="B254" t="s">
+        <v>92</v>
+      </c>
+      <c r="C254" t="s">
+        <v>92</v>
+      </c>
+      <c r="D254" t="s">
+        <v>34</v>
+      </c>
+      <c r="E254" t="b">
+        <v>1</v>
+      </c>
+      <c r="G254" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>2023</v>
+      </c>
+      <c r="B255" t="s">
+        <v>92</v>
+      </c>
+      <c r="C255" t="s">
+        <v>92</v>
+      </c>
+      <c r="D255" t="s">
+        <v>34</v>
+      </c>
+      <c r="E255" t="b">
+        <v>1</v>
+      </c>
+      <c r="G255" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A256" s="14">
+        <v>2018</v>
+      </c>
+      <c r="B256" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C256" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D256" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E256" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F256" s="14"/>
+      <c r="H256" s="14"/>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A257" s="14">
+        <v>2019</v>
+      </c>
+      <c r="B257" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C257" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D257" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E257" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F257" s="14"/>
+      <c r="H257" s="14"/>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A258" s="14">
+        <v>2020</v>
+      </c>
+      <c r="B258" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C258" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D258" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E258" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F258" s="14"/>
+      <c r="H258" s="14"/>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A259" s="14">
+        <v>2021</v>
+      </c>
+      <c r="B259" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C259" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D259" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E259" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F259" s="14"/>
+      <c r="H259" s="14"/>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A260" s="14">
+        <v>2022</v>
+      </c>
+      <c r="B260" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C260" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D260" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E260" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F260" s="14"/>
+      <c r="H260" s="14"/>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A261" s="14">
+        <v>2023</v>
+      </c>
+      <c r="B261" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C261" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D261" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E261" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F261" s="14"/>
+      <c r="H261" s="14"/>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A262" s="14">
+        <v>2018</v>
+      </c>
+      <c r="B262" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C262" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D262" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E262" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F262" s="14"/>
+      <c r="H262" s="14"/>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A263" s="14">
+        <v>2019</v>
+      </c>
+      <c r="B263" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C263" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D263" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E263" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F263" s="14"/>
+      <c r="H263" s="14"/>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A264" s="14">
+        <v>2020</v>
+      </c>
+      <c r="B264" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C264" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D264" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E264" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F264" s="14"/>
+      <c r="H264" s="14"/>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A265" s="14">
+        <v>2021</v>
+      </c>
+      <c r="B265" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C265" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D265" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E265" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F265" s="14"/>
+      <c r="H265" s="14"/>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A266" s="14">
+        <v>2022</v>
+      </c>
+      <c r="B266" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C266" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D266" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E266" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F266" s="14"/>
+      <c r="H266" s="14"/>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A267" s="14">
+        <v>2023</v>
+      </c>
+      <c r="B267" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C267" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D267" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E267" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F267" s="14"/>
+      <c r="H267" s="14"/>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A268" s="14">
+        <v>2019</v>
+      </c>
+      <c r="B268" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C268" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D268" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E268" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F268" s="14"/>
+      <c r="H268" s="14"/>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A269" s="14">
+        <v>2020</v>
+      </c>
+      <c r="B269" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C269" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D269" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E269" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F269" s="14"/>
+      <c r="H269" s="14"/>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A270" s="14">
+        <v>2021</v>
+      </c>
+      <c r="B270" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C270" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D270" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E270" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F270" s="14"/>
+      <c r="H270" s="14"/>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A271" s="14">
+        <v>2022</v>
+      </c>
+      <c r="B271" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C271" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D271" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E271" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F271" s="14"/>
+      <c r="H271" s="14"/>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A272" s="14">
+        <v>2023</v>
+      </c>
+      <c r="B272" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C272" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D272" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E272" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F272" s="14"/>
+      <c r="H272" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6910,17 +7889,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d5cc9fc5-cf59-440a-a506-890d57680064">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B598B773ED9FC644B8B740EB3205C8DA" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6cfe95817d5870f6c066b2c32ab5fb2a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xmlns:ns3="d5cc9fc5-cf59-440a-a506-890d57680064" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a231614a4bf4996e6f4146316e2aaf8" ns2:_="" ns3:_="">
     <xsd:import namespace="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
@@ -7183,6 +8151,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d5cc9fc5-cf59-440a-a506-890d57680064">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3FAF407-B1B6-4FB8-B534-293B9E1D533A}">
   <ds:schemaRefs>
@@ -7192,23 +8171,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA6725D-5CB1-4E78-9F97-F79E79C18DA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="d5cc9fc5-cf59-440a-a506-890d57680064"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B298AB6-2F6D-497E-AD9E-0F97ABEC8463}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7225,4 +8187,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA6725D-5CB1-4E78-9F97-F79E79C18DA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="d5cc9fc5-cf59-440a-a506-890d57680064"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Advanced Placement data
</commit_message>
<xml_diff>
--- a/Local Historic Crosswalk.xlsx
+++ b/Local Historic Crosswalk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasontheisen/Documents/Advance Illinois/Historic Report Card/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46BA818F-7A47-D942-8B1B-143D9515ABB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F49CA340-D0A6-384C-9222-1745A4FA0BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report Card Metadata" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1679" uniqueCount="174">
   <si>
     <t>Year</t>
   </si>
@@ -951,6 +951,118 @@
   </si>
   <si>
     <t>% Students enrolled in Dual Credit Coursework - All</t>
+  </si>
+  <si>
+    <t># Students who took AP classes Grade 9</t>
+  </si>
+  <si>
+    <t>Number of Students who took AP classes Grade 9 Total</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Number </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>demo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of Students who took AP classes Grade 9 Total</t>
+    </r>
+  </si>
+  <si>
+    <t># Students who took AP classes Grade 9 Total</t>
+  </si>
+  <si>
+    <t># Students who took AP classes Grade 10</t>
+  </si>
+  <si>
+    <t># OF GRADE 10 STUDENTS TOOK ONE OR MORE AP COURSES (SCHOOL)</t>
+  </si>
+  <si>
+    <t># OF GRADE 10 STUDENTS TOOK ONE OR MORE AP COURSES (SCHOOL) - demo</t>
+  </si>
+  <si>
+    <t>Number of Students who took AP classes Grade 10 Total</t>
+  </si>
+  <si>
+    <t>Number demo of Students who took AP classes Grade 10 Total</t>
+  </si>
+  <si>
+    <t># Students who took AP classes Grade 10 Total</t>
+  </si>
+  <si>
+    <t># Students who took AP classes Grade 11</t>
+  </si>
+  <si>
+    <t># OF GRADE 11 STUDENTS TOOK ONE OR MORE AP COURSES (SCHOOL)</t>
+  </si>
+  <si>
+    <t># OF GRADE 11 STUDENTS TOOK ONE OR MORE AP COURSES (SCHOOL) - demo</t>
+  </si>
+  <si>
+    <t>Number of Students who took AP classes Grade 11 Total</t>
+  </si>
+  <si>
+    <t>Number demo of Students who took AP classes Grade 11 Total</t>
+  </si>
+  <si>
+    <t># Students who took AP classes Grade 11 Total</t>
+  </si>
+  <si>
+    <t># Students who took AP classes Grade 12</t>
+  </si>
+  <si>
+    <t># OF GRADE 12 STUDENTS TOOK ONE OR MORE AP COURSES (SCHOOL)</t>
+  </si>
+  <si>
+    <t># OF GRADE 12 STUDENTS TOOK ONE OR MORE AP COURSES (SCHOOL) - demo</t>
+  </si>
+  <si>
+    <t>Number of Students who took AP classes Grade 12 Total</t>
+  </si>
+  <si>
+    <t>Number demo of Students who took AP classes Grade 12 Total</t>
+  </si>
+  <si>
+    <t># Students who took AP classes Grade 12 Total</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Students who took AP classes Grade 9 - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>demo</t>
+    </r>
+  </si>
+  <si>
+    <t># Students who took AP classes Grade 10 - demo</t>
+  </si>
+  <si>
+    <t># Students who took AP classes Grade 11 - demo</t>
+  </si>
+  <si>
+    <t># Students who took AP classes Grade 12 - demo</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1132,11 +1244,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="48">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1157,37 +1271,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1571,6 +1654,65 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1599,66 +1741,70 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}" name="Table1" displayName="Table1" ref="A1:AH17" totalsRowShown="0" dataDxfId="43">
-  <autoFilter ref="A1:AH17" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}" name="Table1" displayName="Table1" ref="A1:AL17" totalsRowShown="0" dataDxfId="38">
+  <autoFilter ref="A1:AL17" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O17">
     <sortCondition ref="A1:A17"/>
   </sortState>
-  <tableColumns count="34">
-    <tableColumn id="1" xr3:uid="{6DA6945B-9D7D-0142-A374-7C4A97BBBBAB}" name="Year" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{1617EDAF-51CD-413F-9022-F6E4C97C233F}" name="RCDTS" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{A67D85A4-5303-744E-B7CD-31ECBC6CE0A7}" name="Type" dataDxfId="40"/>
-    <tableColumn id="13" xr3:uid="{C8F50192-B0A1-D84D-96D9-819955E9CE26}" name="District Type" dataDxfId="39"/>
-    <tableColumn id="14" xr3:uid="{A7661728-A363-9840-8182-CBC0352B14C6}" name="School Type" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{94336B41-A312-184A-9F00-C5E1720E28AF}" name="School Name" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{7516DA0D-E868-1941-B0D3-80B0E523A018}" name="District Name" dataDxfId="36"/>
-    <tableColumn id="10" xr3:uid="{DCD59F4B-C55C-2846-9070-7F8CC6CA2F51}" name="City" dataDxfId="35"/>
-    <tableColumn id="11" xr3:uid="{AB642454-853E-F049-84B7-745455B992F3}" name="County" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{5B5F7B45-CEFB-EE48-90E0-380BD11BD347}" name="Student Enrollment" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{DC5BC21C-5B26-D441-96D3-64D606494C9A}" name="Student Attendance Rate" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{16C5B399-2D53-AF41-815C-1F7C3259622D}" name="Student Chronic Truancy Rate" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{E3173650-9CBD-2046-9561-EC76593F21A4}" name="Chronic Absenteeism" dataDxfId="30"/>
-    <tableColumn id="12" xr3:uid="{A5C89E32-E6C7-354A-AD94-8B9E7BF5BEAF}" name="Total Teacher FTE" dataDxfId="29"/>
-    <tableColumn id="15" xr3:uid="{91CEEB72-10AD-5347-AD91-C2EA26951FFD}" name="Teacher Retention Rate" dataDxfId="28"/>
-    <tableColumn id="16" xr3:uid="{B95926A8-CE9E-5E4C-8517-F53E1DD6BB12}" name="Pupil Teacher Ratio - Elementary" dataDxfId="27"/>
-    <tableColumn id="17" xr3:uid="{66E6EF1B-5F71-724F-BE1B-2EAE768FA6E4}" name="Pupil Teacher Ratio - High School" dataDxfId="26"/>
-    <tableColumn id="18" xr3:uid="{FF7C5CB9-8A3F-654A-AAC2-F90DDD57691C}" name="% Novice Teachers" dataDxfId="25"/>
-    <tableColumn id="21" xr3:uid="{14F53AE3-04FD-0049-9CD6-2E8BE716335E}" name="% Novice Teachers - High Poverty Schools" dataDxfId="24"/>
-    <tableColumn id="22" xr3:uid="{1A89C2C1-D5B1-D84E-AF9A-AFFF73A90C04}" name="% Novice Teachers - Low Poverty Schools" dataDxfId="23"/>
-    <tableColumn id="19" xr3:uid="{31BB3C4C-CD8A-9848-85A3-6A3A4A977857}" name="% 8th Grade Passing Algebra 1" dataDxfId="22"/>
-    <tableColumn id="20" xr3:uid="{7DC2CAA5-3B64-9C42-8E87-31C44668510E}" name="% 9th Grade on Track" dataDxfId="21"/>
-    <tableColumn id="23" xr3:uid="{AD3426F6-72EB-7A4F-BA71-66C2A3294CCF}" name="# 9th Grade on Track" dataDxfId="20"/>
-    <tableColumn id="24" xr3:uid="{7124EEF3-D182-7A4B-A827-DEC5EE0B1591}" name="# CTE Enrollment" dataDxfId="19"/>
-    <tableColumn id="25" xr3:uid="{0206B422-7E9A-AF41-A20D-0A4445D084F7}" name="# CTE Participants" dataDxfId="18"/>
-    <tableColumn id="26" xr3:uid="{74152CBC-6192-FA44-8D72-64E4E7284B17}" name="4-Year Graduation Rate (Perkins)" dataDxfId="17"/>
-    <tableColumn id="27" xr3:uid="{E91D57BE-E786-0E41-A6C9-D40C584A25B7}" name="Postsecondary Placement Rate (Perkins)" dataDxfId="16"/>
-    <tableColumn id="28" xr3:uid="{61C1EAC6-2067-F84E-B17C-A8B628C30DA0}" name="Nontraditional Program Enrollment Rate (Perkins)" dataDxfId="15"/>
-    <tableColumn id="29" xr3:uid="{612816CA-7F21-1C4E-9A0F-5C68D82ADF7D}" name="# Students who took Dual Credit classes Grade 9" dataDxfId="14"/>
-    <tableColumn id="30" xr3:uid="{5753F583-62B9-8A44-A3EC-546C676CE502}" name="# Students who took Dual Credit classes Grade 10" dataDxfId="13"/>
-    <tableColumn id="31" xr3:uid="{99388DA0-03B4-324C-93D0-00C4E7DFFD44}" name="# Students who took Dual Credit classes Grade 11" dataDxfId="12"/>
-    <tableColumn id="32" xr3:uid="{100FC056-2E22-0C4B-9AAC-CCBAF3958BB5}" name="# Students who took Dual Credit classes Grade 12" dataDxfId="11"/>
-    <tableColumn id="33" xr3:uid="{7148123E-CBBF-7A4C-A783-2B28AF22F11E}" name="# Students enrolled in Dual Credit Coursework" dataDxfId="10"/>
-    <tableColumn id="34" xr3:uid="{9282E612-FE85-D14F-B5B4-F790B296E915}" name="% Students enrolled in Dual Credit Coursework" dataDxfId="9"/>
+  <tableColumns count="38">
+    <tableColumn id="1" xr3:uid="{6DA6945B-9D7D-0142-A374-7C4A97BBBBAB}" name="Year" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{1617EDAF-51CD-413F-9022-F6E4C97C233F}" name="RCDTS" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{A67D85A4-5303-744E-B7CD-31ECBC6CE0A7}" name="Type" dataDxfId="35"/>
+    <tableColumn id="13" xr3:uid="{C8F50192-B0A1-D84D-96D9-819955E9CE26}" name="District Type" dataDxfId="34"/>
+    <tableColumn id="14" xr3:uid="{A7661728-A363-9840-8182-CBC0352B14C6}" name="School Type" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{94336B41-A312-184A-9F00-C5E1720E28AF}" name="School Name" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{7516DA0D-E868-1941-B0D3-80B0E523A018}" name="District Name" dataDxfId="31"/>
+    <tableColumn id="10" xr3:uid="{DCD59F4B-C55C-2846-9070-7F8CC6CA2F51}" name="City" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{AB642454-853E-F049-84B7-745455B992F3}" name="County" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{5B5F7B45-CEFB-EE48-90E0-380BD11BD347}" name="Student Enrollment" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{DC5BC21C-5B26-D441-96D3-64D606494C9A}" name="Student Attendance Rate" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{16C5B399-2D53-AF41-815C-1F7C3259622D}" name="Student Chronic Truancy Rate" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{E3173650-9CBD-2046-9561-EC76593F21A4}" name="Chronic Absenteeism" dataDxfId="25"/>
+    <tableColumn id="12" xr3:uid="{A5C89E32-E6C7-354A-AD94-8B9E7BF5BEAF}" name="Total Teacher FTE" dataDxfId="24"/>
+    <tableColumn id="15" xr3:uid="{91CEEB72-10AD-5347-AD91-C2EA26951FFD}" name="Teacher Retention Rate" dataDxfId="23"/>
+    <tableColumn id="16" xr3:uid="{B95926A8-CE9E-5E4C-8517-F53E1DD6BB12}" name="Pupil Teacher Ratio - Elementary" dataDxfId="22"/>
+    <tableColumn id="17" xr3:uid="{66E6EF1B-5F71-724F-BE1B-2EAE768FA6E4}" name="Pupil Teacher Ratio - High School" dataDxfId="21"/>
+    <tableColumn id="18" xr3:uid="{FF7C5CB9-8A3F-654A-AAC2-F90DDD57691C}" name="% Novice Teachers" dataDxfId="20"/>
+    <tableColumn id="21" xr3:uid="{14F53AE3-04FD-0049-9CD6-2E8BE716335E}" name="% Novice Teachers - High Poverty Schools" dataDxfId="19"/>
+    <tableColumn id="22" xr3:uid="{1A89C2C1-D5B1-D84E-AF9A-AFFF73A90C04}" name="% Novice Teachers - Low Poverty Schools" dataDxfId="18"/>
+    <tableColumn id="19" xr3:uid="{31BB3C4C-CD8A-9848-85A3-6A3A4A977857}" name="% 8th Grade Passing Algebra 1" dataDxfId="17"/>
+    <tableColumn id="20" xr3:uid="{7DC2CAA5-3B64-9C42-8E87-31C44668510E}" name="% 9th Grade on Track" dataDxfId="16"/>
+    <tableColumn id="23" xr3:uid="{AD3426F6-72EB-7A4F-BA71-66C2A3294CCF}" name="# 9th Grade on Track" dataDxfId="15"/>
+    <tableColumn id="24" xr3:uid="{7124EEF3-D182-7A4B-A827-DEC5EE0B1591}" name="# CTE Enrollment" dataDxfId="14"/>
+    <tableColumn id="25" xr3:uid="{0206B422-7E9A-AF41-A20D-0A4445D084F7}" name="# CTE Participants" dataDxfId="13"/>
+    <tableColumn id="26" xr3:uid="{74152CBC-6192-FA44-8D72-64E4E7284B17}" name="4-Year Graduation Rate (Perkins)" dataDxfId="12"/>
+    <tableColumn id="27" xr3:uid="{E91D57BE-E786-0E41-A6C9-D40C584A25B7}" name="Postsecondary Placement Rate (Perkins)" dataDxfId="11"/>
+    <tableColumn id="28" xr3:uid="{61C1EAC6-2067-F84E-B17C-A8B628C30DA0}" name="Nontraditional Program Enrollment Rate (Perkins)" dataDxfId="10"/>
+    <tableColumn id="29" xr3:uid="{612816CA-7F21-1C4E-9A0F-5C68D82ADF7D}" name="# Students who took Dual Credit classes Grade 9" dataDxfId="9"/>
+    <tableColumn id="30" xr3:uid="{5753F583-62B9-8A44-A3EC-546C676CE502}" name="# Students who took Dual Credit classes Grade 10" dataDxfId="8"/>
+    <tableColumn id="31" xr3:uid="{99388DA0-03B4-324C-93D0-00C4E7DFFD44}" name="# Students who took Dual Credit classes Grade 11" dataDxfId="7"/>
+    <tableColumn id="32" xr3:uid="{100FC056-2E22-0C4B-9AAC-CCBAF3958BB5}" name="# Students who took Dual Credit classes Grade 12" dataDxfId="6"/>
+    <tableColumn id="33" xr3:uid="{7148123E-CBBF-7A4C-A783-2B28AF22F11E}" name="# Students enrolled in Dual Credit Coursework" dataDxfId="5"/>
+    <tableColumn id="34" xr3:uid="{9282E612-FE85-D14F-B5B4-F790B296E915}" name="% Students enrolled in Dual Credit Coursework" dataDxfId="4"/>
+    <tableColumn id="35" xr3:uid="{62431BD2-7051-FC48-BD9B-525CBF545DDD}" name="# Students who took AP classes Grade 9" dataDxfId="3"/>
+    <tableColumn id="36" xr3:uid="{73C469BE-B611-0145-B886-AAA2CB70EAE8}" name="# Students who took AP classes Grade 10" dataDxfId="2"/>
+    <tableColumn id="37" xr3:uid="{CFE88FEF-98CA-654A-B3B8-05790EA4E553}" name="# Students who took AP classes Grade 11" dataDxfId="1"/>
+    <tableColumn id="38" xr3:uid="{CB531B3F-8204-2644-91D3-88ACB4BFD0A7}" name="# Students who took AP classes Grade 12" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}" name="Table44" displayName="Table44" ref="A1:H323" totalsRowShown="0" dataDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="A1:H323" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}" name="Table44" displayName="Table44" ref="A1:H353" totalsRowShown="0" dataDxfId="47" tableBorderDxfId="46">
+  <autoFilter ref="A1:H353" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H323">
     <sortCondition ref="B1:B323"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{CF003222-4DDE-BB47-A657-1775812A7CF9}" name="Year" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{75198FC7-15E7-C749-9856-FF87007012FD}" name="Metric" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{250849D7-E98C-6047-AD29-C748E7E94296}" name="Original Metric" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{2B055042-83EA-3F40-9F97-2E2C80BE4FCE}" name="Sheet" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{FCF3CEDF-90EF-DD4A-BD7C-2C3BB2D372C6}" name="Disaggregated" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{E905735F-4B71-1A4E-AA00-10B4AAD2B5F6}" name="Disaggregation Details" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{CF003222-4DDE-BB47-A657-1775812A7CF9}" name="Year" dataDxfId="45"/>
+    <tableColumn id="8" xr3:uid="{75198FC7-15E7-C749-9856-FF87007012FD}" name="Metric" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{250849D7-E98C-6047-AD29-C748E7E94296}" name="Original Metric" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{2B055042-83EA-3F40-9F97-2E2C80BE4FCE}" name="Sheet" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{FCF3CEDF-90EF-DD4A-BD7C-2C3BB2D372C6}" name="Disaggregated" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{E905735F-4B71-1A4E-AA00-10B4AAD2B5F6}" name="Disaggregation Details" dataDxfId="40"/>
     <tableColumn id="7" xr3:uid="{6FC8DE02-1AAB-8248-8E52-B299C7FFB44A}" name="Disaggregation Format"/>
-    <tableColumn id="6" xr3:uid="{89643796-F484-D048-862D-B85A1B6BB907}" name="Special Format" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{89643796-F484-D048-862D-B85A1B6BB907}" name="Special Format" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2294,11 +2440,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH17"/>
+  <dimension ref="A1:AL17"/>
   <sheetViews>
-    <sheetView zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH15" sqref="AH15:AH17"/>
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AI23" sqref="AI23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2336,9 +2482,11 @@
     <col min="31" max="32" width="44.6640625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="40.5" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="41" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="38" width="56.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2441,8 +2589,20 @@
       <c r="AH1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2008</v>
       </c>
@@ -2486,8 +2646,12 @@
       <c r="Q2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI2" s="16"/>
+      <c r="AJ2" s="16"/>
+      <c r="AK2" s="16"/>
+      <c r="AL2" s="16"/>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2009</v>
       </c>
@@ -2531,8 +2695,12 @@
       <c r="Q3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI3" s="16"/>
+      <c r="AJ3" s="16"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="16"/>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2010</v>
       </c>
@@ -2576,8 +2744,12 @@
       <c r="Q4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI4" s="16"/>
+      <c r="AJ4" s="16"/>
+      <c r="AK4" s="16"/>
+      <c r="AL4" s="16"/>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2011</v>
       </c>
@@ -2621,8 +2793,12 @@
       <c r="Q5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI5" s="16"/>
+      <c r="AJ5" s="16"/>
+      <c r="AK5" s="16"/>
+      <c r="AL5" s="16"/>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2012</v>
       </c>
@@ -2666,8 +2842,12 @@
       <c r="Q6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI6" s="16"/>
+      <c r="AJ6" s="16"/>
+      <c r="AK6" s="16"/>
+      <c r="AL6" s="16"/>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2013</v>
       </c>
@@ -2711,8 +2891,12 @@
       <c r="Q7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI7" s="16"/>
+      <c r="AJ7" s="16"/>
+      <c r="AK7" s="16"/>
+      <c r="AL7" s="16"/>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2014</v>
       </c>
@@ -2762,8 +2946,12 @@
       <c r="V8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI8" s="16"/>
+      <c r="AJ8" s="16"/>
+      <c r="AK8" s="16"/>
+      <c r="AL8" s="16"/>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2015</v>
       </c>
@@ -2816,8 +3004,12 @@
       <c r="V9" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI9" s="16"/>
+      <c r="AJ9" s="16"/>
+      <c r="AK9" s="16"/>
+      <c r="AL9" s="16"/>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2016</v>
       </c>
@@ -2882,8 +3074,18 @@
       <c r="AF10" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI10" s="16"/>
+      <c r="AJ10" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="AK10" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="AL10" s="16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2017</v>
       </c>
@@ -2948,8 +3150,18 @@
       <c r="AF11" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI11" s="16"/>
+      <c r="AJ11" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="AK11" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="AL11" s="16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -3028,8 +3240,20 @@
       <c r="AF12" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI12" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ12" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="AK12" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="AL12" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2019</v>
       </c>
@@ -3114,8 +3338,20 @@
       <c r="AF13" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI13" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ13" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="AK13" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="AL13" s="16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2020</v>
       </c>
@@ -3200,8 +3436,20 @@
       <c r="AF14" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI14" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ14" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="AK14" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="AL14" s="16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2021</v>
       </c>
@@ -3292,8 +3540,20 @@
       <c r="AH15" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI15" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ15" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="AK15" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="AL15" s="16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2022</v>
       </c>
@@ -3396,8 +3656,20 @@
       <c r="AH16" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI16" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ16" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="AK16" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="AL16" s="16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2023</v>
       </c>
@@ -3496,6 +3768,18 @@
       </c>
       <c r="AH17" t="s">
         <v>147</v>
+      </c>
+      <c r="AI17" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ17" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="AK17" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="AL17" s="16" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3510,12 +3794,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249B090D-D7BB-374A-9D81-FFCE8C0599DD}">
-  <dimension ref="A1:H323"/>
+  <dimension ref="A1:H353"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView topLeftCell="A320" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A162" sqref="A162"/>
-      <selection pane="topRight" activeCell="D86" sqref="D86"/>
+      <selection pane="topRight" activeCell="G351" sqref="G351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9453,7 +9737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>2021</v>
       </c>
@@ -9470,7 +9754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>2022</v>
       </c>
@@ -9487,7 +9771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>2023</v>
       </c>
@@ -9503,6 +9787,668 @@
       <c r="E323" t="b">
         <v>0</v>
       </c>
+    </row>
+    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A324" s="16">
+        <v>2018</v>
+      </c>
+      <c r="B324" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C324" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D324" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E324" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F324" s="16"/>
+      <c r="G324" t="s">
+        <v>150</v>
+      </c>
+      <c r="H324" s="16"/>
+    </row>
+    <row r="325" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A325" s="16">
+        <v>2019</v>
+      </c>
+      <c r="B325" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C325" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D325" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E325" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F325" s="16"/>
+      <c r="G325" t="s">
+        <v>170</v>
+      </c>
+      <c r="H325" s="16"/>
+    </row>
+    <row r="326" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A326" s="16">
+        <v>2020</v>
+      </c>
+      <c r="B326" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C326" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D326" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E326" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F326" s="16"/>
+      <c r="G326" t="s">
+        <v>170</v>
+      </c>
+      <c r="H326" s="16"/>
+    </row>
+    <row r="327" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A327" s="16">
+        <v>2021</v>
+      </c>
+      <c r="B327" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C327" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D327" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E327" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F327" s="16"/>
+      <c r="G327" t="s">
+        <v>170</v>
+      </c>
+      <c r="H327" s="16"/>
+    </row>
+    <row r="328" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A328" s="16">
+        <v>2022</v>
+      </c>
+      <c r="B328" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C328" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D328" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E328" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F328" s="16"/>
+      <c r="G328" t="s">
+        <v>170</v>
+      </c>
+      <c r="H328" s="16"/>
+    </row>
+    <row r="329" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A329" s="16">
+        <v>2023</v>
+      </c>
+      <c r="B329" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C329" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D329" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E329" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F329" s="16"/>
+      <c r="G329" t="s">
+        <v>170</v>
+      </c>
+      <c r="H329" s="16"/>
+    </row>
+    <row r="330" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A330" s="16">
+        <v>2016</v>
+      </c>
+      <c r="B330" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C330" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D330" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E330" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F330" s="16"/>
+      <c r="G330" t="s">
+        <v>154</v>
+      </c>
+      <c r="H330" s="16"/>
+    </row>
+    <row r="331" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A331" s="16">
+        <v>2017</v>
+      </c>
+      <c r="B331" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C331" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D331" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E331" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F331" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G331" t="s">
+        <v>154</v>
+      </c>
+      <c r="H331" s="16"/>
+    </row>
+    <row r="332" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A332" s="16">
+        <v>2018</v>
+      </c>
+      <c r="B332" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C332" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D332" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E332" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F332" s="16"/>
+      <c r="G332" t="s">
+        <v>156</v>
+      </c>
+      <c r="H332" s="16"/>
+    </row>
+    <row r="333" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A333" s="16">
+        <v>2019</v>
+      </c>
+      <c r="B333" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C333" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D333" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E333" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F333" s="16"/>
+      <c r="G333" t="s">
+        <v>171</v>
+      </c>
+      <c r="H333" s="16"/>
+    </row>
+    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A334" s="16">
+        <v>2020</v>
+      </c>
+      <c r="B334" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C334" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D334" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E334" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F334" s="16"/>
+      <c r="G334" t="s">
+        <v>171</v>
+      </c>
+      <c r="H334" s="16"/>
+    </row>
+    <row r="335" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A335" s="16">
+        <v>2021</v>
+      </c>
+      <c r="B335" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C335" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D335" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E335" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F335" s="16"/>
+      <c r="G335" t="s">
+        <v>171</v>
+      </c>
+      <c r="H335" s="16"/>
+    </row>
+    <row r="336" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A336" s="16">
+        <v>2022</v>
+      </c>
+      <c r="B336" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C336" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D336" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E336" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F336" s="16"/>
+      <c r="G336" t="s">
+        <v>171</v>
+      </c>
+      <c r="H336" s="16"/>
+    </row>
+    <row r="337" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A337" s="16">
+        <v>2023</v>
+      </c>
+      <c r="B337" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C337" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D337" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E337" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F337" s="16"/>
+      <c r="G337" t="s">
+        <v>171</v>
+      </c>
+      <c r="H337" s="16"/>
+    </row>
+    <row r="338" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A338" s="16">
+        <v>2016</v>
+      </c>
+      <c r="B338" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C338" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="D338" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E338" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F338" s="16"/>
+      <c r="G338" t="s">
+        <v>160</v>
+      </c>
+      <c r="H338" s="16"/>
+    </row>
+    <row r="339" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A339" s="16">
+        <v>2017</v>
+      </c>
+      <c r="B339" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C339" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="D339" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E339" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F339" s="16"/>
+      <c r="G339" t="s">
+        <v>160</v>
+      </c>
+      <c r="H339" s="16"/>
+    </row>
+    <row r="340" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A340" s="16">
+        <v>2018</v>
+      </c>
+      <c r="B340" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C340" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D340" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E340" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F340" s="16"/>
+      <c r="G340" t="s">
+        <v>162</v>
+      </c>
+      <c r="H340" s="16"/>
+    </row>
+    <row r="341" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A341" s="16">
+        <v>2019</v>
+      </c>
+      <c r="B341" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C341" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D341" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E341" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F341" s="16"/>
+      <c r="G341" t="s">
+        <v>172</v>
+      </c>
+      <c r="H341" s="16"/>
+    </row>
+    <row r="342" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A342" s="16">
+        <v>2020</v>
+      </c>
+      <c r="B342" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C342" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D342" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E342" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F342" s="16"/>
+      <c r="G342" t="s">
+        <v>172</v>
+      </c>
+      <c r="H342" s="16"/>
+    </row>
+    <row r="343" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A343" s="16">
+        <v>2021</v>
+      </c>
+      <c r="B343" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C343" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D343" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E343" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F343" s="16"/>
+      <c r="G343" t="s">
+        <v>172</v>
+      </c>
+      <c r="H343" s="16"/>
+    </row>
+    <row r="344" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A344" s="16">
+        <v>2022</v>
+      </c>
+      <c r="B344" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C344" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D344" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E344" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F344" s="16"/>
+      <c r="G344" t="s">
+        <v>172</v>
+      </c>
+      <c r="H344" s="16"/>
+    </row>
+    <row r="345" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A345" s="16">
+        <v>2023</v>
+      </c>
+      <c r="B345" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C345" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D345" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E345" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F345" s="16"/>
+      <c r="G345" t="s">
+        <v>172</v>
+      </c>
+      <c r="H345" s="16"/>
+    </row>
+    <row r="346" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A346" s="16">
+        <v>2016</v>
+      </c>
+      <c r="B346" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C346" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="D346" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E346" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F346" s="16"/>
+      <c r="G346" t="s">
+        <v>166</v>
+      </c>
+      <c r="H346" s="16"/>
+    </row>
+    <row r="347" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A347" s="16">
+        <v>2017</v>
+      </c>
+      <c r="B347" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C347" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="D347" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E347" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F347" s="16"/>
+      <c r="G347" t="s">
+        <v>166</v>
+      </c>
+      <c r="H347" s="16"/>
+    </row>
+    <row r="348" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A348" s="16">
+        <v>2018</v>
+      </c>
+      <c r="B348" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C348" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="D348" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E348" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F348" s="16"/>
+      <c r="G348" t="s">
+        <v>168</v>
+      </c>
+      <c r="H348" s="16"/>
+    </row>
+    <row r="349" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A349" s="16">
+        <v>2019</v>
+      </c>
+      <c r="B349" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C349" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="D349" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E349" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F349" s="16"/>
+      <c r="G349" t="s">
+        <v>173</v>
+      </c>
+      <c r="H349" s="16"/>
+    </row>
+    <row r="350" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A350" s="16">
+        <v>2020</v>
+      </c>
+      <c r="B350" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C350" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="D350" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E350" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F350" s="16"/>
+      <c r="G350" t="s">
+        <v>173</v>
+      </c>
+      <c r="H350" s="16"/>
+    </row>
+    <row r="351" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A351" s="16">
+        <v>2021</v>
+      </c>
+      <c r="B351" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C351" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="D351" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E351" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F351" s="16"/>
+      <c r="G351" t="s">
+        <v>173</v>
+      </c>
+      <c r="H351" s="16"/>
+    </row>
+    <row r="352" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A352" s="16">
+        <v>2022</v>
+      </c>
+      <c r="B352" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C352" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="D352" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E352" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F352" s="16"/>
+      <c r="G352" t="s">
+        <v>173</v>
+      </c>
+      <c r="H352" s="16"/>
+    </row>
+    <row r="353" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A353" s="16">
+        <v>2023</v>
+      </c>
+      <c r="B353" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C353" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="D353" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E353" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F353" s="16"/>
+      <c r="G353" t="s">
+        <v>173</v>
+      </c>
+      <c r="H353" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9514,12 +10460,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d5cc9fc5-cf59-440a-a506-890d57680064">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9786,20 +10734,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d5cc9fc5-cf59-440a-a506-890d57680064">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3FAF407-B1B6-4FB8-B534-293B9E1D533A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA6725D-5CB1-4E78-9F97-F79E79C18DA7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d5cc9fc5-cf59-440a-a506-890d57680064"/>
+    <ds:schemaRef ds:uri="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9824,18 +10779,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA6725D-5CB1-4E78-9F97-F79E79C18DA7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3FAF407-B1B6-4FB8-B534-293B9E1D533A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d5cc9fc5-cf59-440a-a506-890d57680064"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Graduation Rates. Ran into a complication and solved it by trimming all layout file values.
</commit_message>
<xml_diff>
--- a/Local Historic Crosswalk.xlsx
+++ b/Local Historic Crosswalk.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasontheisen/Documents/Advance Illinois/Historic Report Card/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F49CA340-D0A6-384C-9222-1745A4FA0BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F81D6B3B-0887-0246-9B8F-C93A20194320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1679" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2208" uniqueCount="234">
   <si>
     <t>Year</t>
   </si>
@@ -1064,12 +1064,252 @@
   <si>
     <t># Students who took AP classes Grade 12 - demo</t>
   </si>
+  <si>
+    <t># Students who took IB classes Grade 9</t>
+  </si>
+  <si>
+    <t># Students who took IB classes Grade 10</t>
+  </si>
+  <si>
+    <t># Students who took IB classes Grade 11</t>
+  </si>
+  <si>
+    <t># Students who took IB classes Grade 12</t>
+  </si>
+  <si>
+    <t># OF GRADE 10 STUDENTS TOOK ONE OR MORE IB COURSES (SCHOOL)</t>
+  </si>
+  <si>
+    <t># OF GRADE 11 STUDENTS TOOK ONE OR MORE IB COURSES (SCHOOL)</t>
+  </si>
+  <si>
+    <t># OF GRADE 12 STUDENTS TOOK ONE OR MORE IB COURSES (SCHOOL)</t>
+  </si>
+  <si>
+    <t>Number of Students who took IB classes Grade 9 Total</t>
+  </si>
+  <si>
+    <t>Number of Students who took IB classes Grade 10 Total</t>
+  </si>
+  <si>
+    <t>Number of Students who took IB classes Grade 11 Total</t>
+  </si>
+  <si>
+    <t>Number of Students who took IB classes Grade 12 Total</t>
+  </si>
+  <si>
+    <t># Students who took IB classes Grade 9 Total</t>
+  </si>
+  <si>
+    <t># Students who took IB classes Grade 10 Total</t>
+  </si>
+  <si>
+    <t># Students who took IB classes Grade 11 Total</t>
+  </si>
+  <si>
+    <t># Students who took IB classes Grade 12 Total</t>
+  </si>
+  <si>
+    <t>Number demo of Students who took IB classes Grade 9 Total</t>
+  </si>
+  <si>
+    <t># Students who took IB classes Grade 9 - demo</t>
+  </si>
+  <si>
+    <t># OF GRADE 10 STUDENTS TOOK ONE OR MORE IB COURSES (SCHOOL) - demo</t>
+  </si>
+  <si>
+    <t>Number demo of Students who took IB classes Grade 10 Total</t>
+  </si>
+  <si>
+    <t># Students who took IB classes Grade 10 - demo</t>
+  </si>
+  <si>
+    <t># OF GRADE 11 STUDENTS TOOK ONE OR MORE IB COURSES (SCHOOL) - demo</t>
+  </si>
+  <si>
+    <t>Number demo of Students who took IB classes Grade 11 Total</t>
+  </si>
+  <si>
+    <t># Students who took IB classes Grade 11 - demo</t>
+  </si>
+  <si>
+    <t># OF GRADE 12 STUDENTS TOOK ONE OR MORE IB COURSES (SCHOOL) - demo</t>
+  </si>
+  <si>
+    <t>Number demo of Students who took IB classes Grade 12 Total</t>
+  </si>
+  <si>
+    <t># Students who took IB classes Grade 12 - demo</t>
+  </si>
+  <si>
+    <t># Out-of-Field Teachers</t>
+  </si>
+  <si>
+    <t>% Out-of-Field Teachers</t>
+  </si>
+  <si>
+    <t>TeacherOutofField</t>
+  </si>
+  <si>
+    <t>Teachers with Short-Term or Provisional License - High Poverty Schools</t>
+  </si>
+  <si>
+    <t>Teachers with Short-Term or Provisional License - Low Poverty Schools</t>
+  </si>
+  <si>
+    <t>% Teachers with Short-Term or Provisional License</t>
+  </si>
+  <si>
+    <t>% Teachers with Short-Term or Provisional License - High Poverty Schools</t>
+  </si>
+  <si>
+    <t>% Teachers with Short-Term or Provisional License - Low Poverty Schools</t>
+  </si>
+  <si>
+    <t># Teachers with Short-Term or Provisional License - High Poverty Schools</t>
+  </si>
+  <si>
+    <t># Teachers with Short-Term or Provisional License - Low Poverty Schools</t>
+  </si>
+  <si>
+    <t>% TCHRS WITH EMERGENCY OR PROVISIONAL CREDENTIALS(SCHOOL)</t>
+  </si>
+  <si>
+    <t>% EMERGENCY OR PROVISIONAL CREDENTIALS (DISTRICT HIGH POVERTY)</t>
+  </si>
+  <si>
+    <t>% EMERGENCY OR PROVISIONAL CREDENTIALS (DISTRICT LOW POVERTY)</t>
+  </si>
+  <si>
+    <t>% TCHRS WITH EMERGENCY OR PROVISIONAL CREDENTIALS(SCHOOL) - Coming Soon</t>
+  </si>
+  <si>
+    <t>% EMERGENCY OR PROVISIONAL CREDENTIALS (DISTRICT HIGH POVERTY) - Coming Soon</t>
+  </si>
+  <si>
+    <t>% EMERGENCY OR PROVISIONAL CREDENTIALS (DISTRICT LOW POVERTY) - Coming Soon</t>
+  </si>
+  <si>
+    <t>TEACHER ATTENDANCE RATE (SCHOOL)</t>
+  </si>
+  <si>
+    <t>Teacher Attendace Rate</t>
+  </si>
+  <si>
+    <t>Teacher Attendance Rate</t>
+  </si>
+  <si>
+    <t># OF PRINCIPAL TURNOVER WITHIN 6 YEARS (SCHOOL)</t>
+  </si>
+  <si>
+    <t>Principal Turnover within 6 Years</t>
+  </si>
+  <si>
+    <t>HS GRAD RATE SCHOOL %</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">HS GRAD RATE SCHOOL % - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>demo</t>
+    </r>
+  </si>
+  <si>
+    <t>HS 4-YEAR GRAD RATE SCHOOL %</t>
+  </si>
+  <si>
+    <t>HS 6-YEAR GRAD RATE SCHOOL %</t>
+  </si>
+  <si>
+    <t>High School 4-Year Graduation Rate - Total</t>
+  </si>
+  <si>
+    <t>High School 6-Year Graduation Rate - Total</t>
+  </si>
+  <si>
+    <t>High School 6-Year Graduation Rate</t>
+  </si>
+  <si>
+    <t>High School 4-Year Graduation Rate</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">HS 4-YEAR GRAD RATE SCHOOL % - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>demo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">High School 4-Year Graduation Rate - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>demo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">HS 6-YEAR GRAD RATE SCHOOL % - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>demo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">High School 6-Year Graduation Rate - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>demo</t>
+    </r>
+  </si>
+  <si>
+    <t>COUNTY</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1124,8 +1364,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1142,6 +1387,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0E4F5"/>
+        <bgColor rgb="FFC0E4F5"/>
       </patternFill>
     </fill>
   </fills>
@@ -1225,7 +1476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1244,13 +1495,180 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="63">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1654,65 +2072,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1741,70 +2100,85 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}" name="Table1" displayName="Table1" ref="A1:AL17" totalsRowShown="0" dataDxfId="38">
-  <autoFilter ref="A1:AL17" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}" name="Table1" displayName="Table1" ref="A1:BA17" totalsRowShown="0" dataDxfId="62">
+  <autoFilter ref="A1:BA17" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O17">
     <sortCondition ref="A1:A17"/>
   </sortState>
-  <tableColumns count="38">
-    <tableColumn id="1" xr3:uid="{6DA6945B-9D7D-0142-A374-7C4A97BBBBAB}" name="Year" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{1617EDAF-51CD-413F-9022-F6E4C97C233F}" name="RCDTS" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{A67D85A4-5303-744E-B7CD-31ECBC6CE0A7}" name="Type" dataDxfId="35"/>
-    <tableColumn id="13" xr3:uid="{C8F50192-B0A1-D84D-96D9-819955E9CE26}" name="District Type" dataDxfId="34"/>
-    <tableColumn id="14" xr3:uid="{A7661728-A363-9840-8182-CBC0352B14C6}" name="School Type" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{94336B41-A312-184A-9F00-C5E1720E28AF}" name="School Name" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{7516DA0D-E868-1941-B0D3-80B0E523A018}" name="District Name" dataDxfId="31"/>
-    <tableColumn id="10" xr3:uid="{DCD59F4B-C55C-2846-9070-7F8CC6CA2F51}" name="City" dataDxfId="30"/>
-    <tableColumn id="11" xr3:uid="{AB642454-853E-F049-84B7-745455B992F3}" name="County" dataDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{5B5F7B45-CEFB-EE48-90E0-380BD11BD347}" name="Student Enrollment" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{DC5BC21C-5B26-D441-96D3-64D606494C9A}" name="Student Attendance Rate" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{16C5B399-2D53-AF41-815C-1F7C3259622D}" name="Student Chronic Truancy Rate" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{E3173650-9CBD-2046-9561-EC76593F21A4}" name="Chronic Absenteeism" dataDxfId="25"/>
-    <tableColumn id="12" xr3:uid="{A5C89E32-E6C7-354A-AD94-8B9E7BF5BEAF}" name="Total Teacher FTE" dataDxfId="24"/>
-    <tableColumn id="15" xr3:uid="{91CEEB72-10AD-5347-AD91-C2EA26951FFD}" name="Teacher Retention Rate" dataDxfId="23"/>
-    <tableColumn id="16" xr3:uid="{B95926A8-CE9E-5E4C-8517-F53E1DD6BB12}" name="Pupil Teacher Ratio - Elementary" dataDxfId="22"/>
-    <tableColumn id="17" xr3:uid="{66E6EF1B-5F71-724F-BE1B-2EAE768FA6E4}" name="Pupil Teacher Ratio - High School" dataDxfId="21"/>
-    <tableColumn id="18" xr3:uid="{FF7C5CB9-8A3F-654A-AAC2-F90DDD57691C}" name="% Novice Teachers" dataDxfId="20"/>
-    <tableColumn id="21" xr3:uid="{14F53AE3-04FD-0049-9CD6-2E8BE716335E}" name="% Novice Teachers - High Poverty Schools" dataDxfId="19"/>
-    <tableColumn id="22" xr3:uid="{1A89C2C1-D5B1-D84E-AF9A-AFFF73A90C04}" name="% Novice Teachers - Low Poverty Schools" dataDxfId="18"/>
-    <tableColumn id="19" xr3:uid="{31BB3C4C-CD8A-9848-85A3-6A3A4A977857}" name="% 8th Grade Passing Algebra 1" dataDxfId="17"/>
-    <tableColumn id="20" xr3:uid="{7DC2CAA5-3B64-9C42-8E87-31C44668510E}" name="% 9th Grade on Track" dataDxfId="16"/>
-    <tableColumn id="23" xr3:uid="{AD3426F6-72EB-7A4F-BA71-66C2A3294CCF}" name="# 9th Grade on Track" dataDxfId="15"/>
-    <tableColumn id="24" xr3:uid="{7124EEF3-D182-7A4B-A827-DEC5EE0B1591}" name="# CTE Enrollment" dataDxfId="14"/>
-    <tableColumn id="25" xr3:uid="{0206B422-7E9A-AF41-A20D-0A4445D084F7}" name="# CTE Participants" dataDxfId="13"/>
-    <tableColumn id="26" xr3:uid="{74152CBC-6192-FA44-8D72-64E4E7284B17}" name="4-Year Graduation Rate (Perkins)" dataDxfId="12"/>
-    <tableColumn id="27" xr3:uid="{E91D57BE-E786-0E41-A6C9-D40C584A25B7}" name="Postsecondary Placement Rate (Perkins)" dataDxfId="11"/>
-    <tableColumn id="28" xr3:uid="{61C1EAC6-2067-F84E-B17C-A8B628C30DA0}" name="Nontraditional Program Enrollment Rate (Perkins)" dataDxfId="10"/>
-    <tableColumn id="29" xr3:uid="{612816CA-7F21-1C4E-9A0F-5C68D82ADF7D}" name="# Students who took Dual Credit classes Grade 9" dataDxfId="9"/>
-    <tableColumn id="30" xr3:uid="{5753F583-62B9-8A44-A3EC-546C676CE502}" name="# Students who took Dual Credit classes Grade 10" dataDxfId="8"/>
-    <tableColumn id="31" xr3:uid="{99388DA0-03B4-324C-93D0-00C4E7DFFD44}" name="# Students who took Dual Credit classes Grade 11" dataDxfId="7"/>
-    <tableColumn id="32" xr3:uid="{100FC056-2E22-0C4B-9AAC-CCBAF3958BB5}" name="# Students who took Dual Credit classes Grade 12" dataDxfId="6"/>
-    <tableColumn id="33" xr3:uid="{7148123E-CBBF-7A4C-A783-2B28AF22F11E}" name="# Students enrolled in Dual Credit Coursework" dataDxfId="5"/>
-    <tableColumn id="34" xr3:uid="{9282E612-FE85-D14F-B5B4-F790B296E915}" name="% Students enrolled in Dual Credit Coursework" dataDxfId="4"/>
-    <tableColumn id="35" xr3:uid="{62431BD2-7051-FC48-BD9B-525CBF545DDD}" name="# Students who took AP classes Grade 9" dataDxfId="3"/>
-    <tableColumn id="36" xr3:uid="{73C469BE-B611-0145-B886-AAA2CB70EAE8}" name="# Students who took AP classes Grade 10" dataDxfId="2"/>
-    <tableColumn id="37" xr3:uid="{CFE88FEF-98CA-654A-B3B8-05790EA4E553}" name="# Students who took AP classes Grade 11" dataDxfId="1"/>
-    <tableColumn id="38" xr3:uid="{CB531B3F-8204-2644-91D3-88ACB4BFD0A7}" name="# Students who took AP classes Grade 12" dataDxfId="0"/>
+  <tableColumns count="53">
+    <tableColumn id="1" xr3:uid="{6DA6945B-9D7D-0142-A374-7C4A97BBBBAB}" name="Year" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{1617EDAF-51CD-413F-9022-F6E4C97C233F}" name="RCDTS" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{A67D85A4-5303-744E-B7CD-31ECBC6CE0A7}" name="Type" dataDxfId="59"/>
+    <tableColumn id="13" xr3:uid="{C8F50192-B0A1-D84D-96D9-819955E9CE26}" name="District Type" dataDxfId="58"/>
+    <tableColumn id="14" xr3:uid="{A7661728-A363-9840-8182-CBC0352B14C6}" name="School Type" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{94336B41-A312-184A-9F00-C5E1720E28AF}" name="School Name" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{7516DA0D-E868-1941-B0D3-80B0E523A018}" name="District Name" dataDxfId="55"/>
+    <tableColumn id="10" xr3:uid="{DCD59F4B-C55C-2846-9070-7F8CC6CA2F51}" name="City" dataDxfId="54"/>
+    <tableColumn id="11" xr3:uid="{AB642454-853E-F049-84B7-745455B992F3}" name="County" dataDxfId="53"/>
+    <tableColumn id="9" xr3:uid="{5B5F7B45-CEFB-EE48-90E0-380BD11BD347}" name="Student Enrollment" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{DC5BC21C-5B26-D441-96D3-64D606494C9A}" name="Student Attendance Rate" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{16C5B399-2D53-AF41-815C-1F7C3259622D}" name="Student Chronic Truancy Rate" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{E3173650-9CBD-2046-9561-EC76593F21A4}" name="Chronic Absenteeism" dataDxfId="49"/>
+    <tableColumn id="12" xr3:uid="{A5C89E32-E6C7-354A-AD94-8B9E7BF5BEAF}" name="Total Teacher FTE" dataDxfId="48"/>
+    <tableColumn id="15" xr3:uid="{91CEEB72-10AD-5347-AD91-C2EA26951FFD}" name="Teacher Retention Rate" dataDxfId="47"/>
+    <tableColumn id="16" xr3:uid="{B95926A8-CE9E-5E4C-8517-F53E1DD6BB12}" name="Pupil Teacher Ratio - Elementary" dataDxfId="46"/>
+    <tableColumn id="17" xr3:uid="{66E6EF1B-5F71-724F-BE1B-2EAE768FA6E4}" name="Pupil Teacher Ratio - High School" dataDxfId="45"/>
+    <tableColumn id="18" xr3:uid="{FF7C5CB9-8A3F-654A-AAC2-F90DDD57691C}" name="% Novice Teachers" dataDxfId="44"/>
+    <tableColumn id="21" xr3:uid="{14F53AE3-04FD-0049-9CD6-2E8BE716335E}" name="% Novice Teachers - High Poverty Schools" dataDxfId="43"/>
+    <tableColumn id="22" xr3:uid="{1A89C2C1-D5B1-D84E-AF9A-AFFF73A90C04}" name="% Novice Teachers - Low Poverty Schools" dataDxfId="42"/>
+    <tableColumn id="19" xr3:uid="{31BB3C4C-CD8A-9848-85A3-6A3A4A977857}" name="% 8th Grade Passing Algebra 1" dataDxfId="41"/>
+    <tableColumn id="20" xr3:uid="{7DC2CAA5-3B64-9C42-8E87-31C44668510E}" name="% 9th Grade on Track" dataDxfId="40"/>
+    <tableColumn id="23" xr3:uid="{AD3426F6-72EB-7A4F-BA71-66C2A3294CCF}" name="# 9th Grade on Track" dataDxfId="39"/>
+    <tableColumn id="24" xr3:uid="{7124EEF3-D182-7A4B-A827-DEC5EE0B1591}" name="# CTE Enrollment" dataDxfId="38"/>
+    <tableColumn id="25" xr3:uid="{0206B422-7E9A-AF41-A20D-0A4445D084F7}" name="# CTE Participants" dataDxfId="37"/>
+    <tableColumn id="26" xr3:uid="{74152CBC-6192-FA44-8D72-64E4E7284B17}" name="4-Year Graduation Rate (Perkins)" dataDxfId="36"/>
+    <tableColumn id="27" xr3:uid="{E91D57BE-E786-0E41-A6C9-D40C584A25B7}" name="Postsecondary Placement Rate (Perkins)" dataDxfId="35"/>
+    <tableColumn id="28" xr3:uid="{61C1EAC6-2067-F84E-B17C-A8B628C30DA0}" name="Nontraditional Program Enrollment Rate (Perkins)" dataDxfId="34"/>
+    <tableColumn id="29" xr3:uid="{612816CA-7F21-1C4E-9A0F-5C68D82ADF7D}" name="# Students who took Dual Credit classes Grade 9" dataDxfId="33"/>
+    <tableColumn id="30" xr3:uid="{5753F583-62B9-8A44-A3EC-546C676CE502}" name="# Students who took Dual Credit classes Grade 10" dataDxfId="32"/>
+    <tableColumn id="31" xr3:uid="{99388DA0-03B4-324C-93D0-00C4E7DFFD44}" name="# Students who took Dual Credit classes Grade 11" dataDxfId="31"/>
+    <tableColumn id="32" xr3:uid="{100FC056-2E22-0C4B-9AAC-CCBAF3958BB5}" name="# Students who took Dual Credit classes Grade 12" dataDxfId="30"/>
+    <tableColumn id="33" xr3:uid="{7148123E-CBBF-7A4C-A783-2B28AF22F11E}" name="# Students enrolled in Dual Credit Coursework" dataDxfId="29"/>
+    <tableColumn id="34" xr3:uid="{9282E612-FE85-D14F-B5B4-F790B296E915}" name="% Students enrolled in Dual Credit Coursework" dataDxfId="28"/>
+    <tableColumn id="35" xr3:uid="{62431BD2-7051-FC48-BD9B-525CBF545DDD}" name="# Students who took AP classes Grade 9" dataDxfId="27"/>
+    <tableColumn id="36" xr3:uid="{73C469BE-B611-0145-B886-AAA2CB70EAE8}" name="# Students who took AP classes Grade 10" dataDxfId="26"/>
+    <tableColumn id="37" xr3:uid="{CFE88FEF-98CA-654A-B3B8-05790EA4E553}" name="# Students who took AP classes Grade 11" dataDxfId="25"/>
+    <tableColumn id="38" xr3:uid="{CB531B3F-8204-2644-91D3-88ACB4BFD0A7}" name="# Students who took AP classes Grade 12" dataDxfId="24"/>
+    <tableColumn id="39" xr3:uid="{97ED4799-6B71-FF44-A7E9-0D6FEC826075}" name="# Students who took IB classes Grade 9" dataDxfId="23"/>
+    <tableColumn id="40" xr3:uid="{F30102B8-881A-CA42-88CE-89D1D66A2AFB}" name="# Students who took IB classes Grade 10" dataDxfId="22"/>
+    <tableColumn id="41" xr3:uid="{99E2E959-F950-414B-BBF3-82CF023E0766}" name="# Students who took IB classes Grade 11" dataDxfId="21"/>
+    <tableColumn id="42" xr3:uid="{E9437747-1EEE-D94C-8B2E-5EB4508C3746}" name="# Students who took IB classes Grade 12" dataDxfId="20"/>
+    <tableColumn id="43" xr3:uid="{3CBA554F-964A-B546-B1CB-F3FFBC958E43}" name="# Out-of-Field Teachers" dataDxfId="19"/>
+    <tableColumn id="44" xr3:uid="{C4CCD547-D042-A040-8E97-CD2FA1F749A9}" name="% Out-of-Field Teachers" dataDxfId="18"/>
+    <tableColumn id="45" xr3:uid="{DC129293-5D55-4C48-A979-6304ABE3CAB9}" name="% Teachers with Short-Term or Provisional License" dataDxfId="17"/>
+    <tableColumn id="46" xr3:uid="{69922C1F-B1F6-AA41-8916-728215E1A659}" name="% Teachers with Short-Term or Provisional License - High Poverty Schools" dataDxfId="16"/>
+    <tableColumn id="47" xr3:uid="{CB9F66DB-18B6-4A41-A560-2737C375BEAA}" name="% Teachers with Short-Term or Provisional License - Low Poverty Schools" dataDxfId="15"/>
+    <tableColumn id="48" xr3:uid="{FA593E29-37FA-2F49-B1E2-8A20B24707C0}" name="# Teachers with Short-Term or Provisional License - High Poverty Schools" dataDxfId="14"/>
+    <tableColumn id="49" xr3:uid="{F17AD799-AAF2-CA4B-9052-79526ED68F55}" name="# Teachers with Short-Term or Provisional License - Low Poverty Schools" dataDxfId="13"/>
+    <tableColumn id="50" xr3:uid="{95D43F71-6E78-7545-8A4C-AE8258AA92BA}" name="Teacher Attendance Rate" dataDxfId="12"/>
+    <tableColumn id="51" xr3:uid="{35904462-8ACF-104B-8595-F9EDDB9D005D}" name="Principal Turnover within 6 Years" dataDxfId="11"/>
+    <tableColumn id="52" xr3:uid="{37C54579-1382-4047-B32E-9B6DCF4C6D1A}" name="High School 4-Year Graduation Rate" dataDxfId="10"/>
+    <tableColumn id="53" xr3:uid="{76C7C142-3803-C743-ACB8-2AC253A56510}" name="High School 6-Year Graduation Rate" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}" name="Table44" displayName="Table44" ref="A1:H353" totalsRowShown="0" dataDxfId="47" tableBorderDxfId="46">
-  <autoFilter ref="A1:H353" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}" name="Table44" displayName="Table44" ref="A1:H468" totalsRowShown="0" dataDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A1:H468" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H323">
     <sortCondition ref="B1:B323"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{CF003222-4DDE-BB47-A657-1775812A7CF9}" name="Year" dataDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{75198FC7-15E7-C749-9856-FF87007012FD}" name="Metric" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{250849D7-E98C-6047-AD29-C748E7E94296}" name="Original Metric" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{2B055042-83EA-3F40-9F97-2E2C80BE4FCE}" name="Sheet" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{FCF3CEDF-90EF-DD4A-BD7C-2C3BB2D372C6}" name="Disaggregated" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{E905735F-4B71-1A4E-AA00-10B4AAD2B5F6}" name="Disaggregation Details" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{CF003222-4DDE-BB47-A657-1775812A7CF9}" name="Year" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{75198FC7-15E7-C749-9856-FF87007012FD}" name="Metric" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{250849D7-E98C-6047-AD29-C748E7E94296}" name="Original Metric" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{2B055042-83EA-3F40-9F97-2E2C80BE4FCE}" name="Sheet" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{FCF3CEDF-90EF-DD4A-BD7C-2C3BB2D372C6}" name="Disaggregated" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{E905735F-4B71-1A4E-AA00-10B4AAD2B5F6}" name="Disaggregation Details" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{6FC8DE02-1AAB-8248-8E52-B299C7FFB44A}" name="Disaggregation Format"/>
-    <tableColumn id="6" xr3:uid="{89643796-F484-D048-862D-B85A1B6BB907}" name="Special Format" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{89643796-F484-D048-862D-B85A1B6BB907}" name="Special Format" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2440,11 +2814,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL17"/>
+  <dimension ref="A1:BA26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AF1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AI23" sqref="AI23"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I22" sqref="I22:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2484,9 +2858,21 @@
     <col min="34" max="34" width="41" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="42.5" bestFit="1" customWidth="1"/>
     <col min="36" max="38" width="56.1640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="42" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="22" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="61.5" bestFit="1" customWidth="1"/>
+    <col min="47" max="48" width="61" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="42.83203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:53" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2601,8 +2987,53 @@
       <c r="AL1" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AM1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>208</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>228</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2008</v>
       </c>
@@ -2626,7 +3057,7 @@
         <v>53</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>54</v>
+        <v>233</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>48</v>
@@ -2646,12 +3077,20 @@
       <c r="Q2" t="s">
         <v>83</v>
       </c>
-      <c r="AI2" s="16"/>
-      <c r="AJ2" s="16"/>
-      <c r="AK2" s="16"/>
-      <c r="AL2" s="16"/>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AS2" t="s">
+        <v>210</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>211</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>212</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2009</v>
       </c>
@@ -2675,7 +3114,7 @@
         <v>53</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>54</v>
+        <v>233</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>48</v>
@@ -2695,12 +3134,20 @@
       <c r="Q3" t="s">
         <v>83</v>
       </c>
-      <c r="AI3" s="16"/>
-      <c r="AJ3" s="16"/>
-      <c r="AK3" s="16"/>
-      <c r="AL3" s="16"/>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AS3" t="s">
+        <v>210</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>211</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>212</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2010</v>
       </c>
@@ -2724,7 +3171,7 @@
         <v>53</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>54</v>
+        <v>233</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>48</v>
@@ -2744,12 +3191,20 @@
       <c r="Q4" t="s">
         <v>83</v>
       </c>
-      <c r="AI4" s="16"/>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="16"/>
-      <c r="AL4" s="16"/>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AS4" t="s">
+        <v>210</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>211</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>212</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2011</v>
       </c>
@@ -2773,7 +3228,7 @@
         <v>53</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>54</v>
+        <v>233</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>48</v>
@@ -2793,12 +3248,20 @@
       <c r="Q5" t="s">
         <v>83</v>
       </c>
-      <c r="AI5" s="16"/>
-      <c r="AJ5" s="16"/>
-      <c r="AK5" s="16"/>
-      <c r="AL5" s="16"/>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AS5" t="s">
+        <v>210</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>211</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>212</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2012</v>
       </c>
@@ -2822,7 +3285,7 @@
         <v>53</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>54</v>
+        <v>233</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>48</v>
@@ -2842,12 +3305,20 @@
       <c r="Q6" t="s">
         <v>83</v>
       </c>
-      <c r="AI6" s="16"/>
-      <c r="AJ6" s="16"/>
-      <c r="AK6" s="16"/>
-      <c r="AL6" s="16"/>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AS6" t="s">
+        <v>210</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>211</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>212</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2013</v>
       </c>
@@ -2871,7 +3342,7 @@
         <v>53</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>54</v>
+        <v>233</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>48</v>
@@ -2891,12 +3362,20 @@
       <c r="Q7" t="s">
         <v>84</v>
       </c>
-      <c r="AI7" s="16"/>
-      <c r="AJ7" s="16"/>
-      <c r="AK7" s="16"/>
-      <c r="AL7" s="16"/>
-    </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AS7" t="s">
+        <v>213</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>214</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>215</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2014</v>
       </c>
@@ -2920,7 +3399,7 @@
         <v>53</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>54</v>
+        <v>233</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>48</v>
@@ -2946,12 +3425,23 @@
       <c r="V8" t="s">
         <v>90</v>
       </c>
-      <c r="AI8" s="16"/>
-      <c r="AJ8" s="16"/>
-      <c r="AK8" s="16"/>
-      <c r="AL8" s="16"/>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AS8" t="s">
+        <v>210</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>211</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>212</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>219</v>
+      </c>
+      <c r="AZ8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2015</v>
       </c>
@@ -2975,7 +3465,7 @@
         <v>53</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>54</v>
+        <v>233</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>48</v>
@@ -3004,12 +3494,23 @@
       <c r="V9" t="s">
         <v>90</v>
       </c>
-      <c r="AI9" s="16"/>
-      <c r="AJ9" s="16"/>
-      <c r="AK9" s="16"/>
-      <c r="AL9" s="16"/>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AS9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>211</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>212</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>219</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2016</v>
       </c>
@@ -3033,7 +3534,7 @@
         <v>53</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>54</v>
+        <v>233</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>48</v>
@@ -3074,18 +3575,38 @@
       <c r="AF10" t="s">
         <v>124</v>
       </c>
-      <c r="AI10" s="16"/>
-      <c r="AJ10" s="16" t="s">
+      <c r="AJ10" t="s">
         <v>153</v>
       </c>
-      <c r="AK10" s="16" t="s">
+      <c r="AK10" t="s">
         <v>159</v>
       </c>
-      <c r="AL10" s="16" t="s">
+      <c r="AL10" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AN10" t="s">
+        <v>178</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>180</v>
+      </c>
+      <c r="AX10" t="s">
+        <v>216</v>
+      </c>
+      <c r="AY10" t="s">
+        <v>219</v>
+      </c>
+      <c r="AZ10" t="s">
+        <v>223</v>
+      </c>
+      <c r="BA10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2017</v>
       </c>
@@ -3109,7 +3630,7 @@
         <v>53</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>54</v>
+        <v>233</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>48</v>
@@ -3150,18 +3671,38 @@
       <c r="AF11" t="s">
         <v>124</v>
       </c>
-      <c r="AI11" s="16"/>
-      <c r="AJ11" s="16" t="s">
+      <c r="AJ11" t="s">
         <v>153</v>
       </c>
-      <c r="AK11" s="16" t="s">
+      <c r="AK11" t="s">
         <v>159</v>
       </c>
-      <c r="AL11" s="16" t="s">
+      <c r="AL11" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AN11" t="s">
+        <v>178</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>180</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>216</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>219</v>
+      </c>
+      <c r="AZ11" t="s">
+        <v>223</v>
+      </c>
+      <c r="BA11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -3240,20 +3781,50 @@
       <c r="AF12" t="s">
         <v>128</v>
       </c>
-      <c r="AI12" s="16" t="s">
+      <c r="AI12" t="s">
         <v>149</v>
       </c>
-      <c r="AJ12" s="16" t="s">
+      <c r="AJ12" t="s">
         <v>155</v>
       </c>
-      <c r="AK12" s="16" t="s">
+      <c r="AK12" t="s">
         <v>161</v>
       </c>
-      <c r="AL12" s="16" t="s">
+      <c r="AL12" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AM12" t="s">
+        <v>181</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>182</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>183</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>184</v>
+      </c>
+      <c r="AV12" t="s">
+        <v>203</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>204</v>
+      </c>
+      <c r="AX12" t="s">
+        <v>217</v>
+      </c>
+      <c r="AY12" t="s">
+        <v>220</v>
+      </c>
+      <c r="AZ12" t="s">
+        <v>225</v>
+      </c>
+      <c r="BA12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2019</v>
       </c>
@@ -3338,20 +3909,53 @@
       <c r="AF13" t="s">
         <v>119</v>
       </c>
-      <c r="AI13" s="16" t="s">
+      <c r="AI13" t="s">
         <v>151</v>
       </c>
-      <c r="AJ13" s="16" t="s">
+      <c r="AJ13" t="s">
         <v>157</v>
       </c>
-      <c r="AK13" s="16" t="s">
+      <c r="AK13" t="s">
         <v>163</v>
       </c>
-      <c r="AL13" s="16" t="s">
+      <c r="AL13" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AM13" t="s">
+        <v>185</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>186</v>
+      </c>
+      <c r="AO13" t="s">
+        <v>187</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>188</v>
+      </c>
+      <c r="AS13" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>206</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>207</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>217</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>220</v>
+      </c>
+      <c r="AZ13" t="s">
+        <v>225</v>
+      </c>
+      <c r="BA13" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2020</v>
       </c>
@@ -3436,20 +4040,53 @@
       <c r="AF14" t="s">
         <v>119</v>
       </c>
-      <c r="AI14" s="16" t="s">
+      <c r="AI14" t="s">
         <v>151</v>
       </c>
-      <c r="AJ14" s="16" t="s">
+      <c r="AJ14" t="s">
         <v>157</v>
       </c>
-      <c r="AK14" s="16" t="s">
+      <c r="AK14" t="s">
         <v>163</v>
       </c>
-      <c r="AL14" s="16" t="s">
+      <c r="AL14" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AM14" t="s">
+        <v>185</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>186</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>187</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>188</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>206</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>207</v>
+      </c>
+      <c r="AX14" t="s">
+        <v>217</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>220</v>
+      </c>
+      <c r="AZ14" t="s">
+        <v>225</v>
+      </c>
+      <c r="BA14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2021</v>
       </c>
@@ -3540,20 +4177,53 @@
       <c r="AH15" t="s">
         <v>147</v>
       </c>
-      <c r="AI15" s="16" t="s">
+      <c r="AI15" t="s">
         <v>151</v>
       </c>
-      <c r="AJ15" s="16" t="s">
+      <c r="AJ15" t="s">
         <v>157</v>
       </c>
-      <c r="AK15" s="16" t="s">
+      <c r="AK15" t="s">
         <v>163</v>
       </c>
-      <c r="AL15" s="16" t="s">
+      <c r="AL15" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AM15" t="s">
+        <v>185</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>186</v>
+      </c>
+      <c r="AO15" t="s">
+        <v>187</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>188</v>
+      </c>
+      <c r="AS15" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>206</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>207</v>
+      </c>
+      <c r="AX15" t="s">
+        <v>217</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>220</v>
+      </c>
+      <c r="AZ15" t="s">
+        <v>225</v>
+      </c>
+      <c r="BA15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2022</v>
       </c>
@@ -3656,20 +4326,53 @@
       <c r="AH16" t="s">
         <v>147</v>
       </c>
-      <c r="AI16" s="16" t="s">
+      <c r="AI16" t="s">
         <v>151</v>
       </c>
-      <c r="AJ16" s="16" t="s">
+      <c r="AJ16" t="s">
         <v>157</v>
       </c>
-      <c r="AK16" s="16" t="s">
+      <c r="AK16" t="s">
         <v>163</v>
       </c>
-      <c r="AL16" s="16" t="s">
+      <c r="AL16" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AM16" t="s">
+        <v>185</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>186</v>
+      </c>
+      <c r="AO16" t="s">
+        <v>187</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>188</v>
+      </c>
+      <c r="AS16" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>206</v>
+      </c>
+      <c r="AU16" t="s">
+        <v>207</v>
+      </c>
+      <c r="AX16" t="s">
+        <v>217</v>
+      </c>
+      <c r="AY16" t="s">
+        <v>220</v>
+      </c>
+      <c r="AZ16" t="s">
+        <v>225</v>
+      </c>
+      <c r="BA16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2023</v>
       </c>
@@ -3769,18 +4472,63 @@
       <c r="AH17" t="s">
         <v>147</v>
       </c>
-      <c r="AI17" s="16" t="s">
+      <c r="AI17" t="s">
         <v>151</v>
       </c>
-      <c r="AJ17" s="16" t="s">
+      <c r="AJ17" t="s">
         <v>157</v>
       </c>
-      <c r="AK17" s="16" t="s">
+      <c r="AK17" t="s">
         <v>163</v>
       </c>
-      <c r="AL17" s="16" t="s">
+      <c r="AL17" t="s">
         <v>169</v>
       </c>
+      <c r="AM17" t="s">
+        <v>185</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>186</v>
+      </c>
+      <c r="AO17" t="s">
+        <v>187</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>188</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>200</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>201</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>206</v>
+      </c>
+      <c r="AU17" t="s">
+        <v>207</v>
+      </c>
+      <c r="AX17" t="s">
+        <v>217</v>
+      </c>
+      <c r="AY17" t="s">
+        <v>220</v>
+      </c>
+      <c r="AZ17" t="s">
+        <v>225</v>
+      </c>
+      <c r="BA17" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="AZ19" s="18"/>
+    </row>
+    <row r="26" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="AP26" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3794,12 +4542,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249B090D-D7BB-374A-9D81-FFCE8C0599DD}">
-  <dimension ref="A1:H353"/>
+  <dimension ref="A1:H468"/>
   <sheetViews>
-    <sheetView topLeftCell="A320" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView topLeftCell="A436" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A162" sqref="A162"/>
-      <selection pane="topRight" activeCell="G351" sqref="G351"/>
+      <selection pane="topRight" activeCell="C446" sqref="C446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9737,7 +10485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>2021</v>
       </c>
@@ -9754,7 +10502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>2022</v>
       </c>
@@ -9771,7 +10519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>2023</v>
       </c>
@@ -9788,667 +10536,2725 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A324" s="16">
+    <row r="324" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A324">
         <v>2018</v>
       </c>
-      <c r="B324" s="17" t="s">
+      <c r="B324" t="s">
         <v>148</v>
       </c>
-      <c r="C324" s="16" t="s">
+      <c r="C324" t="s">
         <v>149</v>
       </c>
-      <c r="D324" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E324" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F324" s="16"/>
+      <c r="D324" t="s">
+        <v>34</v>
+      </c>
+      <c r="E324" t="b">
+        <v>1</v>
+      </c>
       <c r="G324" t="s">
         <v>150</v>
       </c>
-      <c r="H324" s="16"/>
-    </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A325" s="16">
+    </row>
+    <row r="325" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A325">
         <v>2019</v>
       </c>
-      <c r="B325" s="17" t="s">
+      <c r="B325" t="s">
         <v>148</v>
       </c>
-      <c r="C325" s="16" t="s">
+      <c r="C325" t="s">
         <v>151</v>
       </c>
-      <c r="D325" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E325" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F325" s="16"/>
+      <c r="D325" t="s">
+        <v>34</v>
+      </c>
+      <c r="E325" t="b">
+        <v>1</v>
+      </c>
       <c r="G325" t="s">
         <v>170</v>
       </c>
-      <c r="H325" s="16"/>
-    </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A326" s="16">
+    </row>
+    <row r="326" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A326">
         <v>2020</v>
       </c>
-      <c r="B326" s="17" t="s">
+      <c r="B326" t="s">
         <v>148</v>
       </c>
-      <c r="C326" s="16" t="s">
+      <c r="C326" t="s">
         <v>151</v>
       </c>
-      <c r="D326" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E326" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F326" s="16"/>
+      <c r="D326" t="s">
+        <v>34</v>
+      </c>
+      <c r="E326" t="b">
+        <v>1</v>
+      </c>
       <c r="G326" t="s">
         <v>170</v>
       </c>
-      <c r="H326" s="16"/>
-    </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A327" s="16">
+    </row>
+    <row r="327" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A327">
         <v>2021</v>
       </c>
-      <c r="B327" s="17" t="s">
+      <c r="B327" t="s">
         <v>148</v>
       </c>
-      <c r="C327" s="16" t="s">
+      <c r="C327" t="s">
         <v>151</v>
       </c>
-      <c r="D327" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E327" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F327" s="16"/>
+      <c r="D327" t="s">
+        <v>34</v>
+      </c>
+      <c r="E327" t="b">
+        <v>1</v>
+      </c>
       <c r="G327" t="s">
         <v>170</v>
       </c>
-      <c r="H327" s="16"/>
-    </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A328" s="16">
+    </row>
+    <row r="328" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A328">
         <v>2022</v>
       </c>
-      <c r="B328" s="17" t="s">
+      <c r="B328" t="s">
         <v>148</v>
       </c>
-      <c r="C328" s="16" t="s">
+      <c r="C328" t="s">
         <v>151</v>
       </c>
-      <c r="D328" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E328" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F328" s="16"/>
+      <c r="D328" t="s">
+        <v>34</v>
+      </c>
+      <c r="E328" t="b">
+        <v>1</v>
+      </c>
       <c r="G328" t="s">
         <v>170</v>
       </c>
-      <c r="H328" s="16"/>
-    </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A329" s="16">
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A329">
         <v>2023</v>
       </c>
-      <c r="B329" s="17" t="s">
+      <c r="B329" t="s">
         <v>148</v>
       </c>
-      <c r="C329" s="16" t="s">
+      <c r="C329" t="s">
         <v>151</v>
       </c>
-      <c r="D329" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E329" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F329" s="16"/>
+      <c r="D329" t="s">
+        <v>34</v>
+      </c>
+      <c r="E329" t="b">
+        <v>1</v>
+      </c>
       <c r="G329" t="s">
         <v>170</v>
       </c>
-      <c r="H329" s="16"/>
-    </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A330" s="16">
+    </row>
+    <row r="330" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A330">
         <v>2016</v>
       </c>
-      <c r="B330" s="17" t="s">
+      <c r="B330" t="s">
         <v>152</v>
       </c>
-      <c r="C330" s="16" t="s">
+      <c r="C330" t="s">
         <v>153</v>
       </c>
-      <c r="D330" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E330" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F330" s="16"/>
+      <c r="D330" t="s">
+        <v>37</v>
+      </c>
+      <c r="E330" t="b">
+        <v>1</v>
+      </c>
       <c r="G330" t="s">
         <v>154</v>
       </c>
-      <c r="H330" s="16"/>
-    </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A331" s="16">
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A331">
         <v>2017</v>
       </c>
-      <c r="B331" s="17" t="s">
+      <c r="B331" t="s">
         <v>152</v>
       </c>
-      <c r="C331" s="16" t="s">
+      <c r="C331" t="s">
         <v>153</v>
       </c>
-      <c r="D331" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E331" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F331" s="16" t="b">
+      <c r="D331" t="s">
+        <v>37</v>
+      </c>
+      <c r="E331" t="b">
+        <v>1</v>
+      </c>
+      <c r="F331" t="b">
         <v>1</v>
       </c>
       <c r="G331" t="s">
         <v>154</v>
       </c>
-      <c r="H331" s="16"/>
-    </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A332" s="16">
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A332">
         <v>2018</v>
       </c>
-      <c r="B332" s="17" t="s">
+      <c r="B332" t="s">
         <v>152</v>
       </c>
-      <c r="C332" s="16" t="s">
+      <c r="C332" t="s">
         <v>155</v>
       </c>
-      <c r="D332" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E332" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F332" s="16"/>
+      <c r="D332" t="s">
+        <v>34</v>
+      </c>
+      <c r="E332" t="b">
+        <v>1</v>
+      </c>
       <c r="G332" t="s">
         <v>156</v>
       </c>
-      <c r="H332" s="16"/>
-    </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A333" s="16">
+    </row>
+    <row r="333" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A333">
         <v>2019</v>
       </c>
-      <c r="B333" s="17" t="s">
+      <c r="B333" t="s">
         <v>152</v>
       </c>
-      <c r="C333" s="16" t="s">
+      <c r="C333" t="s">
         <v>157</v>
       </c>
-      <c r="D333" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E333" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F333" s="16"/>
+      <c r="D333" t="s">
+        <v>34</v>
+      </c>
+      <c r="E333" t="b">
+        <v>1</v>
+      </c>
       <c r="G333" t="s">
         <v>171</v>
       </c>
-      <c r="H333" s="16"/>
-    </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A334" s="16">
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A334">
         <v>2020</v>
       </c>
-      <c r="B334" s="17" t="s">
+      <c r="B334" t="s">
         <v>152</v>
       </c>
-      <c r="C334" s="16" t="s">
+      <c r="C334" t="s">
         <v>157</v>
       </c>
-      <c r="D334" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E334" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F334" s="16"/>
+      <c r="D334" t="s">
+        <v>34</v>
+      </c>
+      <c r="E334" t="b">
+        <v>1</v>
+      </c>
       <c r="G334" t="s">
         <v>171</v>
       </c>
-      <c r="H334" s="16"/>
-    </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A335" s="16">
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A335">
         <v>2021</v>
       </c>
-      <c r="B335" s="17" t="s">
+      <c r="B335" t="s">
         <v>152</v>
       </c>
-      <c r="C335" s="16" t="s">
+      <c r="C335" t="s">
         <v>157</v>
       </c>
-      <c r="D335" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E335" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F335" s="16"/>
+      <c r="D335" t="s">
+        <v>34</v>
+      </c>
+      <c r="E335" t="b">
+        <v>1</v>
+      </c>
       <c r="G335" t="s">
         <v>171</v>
       </c>
-      <c r="H335" s="16"/>
-    </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A336" s="16">
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A336">
         <v>2022</v>
       </c>
-      <c r="B336" s="17" t="s">
+      <c r="B336" t="s">
         <v>152</v>
       </c>
-      <c r="C336" s="16" t="s">
+      <c r="C336" t="s">
         <v>157</v>
       </c>
-      <c r="D336" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E336" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F336" s="16"/>
+      <c r="D336" t="s">
+        <v>34</v>
+      </c>
+      <c r="E336" t="b">
+        <v>1</v>
+      </c>
       <c r="G336" t="s">
         <v>171</v>
       </c>
-      <c r="H336" s="16"/>
-    </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A337" s="16">
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A337">
         <v>2023</v>
       </c>
-      <c r="B337" s="17" t="s">
+      <c r="B337" t="s">
         <v>152</v>
       </c>
-      <c r="C337" s="16" t="s">
+      <c r="C337" t="s">
         <v>157</v>
       </c>
-      <c r="D337" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E337" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F337" s="16"/>
+      <c r="D337" t="s">
+        <v>34</v>
+      </c>
+      <c r="E337" t="b">
+        <v>1</v>
+      </c>
       <c r="G337" t="s">
         <v>171</v>
       </c>
-      <c r="H337" s="16"/>
-    </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A338" s="16">
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A338">
         <v>2016</v>
       </c>
-      <c r="B338" s="17" t="s">
+      <c r="B338" t="s">
         <v>158</v>
       </c>
-      <c r="C338" s="16" t="s">
+      <c r="C338" t="s">
         <v>159</v>
       </c>
-      <c r="D338" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E338" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F338" s="16"/>
+      <c r="D338" t="s">
+        <v>37</v>
+      </c>
+      <c r="E338" t="b">
+        <v>1</v>
+      </c>
       <c r="G338" t="s">
         <v>160</v>
       </c>
-      <c r="H338" s="16"/>
-    </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A339" s="16">
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A339">
         <v>2017</v>
       </c>
-      <c r="B339" s="17" t="s">
+      <c r="B339" t="s">
         <v>158</v>
       </c>
-      <c r="C339" s="16" t="s">
+      <c r="C339" t="s">
         <v>159</v>
       </c>
-      <c r="D339" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E339" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F339" s="16"/>
+      <c r="D339" t="s">
+        <v>37</v>
+      </c>
+      <c r="E339" t="b">
+        <v>1</v>
+      </c>
       <c r="G339" t="s">
         <v>160</v>
       </c>
-      <c r="H339" s="16"/>
-    </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A340" s="16">
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A340">
         <v>2018</v>
       </c>
-      <c r="B340" s="17" t="s">
+      <c r="B340" t="s">
         <v>158</v>
       </c>
-      <c r="C340" s="16" t="s">
+      <c r="C340" t="s">
         <v>161</v>
       </c>
-      <c r="D340" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E340" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F340" s="16"/>
+      <c r="D340" t="s">
+        <v>34</v>
+      </c>
+      <c r="E340" t="b">
+        <v>1</v>
+      </c>
       <c r="G340" t="s">
         <v>162</v>
       </c>
-      <c r="H340" s="16"/>
-    </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A341" s="16">
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A341">
         <v>2019</v>
       </c>
-      <c r="B341" s="17" t="s">
+      <c r="B341" t="s">
         <v>158</v>
       </c>
-      <c r="C341" s="16" t="s">
+      <c r="C341" t="s">
         <v>163</v>
       </c>
-      <c r="D341" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E341" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F341" s="16"/>
+      <c r="D341" t="s">
+        <v>34</v>
+      </c>
+      <c r="E341" t="b">
+        <v>1</v>
+      </c>
       <c r="G341" t="s">
         <v>172</v>
       </c>
-      <c r="H341" s="16"/>
-    </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A342" s="16">
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A342">
         <v>2020</v>
       </c>
-      <c r="B342" s="17" t="s">
+      <c r="B342" t="s">
         <v>158</v>
       </c>
-      <c r="C342" s="16" t="s">
+      <c r="C342" t="s">
         <v>163</v>
       </c>
-      <c r="D342" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E342" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F342" s="16"/>
+      <c r="D342" t="s">
+        <v>34</v>
+      </c>
+      <c r="E342" t="b">
+        <v>1</v>
+      </c>
       <c r="G342" t="s">
         <v>172</v>
       </c>
-      <c r="H342" s="16"/>
-    </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A343" s="16">
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A343">
         <v>2021</v>
       </c>
-      <c r="B343" s="17" t="s">
+      <c r="B343" t="s">
         <v>158</v>
       </c>
-      <c r="C343" s="16" t="s">
+      <c r="C343" t="s">
         <v>163</v>
       </c>
-      <c r="D343" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E343" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F343" s="16"/>
+      <c r="D343" t="s">
+        <v>34</v>
+      </c>
+      <c r="E343" t="b">
+        <v>1</v>
+      </c>
       <c r="G343" t="s">
         <v>172</v>
       </c>
-      <c r="H343" s="16"/>
-    </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A344" s="16">
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A344">
         <v>2022</v>
       </c>
-      <c r="B344" s="17" t="s">
+      <c r="B344" t="s">
         <v>158</v>
       </c>
-      <c r="C344" s="16" t="s">
+      <c r="C344" t="s">
         <v>163</v>
       </c>
-      <c r="D344" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E344" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F344" s="16"/>
+      <c r="D344" t="s">
+        <v>34</v>
+      </c>
+      <c r="E344" t="b">
+        <v>1</v>
+      </c>
       <c r="G344" t="s">
         <v>172</v>
       </c>
-      <c r="H344" s="16"/>
-    </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A345" s="16">
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A345">
         <v>2023</v>
       </c>
-      <c r="B345" s="17" t="s">
+      <c r="B345" t="s">
         <v>158</v>
       </c>
-      <c r="C345" s="16" t="s">
+      <c r="C345" t="s">
         <v>163</v>
       </c>
-      <c r="D345" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E345" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F345" s="16"/>
+      <c r="D345" t="s">
+        <v>34</v>
+      </c>
+      <c r="E345" t="b">
+        <v>1</v>
+      </c>
       <c r="G345" t="s">
         <v>172</v>
       </c>
-      <c r="H345" s="16"/>
-    </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A346" s="16">
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A346">
         <v>2016</v>
       </c>
-      <c r="B346" s="17" t="s">
+      <c r="B346" t="s">
         <v>164</v>
       </c>
-      <c r="C346" s="16" t="s">
+      <c r="C346" t="s">
         <v>165</v>
       </c>
-      <c r="D346" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E346" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F346" s="16"/>
+      <c r="D346" t="s">
+        <v>37</v>
+      </c>
+      <c r="E346" t="b">
+        <v>1</v>
+      </c>
       <c r="G346" t="s">
         <v>166</v>
       </c>
-      <c r="H346" s="16"/>
-    </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A347" s="16">
+    </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A347">
         <v>2017</v>
       </c>
-      <c r="B347" s="17" t="s">
+      <c r="B347" t="s">
         <v>164</v>
       </c>
-      <c r="C347" s="16" t="s">
+      <c r="C347" t="s">
         <v>165</v>
       </c>
-      <c r="D347" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E347" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F347" s="16"/>
+      <c r="D347" t="s">
+        <v>37</v>
+      </c>
+      <c r="E347" t="b">
+        <v>1</v>
+      </c>
       <c r="G347" t="s">
         <v>166</v>
       </c>
-      <c r="H347" s="16"/>
-    </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A348" s="16">
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A348">
         <v>2018</v>
       </c>
-      <c r="B348" s="17" t="s">
+      <c r="B348" t="s">
         <v>164</v>
       </c>
-      <c r="C348" s="16" t="s">
+      <c r="C348" t="s">
         <v>167</v>
       </c>
-      <c r="D348" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E348" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F348" s="16"/>
+      <c r="D348" t="s">
+        <v>34</v>
+      </c>
+      <c r="E348" t="b">
+        <v>1</v>
+      </c>
       <c r="G348" t="s">
         <v>168</v>
       </c>
-      <c r="H348" s="16"/>
-    </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A349" s="16">
+    </row>
+    <row r="349" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A349">
         <v>2019</v>
       </c>
-      <c r="B349" s="17" t="s">
+      <c r="B349" t="s">
         <v>164</v>
       </c>
-      <c r="C349" s="16" t="s">
+      <c r="C349" t="s">
         <v>169</v>
       </c>
-      <c r="D349" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E349" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F349" s="16"/>
+      <c r="D349" t="s">
+        <v>34</v>
+      </c>
+      <c r="E349" t="b">
+        <v>1</v>
+      </c>
       <c r="G349" t="s">
         <v>173</v>
       </c>
-      <c r="H349" s="16"/>
-    </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A350" s="16">
+    </row>
+    <row r="350" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A350">
         <v>2020</v>
       </c>
-      <c r="B350" s="17" t="s">
+      <c r="B350" t="s">
         <v>164</v>
       </c>
-      <c r="C350" s="16" t="s">
+      <c r="C350" t="s">
         <v>169</v>
       </c>
-      <c r="D350" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E350" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F350" s="16"/>
+      <c r="D350" t="s">
+        <v>34</v>
+      </c>
+      <c r="E350" t="b">
+        <v>1</v>
+      </c>
       <c r="G350" t="s">
         <v>173</v>
       </c>
-      <c r="H350" s="16"/>
-    </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A351" s="16">
+    </row>
+    <row r="351" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A351">
         <v>2021</v>
       </c>
-      <c r="B351" s="17" t="s">
+      <c r="B351" t="s">
         <v>164</v>
       </c>
-      <c r="C351" s="16" t="s">
+      <c r="C351" t="s">
         <v>169</v>
       </c>
-      <c r="D351" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E351" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F351" s="16"/>
+      <c r="D351" t="s">
+        <v>34</v>
+      </c>
+      <c r="E351" t="b">
+        <v>1</v>
+      </c>
       <c r="G351" t="s">
         <v>173</v>
       </c>
-      <c r="H351" s="16"/>
-    </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A352" s="16">
+    </row>
+    <row r="352" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A352">
         <v>2022</v>
       </c>
-      <c r="B352" s="17" t="s">
+      <c r="B352" t="s">
         <v>164</v>
       </c>
-      <c r="C352" s="16" t="s">
+      <c r="C352" t="s">
         <v>169</v>
       </c>
-      <c r="D352" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E352" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F352" s="16"/>
+      <c r="D352" t="s">
+        <v>34</v>
+      </c>
+      <c r="E352" t="b">
+        <v>1</v>
+      </c>
       <c r="G352" t="s">
         <v>173</v>
       </c>
-      <c r="H352" s="16"/>
-    </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A353" s="16">
+    </row>
+    <row r="353" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A353">
         <v>2023</v>
       </c>
-      <c r="B353" s="17" t="s">
+      <c r="B353" t="s">
         <v>164</v>
       </c>
-      <c r="C353" s="16" t="s">
+      <c r="C353" t="s">
         <v>169</v>
       </c>
-      <c r="D353" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E353" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F353" s="16"/>
+      <c r="D353" t="s">
+        <v>34</v>
+      </c>
+      <c r="E353" t="b">
+        <v>1</v>
+      </c>
       <c r="G353" t="s">
         <v>173</v>
       </c>
-      <c r="H353" s="16"/>
+    </row>
+    <row r="354" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A354">
+        <v>2018</v>
+      </c>
+      <c r="B354" t="s">
+        <v>174</v>
+      </c>
+      <c r="C354" t="s">
+        <v>181</v>
+      </c>
+      <c r="D354" t="s">
+        <v>34</v>
+      </c>
+      <c r="E354" t="b">
+        <v>1</v>
+      </c>
+      <c r="G354" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="355" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A355">
+        <v>2019</v>
+      </c>
+      <c r="B355" t="s">
+        <v>174</v>
+      </c>
+      <c r="C355" t="s">
+        <v>185</v>
+      </c>
+      <c r="D355" t="s">
+        <v>34</v>
+      </c>
+      <c r="E355" t="b">
+        <v>1</v>
+      </c>
+      <c r="G355" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="356" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A356">
+        <v>2020</v>
+      </c>
+      <c r="B356" t="s">
+        <v>174</v>
+      </c>
+      <c r="C356" t="s">
+        <v>185</v>
+      </c>
+      <c r="D356" t="s">
+        <v>34</v>
+      </c>
+      <c r="E356" t="b">
+        <v>1</v>
+      </c>
+      <c r="G356" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="357" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A357">
+        <v>2021</v>
+      </c>
+      <c r="B357" t="s">
+        <v>174</v>
+      </c>
+      <c r="C357" t="s">
+        <v>185</v>
+      </c>
+      <c r="D357" t="s">
+        <v>34</v>
+      </c>
+      <c r="E357" t="b">
+        <v>1</v>
+      </c>
+      <c r="G357" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A358">
+        <v>2022</v>
+      </c>
+      <c r="B358" t="s">
+        <v>174</v>
+      </c>
+      <c r="C358" t="s">
+        <v>185</v>
+      </c>
+      <c r="D358" t="s">
+        <v>34</v>
+      </c>
+      <c r="E358" t="b">
+        <v>1</v>
+      </c>
+      <c r="G358" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A359">
+        <v>2023</v>
+      </c>
+      <c r="B359" t="s">
+        <v>174</v>
+      </c>
+      <c r="C359" t="s">
+        <v>185</v>
+      </c>
+      <c r="D359" t="s">
+        <v>34</v>
+      </c>
+      <c r="E359" t="b">
+        <v>1</v>
+      </c>
+      <c r="G359" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="360" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A360">
+        <v>2016</v>
+      </c>
+      <c r="B360" t="s">
+        <v>175</v>
+      </c>
+      <c r="C360" t="s">
+        <v>178</v>
+      </c>
+      <c r="D360" t="s">
+        <v>37</v>
+      </c>
+      <c r="E360" t="b">
+        <v>1</v>
+      </c>
+      <c r="G360" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="361" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A361">
+        <v>2017</v>
+      </c>
+      <c r="B361" t="s">
+        <v>175</v>
+      </c>
+      <c r="C361" t="s">
+        <v>178</v>
+      </c>
+      <c r="D361" t="s">
+        <v>37</v>
+      </c>
+      <c r="E361" t="b">
+        <v>1</v>
+      </c>
+      <c r="G361" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="362" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A362">
+        <v>2018</v>
+      </c>
+      <c r="B362" t="s">
+        <v>175</v>
+      </c>
+      <c r="C362" t="s">
+        <v>182</v>
+      </c>
+      <c r="D362" t="s">
+        <v>34</v>
+      </c>
+      <c r="E362" t="b">
+        <v>1</v>
+      </c>
+      <c r="G362" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="363" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A363">
+        <v>2019</v>
+      </c>
+      <c r="B363" t="s">
+        <v>175</v>
+      </c>
+      <c r="C363" t="s">
+        <v>186</v>
+      </c>
+      <c r="D363" t="s">
+        <v>34</v>
+      </c>
+      <c r="E363" t="b">
+        <v>1</v>
+      </c>
+      <c r="G363" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="364" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A364">
+        <v>2020</v>
+      </c>
+      <c r="B364" t="s">
+        <v>175</v>
+      </c>
+      <c r="C364" t="s">
+        <v>186</v>
+      </c>
+      <c r="D364" t="s">
+        <v>34</v>
+      </c>
+      <c r="E364" t="b">
+        <v>1</v>
+      </c>
+      <c r="G364" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="365" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A365">
+        <v>2021</v>
+      </c>
+      <c r="B365" t="s">
+        <v>175</v>
+      </c>
+      <c r="C365" t="s">
+        <v>186</v>
+      </c>
+      <c r="D365" t="s">
+        <v>34</v>
+      </c>
+      <c r="E365" t="b">
+        <v>1</v>
+      </c>
+      <c r="G365" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="366" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A366">
+        <v>2022</v>
+      </c>
+      <c r="B366" t="s">
+        <v>175</v>
+      </c>
+      <c r="C366" t="s">
+        <v>186</v>
+      </c>
+      <c r="D366" t="s">
+        <v>34</v>
+      </c>
+      <c r="E366" t="b">
+        <v>1</v>
+      </c>
+      <c r="G366" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="367" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A367">
+        <v>2023</v>
+      </c>
+      <c r="B367" t="s">
+        <v>175</v>
+      </c>
+      <c r="C367" t="s">
+        <v>186</v>
+      </c>
+      <c r="D367" t="s">
+        <v>34</v>
+      </c>
+      <c r="E367" t="b">
+        <v>1</v>
+      </c>
+      <c r="G367" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="368" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A368">
+        <v>2016</v>
+      </c>
+      <c r="B368" t="s">
+        <v>176</v>
+      </c>
+      <c r="C368" t="s">
+        <v>179</v>
+      </c>
+      <c r="D368" t="s">
+        <v>37</v>
+      </c>
+      <c r="E368" t="b">
+        <v>1</v>
+      </c>
+      <c r="G368" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="369" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A369">
+        <v>2017</v>
+      </c>
+      <c r="B369" t="s">
+        <v>176</v>
+      </c>
+      <c r="C369" t="s">
+        <v>179</v>
+      </c>
+      <c r="D369" t="s">
+        <v>37</v>
+      </c>
+      <c r="E369" t="b">
+        <v>1</v>
+      </c>
+      <c r="G369" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="370" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A370">
+        <v>2018</v>
+      </c>
+      <c r="B370" t="s">
+        <v>176</v>
+      </c>
+      <c r="C370" t="s">
+        <v>183</v>
+      </c>
+      <c r="D370" t="s">
+        <v>34</v>
+      </c>
+      <c r="E370" t="b">
+        <v>1</v>
+      </c>
+      <c r="G370" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A371">
+        <v>2019</v>
+      </c>
+      <c r="B371" t="s">
+        <v>176</v>
+      </c>
+      <c r="C371" t="s">
+        <v>187</v>
+      </c>
+      <c r="D371" t="s">
+        <v>34</v>
+      </c>
+      <c r="E371" t="b">
+        <v>1</v>
+      </c>
+      <c r="G371" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="372" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A372">
+        <v>2020</v>
+      </c>
+      <c r="B372" t="s">
+        <v>176</v>
+      </c>
+      <c r="C372" t="s">
+        <v>187</v>
+      </c>
+      <c r="D372" t="s">
+        <v>34</v>
+      </c>
+      <c r="E372" t="b">
+        <v>1</v>
+      </c>
+      <c r="G372" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A373">
+        <v>2021</v>
+      </c>
+      <c r="B373" t="s">
+        <v>176</v>
+      </c>
+      <c r="C373" t="s">
+        <v>187</v>
+      </c>
+      <c r="D373" t="s">
+        <v>34</v>
+      </c>
+      <c r="E373" t="b">
+        <v>1</v>
+      </c>
+      <c r="G373" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="374" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A374">
+        <v>2022</v>
+      </c>
+      <c r="B374" t="s">
+        <v>176</v>
+      </c>
+      <c r="C374" t="s">
+        <v>187</v>
+      </c>
+      <c r="D374" t="s">
+        <v>34</v>
+      </c>
+      <c r="E374" t="b">
+        <v>1</v>
+      </c>
+      <c r="G374" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="375" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A375">
+        <v>2023</v>
+      </c>
+      <c r="B375" t="s">
+        <v>176</v>
+      </c>
+      <c r="C375" t="s">
+        <v>187</v>
+      </c>
+      <c r="D375" t="s">
+        <v>34</v>
+      </c>
+      <c r="E375" t="b">
+        <v>1</v>
+      </c>
+      <c r="G375" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="376" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A376">
+        <v>2016</v>
+      </c>
+      <c r="B376" t="s">
+        <v>177</v>
+      </c>
+      <c r="C376" t="s">
+        <v>180</v>
+      </c>
+      <c r="D376" t="s">
+        <v>37</v>
+      </c>
+      <c r="E376" t="b">
+        <v>1</v>
+      </c>
+      <c r="G376" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="377" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A377">
+        <v>2017</v>
+      </c>
+      <c r="B377" t="s">
+        <v>177</v>
+      </c>
+      <c r="C377" t="s">
+        <v>180</v>
+      </c>
+      <c r="D377" t="s">
+        <v>37</v>
+      </c>
+      <c r="E377" t="b">
+        <v>1</v>
+      </c>
+      <c r="G377" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="378" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A378">
+        <v>2018</v>
+      </c>
+      <c r="B378" t="s">
+        <v>177</v>
+      </c>
+      <c r="C378" t="s">
+        <v>184</v>
+      </c>
+      <c r="D378" t="s">
+        <v>34</v>
+      </c>
+      <c r="E378" t="b">
+        <v>1</v>
+      </c>
+      <c r="G378" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="379" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A379">
+        <v>2019</v>
+      </c>
+      <c r="B379" t="s">
+        <v>177</v>
+      </c>
+      <c r="C379" t="s">
+        <v>188</v>
+      </c>
+      <c r="D379" t="s">
+        <v>34</v>
+      </c>
+      <c r="E379" t="b">
+        <v>1</v>
+      </c>
+      <c r="G379" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="380" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A380">
+        <v>2020</v>
+      </c>
+      <c r="B380" t="s">
+        <v>177</v>
+      </c>
+      <c r="C380" t="s">
+        <v>188</v>
+      </c>
+      <c r="D380" t="s">
+        <v>34</v>
+      </c>
+      <c r="E380" t="b">
+        <v>1</v>
+      </c>
+      <c r="G380" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="381" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A381">
+        <v>2021</v>
+      </c>
+      <c r="B381" t="s">
+        <v>177</v>
+      </c>
+      <c r="C381" t="s">
+        <v>188</v>
+      </c>
+      <c r="D381" t="s">
+        <v>34</v>
+      </c>
+      <c r="E381" t="b">
+        <v>1</v>
+      </c>
+      <c r="G381" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="382" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A382">
+        <v>2022</v>
+      </c>
+      <c r="B382" t="s">
+        <v>177</v>
+      </c>
+      <c r="C382" t="s">
+        <v>188</v>
+      </c>
+      <c r="D382" t="s">
+        <v>34</v>
+      </c>
+      <c r="E382" t="b">
+        <v>1</v>
+      </c>
+      <c r="G382" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A383">
+        <v>2023</v>
+      </c>
+      <c r="B383" t="s">
+        <v>177</v>
+      </c>
+      <c r="C383" t="s">
+        <v>188</v>
+      </c>
+      <c r="D383" t="s">
+        <v>34</v>
+      </c>
+      <c r="E383" t="b">
+        <v>1</v>
+      </c>
+      <c r="G383" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A384">
+        <v>2023</v>
+      </c>
+      <c r="B384" t="s">
+        <v>200</v>
+      </c>
+      <c r="C384" t="s">
+        <v>200</v>
+      </c>
+      <c r="D384" t="s">
+        <v>202</v>
+      </c>
+      <c r="E384" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="385" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A385">
+        <v>2023</v>
+      </c>
+      <c r="B385" t="s">
+        <v>201</v>
+      </c>
+      <c r="C385" t="s">
+        <v>201</v>
+      </c>
+      <c r="D385" t="s">
+        <v>202</v>
+      </c>
+      <c r="E385" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A386">
+        <v>2019</v>
+      </c>
+      <c r="B386" t="s">
+        <v>205</v>
+      </c>
+      <c r="C386" t="s">
+        <v>205</v>
+      </c>
+      <c r="D386" t="s">
+        <v>34</v>
+      </c>
+      <c r="E386" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A387">
+        <v>2020</v>
+      </c>
+      <c r="B387" t="s">
+        <v>205</v>
+      </c>
+      <c r="C387" t="s">
+        <v>205</v>
+      </c>
+      <c r="D387" t="s">
+        <v>34</v>
+      </c>
+      <c r="E387" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A388">
+        <v>2021</v>
+      </c>
+      <c r="B388" t="s">
+        <v>205</v>
+      </c>
+      <c r="C388" t="s">
+        <v>205</v>
+      </c>
+      <c r="D388" t="s">
+        <v>34</v>
+      </c>
+      <c r="E388" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A389">
+        <v>2022</v>
+      </c>
+      <c r="B389" t="s">
+        <v>205</v>
+      </c>
+      <c r="C389" t="s">
+        <v>205</v>
+      </c>
+      <c r="D389" t="s">
+        <v>34</v>
+      </c>
+      <c r="E389" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="390" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A390">
+        <v>2023</v>
+      </c>
+      <c r="B390" t="s">
+        <v>205</v>
+      </c>
+      <c r="C390" t="s">
+        <v>205</v>
+      </c>
+      <c r="D390" t="s">
+        <v>34</v>
+      </c>
+      <c r="E390" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="391" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A391">
+        <v>2019</v>
+      </c>
+      <c r="B391" t="s">
+        <v>206</v>
+      </c>
+      <c r="C391" t="s">
+        <v>206</v>
+      </c>
+      <c r="D391" t="s">
+        <v>34</v>
+      </c>
+      <c r="E391" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="392" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A392">
+        <v>2020</v>
+      </c>
+      <c r="B392" t="s">
+        <v>206</v>
+      </c>
+      <c r="C392" t="s">
+        <v>206</v>
+      </c>
+      <c r="D392" t="s">
+        <v>34</v>
+      </c>
+      <c r="E392" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="393" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A393">
+        <v>2021</v>
+      </c>
+      <c r="B393" t="s">
+        <v>206</v>
+      </c>
+      <c r="C393" t="s">
+        <v>206</v>
+      </c>
+      <c r="D393" t="s">
+        <v>34</v>
+      </c>
+      <c r="E393" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="394" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A394">
+        <v>2022</v>
+      </c>
+      <c r="B394" t="s">
+        <v>206</v>
+      </c>
+      <c r="C394" t="s">
+        <v>206</v>
+      </c>
+      <c r="D394" t="s">
+        <v>34</v>
+      </c>
+      <c r="E394" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="395" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A395">
+        <v>2023</v>
+      </c>
+      <c r="B395" t="s">
+        <v>206</v>
+      </c>
+      <c r="C395" t="s">
+        <v>206</v>
+      </c>
+      <c r="D395" t="s">
+        <v>34</v>
+      </c>
+      <c r="E395" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="396" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A396">
+        <v>2019</v>
+      </c>
+      <c r="B396" t="s">
+        <v>207</v>
+      </c>
+      <c r="C396" t="s">
+        <v>207</v>
+      </c>
+      <c r="D396" t="s">
+        <v>34</v>
+      </c>
+      <c r="E396" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="397" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A397">
+        <v>2020</v>
+      </c>
+      <c r="B397" t="s">
+        <v>207</v>
+      </c>
+      <c r="C397" t="s">
+        <v>207</v>
+      </c>
+      <c r="D397" t="s">
+        <v>34</v>
+      </c>
+      <c r="E397" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="398" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A398">
+        <v>2021</v>
+      </c>
+      <c r="B398" t="s">
+        <v>207</v>
+      </c>
+      <c r="C398" t="s">
+        <v>207</v>
+      </c>
+      <c r="D398" t="s">
+        <v>34</v>
+      </c>
+      <c r="E398" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="399" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A399">
+        <v>2022</v>
+      </c>
+      <c r="B399" t="s">
+        <v>207</v>
+      </c>
+      <c r="C399" t="s">
+        <v>207</v>
+      </c>
+      <c r="D399" t="s">
+        <v>34</v>
+      </c>
+      <c r="E399" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="400" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A400">
+        <v>2023</v>
+      </c>
+      <c r="B400" t="s">
+        <v>207</v>
+      </c>
+      <c r="C400" t="s">
+        <v>207</v>
+      </c>
+      <c r="D400" t="s">
+        <v>34</v>
+      </c>
+      <c r="E400" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="401" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A401">
+        <v>2018</v>
+      </c>
+      <c r="B401" t="s">
+        <v>208</v>
+      </c>
+      <c r="C401" t="s">
+        <v>203</v>
+      </c>
+      <c r="D401" t="s">
+        <v>34</v>
+      </c>
+      <c r="E401" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="402" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A402">
+        <v>2018</v>
+      </c>
+      <c r="B402" t="s">
+        <v>209</v>
+      </c>
+      <c r="C402" t="s">
+        <v>204</v>
+      </c>
+      <c r="D402" t="s">
+        <v>34</v>
+      </c>
+      <c r="E402" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="403" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A403">
+        <v>2008</v>
+      </c>
+      <c r="B403" t="s">
+        <v>205</v>
+      </c>
+      <c r="C403" t="s">
+        <v>210</v>
+      </c>
+      <c r="D403" t="s">
+        <v>37</v>
+      </c>
+      <c r="E403" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="404" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A404">
+        <v>2009</v>
+      </c>
+      <c r="B404" t="s">
+        <v>205</v>
+      </c>
+      <c r="C404" t="s">
+        <v>210</v>
+      </c>
+      <c r="D404" t="s">
+        <v>37</v>
+      </c>
+      <c r="E404" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="405" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A405">
+        <v>2010</v>
+      </c>
+      <c r="B405" t="s">
+        <v>205</v>
+      </c>
+      <c r="C405" t="s">
+        <v>210</v>
+      </c>
+      <c r="D405" t="s">
+        <v>37</v>
+      </c>
+      <c r="E405" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="406" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A406">
+        <v>2011</v>
+      </c>
+      <c r="B406" t="s">
+        <v>205</v>
+      </c>
+      <c r="C406" t="s">
+        <v>210</v>
+      </c>
+      <c r="D406" t="s">
+        <v>37</v>
+      </c>
+      <c r="E406" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="407" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A407">
+        <v>2012</v>
+      </c>
+      <c r="B407" t="s">
+        <v>205</v>
+      </c>
+      <c r="C407" t="s">
+        <v>210</v>
+      </c>
+      <c r="D407" t="s">
+        <v>37</v>
+      </c>
+      <c r="E407" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="408" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A408">
+        <v>2013</v>
+      </c>
+      <c r="B408" t="s">
+        <v>205</v>
+      </c>
+      <c r="C408" t="s">
+        <v>213</v>
+      </c>
+      <c r="D408" t="s">
+        <v>37</v>
+      </c>
+      <c r="E408" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="409" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A409">
+        <v>2014</v>
+      </c>
+      <c r="B409" t="s">
+        <v>205</v>
+      </c>
+      <c r="C409" t="s">
+        <v>210</v>
+      </c>
+      <c r="D409" t="s">
+        <v>37</v>
+      </c>
+      <c r="E409" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="410" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A410">
+        <v>2015</v>
+      </c>
+      <c r="B410" t="s">
+        <v>205</v>
+      </c>
+      <c r="C410" t="s">
+        <v>210</v>
+      </c>
+      <c r="D410" t="s">
+        <v>37</v>
+      </c>
+      <c r="E410" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="411" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A411">
+        <v>2008</v>
+      </c>
+      <c r="B411" t="s">
+        <v>207</v>
+      </c>
+      <c r="C411" t="s">
+        <v>212</v>
+      </c>
+      <c r="D411" t="s">
+        <v>37</v>
+      </c>
+      <c r="E411" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="412" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A412">
+        <v>2009</v>
+      </c>
+      <c r="B412" t="s">
+        <v>207</v>
+      </c>
+      <c r="C412" t="s">
+        <v>212</v>
+      </c>
+      <c r="D412" t="s">
+        <v>37</v>
+      </c>
+      <c r="E412" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="413" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A413">
+        <v>2010</v>
+      </c>
+      <c r="B413" t="s">
+        <v>207</v>
+      </c>
+      <c r="C413" t="s">
+        <v>212</v>
+      </c>
+      <c r="D413" t="s">
+        <v>37</v>
+      </c>
+      <c r="E413" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="414" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A414">
+        <v>2011</v>
+      </c>
+      <c r="B414" t="s">
+        <v>207</v>
+      </c>
+      <c r="C414" t="s">
+        <v>212</v>
+      </c>
+      <c r="D414" t="s">
+        <v>37</v>
+      </c>
+      <c r="E414" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="415" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A415">
+        <v>2012</v>
+      </c>
+      <c r="B415" t="s">
+        <v>207</v>
+      </c>
+      <c r="C415" t="s">
+        <v>212</v>
+      </c>
+      <c r="D415" t="s">
+        <v>37</v>
+      </c>
+      <c r="E415" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="416" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A416">
+        <v>2013</v>
+      </c>
+      <c r="B416" t="s">
+        <v>207</v>
+      </c>
+      <c r="C416" t="s">
+        <v>215</v>
+      </c>
+      <c r="D416" t="s">
+        <v>37</v>
+      </c>
+      <c r="E416" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="417" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A417">
+        <v>2014</v>
+      </c>
+      <c r="B417" t="s">
+        <v>207</v>
+      </c>
+      <c r="C417" t="s">
+        <v>212</v>
+      </c>
+      <c r="D417" t="s">
+        <v>37</v>
+      </c>
+      <c r="E417" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="418" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A418">
+        <v>2015</v>
+      </c>
+      <c r="B418" t="s">
+        <v>207</v>
+      </c>
+      <c r="C418" t="s">
+        <v>212</v>
+      </c>
+      <c r="D418" t="s">
+        <v>37</v>
+      </c>
+      <c r="E418" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="419" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A419">
+        <v>2008</v>
+      </c>
+      <c r="B419" t="s">
+        <v>206</v>
+      </c>
+      <c r="C419" t="s">
+        <v>211</v>
+      </c>
+      <c r="D419" t="s">
+        <v>37</v>
+      </c>
+      <c r="E419" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="420" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A420">
+        <v>2009</v>
+      </c>
+      <c r="B420" t="s">
+        <v>206</v>
+      </c>
+      <c r="C420" t="s">
+        <v>211</v>
+      </c>
+      <c r="D420" t="s">
+        <v>37</v>
+      </c>
+      <c r="E420" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="421" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A421">
+        <v>2010</v>
+      </c>
+      <c r="B421" t="s">
+        <v>206</v>
+      </c>
+      <c r="C421" t="s">
+        <v>211</v>
+      </c>
+      <c r="D421" t="s">
+        <v>37</v>
+      </c>
+      <c r="E421" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="422" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A422">
+        <v>2011</v>
+      </c>
+      <c r="B422" t="s">
+        <v>206</v>
+      </c>
+      <c r="C422" t="s">
+        <v>211</v>
+      </c>
+      <c r="D422" t="s">
+        <v>37</v>
+      </c>
+      <c r="E422" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="423" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A423">
+        <v>2012</v>
+      </c>
+      <c r="B423" t="s">
+        <v>206</v>
+      </c>
+      <c r="C423" t="s">
+        <v>211</v>
+      </c>
+      <c r="D423" t="s">
+        <v>37</v>
+      </c>
+      <c r="E423" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="424" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A424">
+        <v>2013</v>
+      </c>
+      <c r="B424" t="s">
+        <v>206</v>
+      </c>
+      <c r="C424" t="s">
+        <v>214</v>
+      </c>
+      <c r="D424" t="s">
+        <v>37</v>
+      </c>
+      <c r="E424" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="425" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A425">
+        <v>2014</v>
+      </c>
+      <c r="B425" t="s">
+        <v>206</v>
+      </c>
+      <c r="C425" t="s">
+        <v>211</v>
+      </c>
+      <c r="D425" t="s">
+        <v>37</v>
+      </c>
+      <c r="E425" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="426" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A426">
+        <v>2015</v>
+      </c>
+      <c r="B426" t="s">
+        <v>206</v>
+      </c>
+      <c r="C426" t="s">
+        <v>211</v>
+      </c>
+      <c r="D426" t="s">
+        <v>37</v>
+      </c>
+      <c r="E426" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="427" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A427">
+        <v>2016</v>
+      </c>
+      <c r="B427" t="s">
+        <v>218</v>
+      </c>
+      <c r="C427" t="s">
+        <v>216</v>
+      </c>
+      <c r="D427" t="s">
+        <v>37</v>
+      </c>
+      <c r="E427" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A428">
+        <v>2017</v>
+      </c>
+      <c r="B428" t="s">
+        <v>218</v>
+      </c>
+      <c r="C428" t="s">
+        <v>216</v>
+      </c>
+      <c r="D428" t="s">
+        <v>37</v>
+      </c>
+      <c r="E428" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="429" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A429">
+        <v>2018</v>
+      </c>
+      <c r="B429" t="s">
+        <v>218</v>
+      </c>
+      <c r="C429" t="s">
+        <v>217</v>
+      </c>
+      <c r="D429" t="s">
+        <v>34</v>
+      </c>
+      <c r="E429" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="430" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A430">
+        <v>2019</v>
+      </c>
+      <c r="B430" t="s">
+        <v>218</v>
+      </c>
+      <c r="C430" t="s">
+        <v>217</v>
+      </c>
+      <c r="D430" t="s">
+        <v>34</v>
+      </c>
+      <c r="E430" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="431" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A431">
+        <v>2020</v>
+      </c>
+      <c r="B431" t="s">
+        <v>218</v>
+      </c>
+      <c r="C431" t="s">
+        <v>217</v>
+      </c>
+      <c r="D431" t="s">
+        <v>34</v>
+      </c>
+      <c r="E431" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A432">
+        <v>2021</v>
+      </c>
+      <c r="B432" t="s">
+        <v>218</v>
+      </c>
+      <c r="C432" t="s">
+        <v>217</v>
+      </c>
+      <c r="D432" t="s">
+        <v>34</v>
+      </c>
+      <c r="E432" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="433" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A433">
+        <v>2022</v>
+      </c>
+      <c r="B433" t="s">
+        <v>218</v>
+      </c>
+      <c r="C433" t="s">
+        <v>217</v>
+      </c>
+      <c r="D433" t="s">
+        <v>34</v>
+      </c>
+      <c r="E433" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="434" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A434">
+        <v>2023</v>
+      </c>
+      <c r="B434" t="s">
+        <v>218</v>
+      </c>
+      <c r="C434" t="s">
+        <v>217</v>
+      </c>
+      <c r="D434" t="s">
+        <v>34</v>
+      </c>
+      <c r="E434" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="435" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A435">
+        <v>2014</v>
+      </c>
+      <c r="B435" t="s">
+        <v>220</v>
+      </c>
+      <c r="C435" t="s">
+        <v>219</v>
+      </c>
+      <c r="D435" t="s">
+        <v>37</v>
+      </c>
+      <c r="E435" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="436" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A436">
+        <v>2015</v>
+      </c>
+      <c r="B436" t="s">
+        <v>220</v>
+      </c>
+      <c r="C436" t="s">
+        <v>219</v>
+      </c>
+      <c r="D436" t="s">
+        <v>37</v>
+      </c>
+      <c r="E436" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="437" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A437">
+        <v>2016</v>
+      </c>
+      <c r="B437" t="s">
+        <v>220</v>
+      </c>
+      <c r="C437" t="s">
+        <v>219</v>
+      </c>
+      <c r="D437" t="s">
+        <v>37</v>
+      </c>
+      <c r="E437" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="438" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A438">
+        <v>2017</v>
+      </c>
+      <c r="B438" t="s">
+        <v>220</v>
+      </c>
+      <c r="C438" t="s">
+        <v>219</v>
+      </c>
+      <c r="D438" t="s">
+        <v>37</v>
+      </c>
+      <c r="E438" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="439" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A439">
+        <v>2018</v>
+      </c>
+      <c r="B439" t="s">
+        <v>220</v>
+      </c>
+      <c r="C439" t="s">
+        <v>220</v>
+      </c>
+      <c r="D439" t="s">
+        <v>34</v>
+      </c>
+      <c r="E439" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="440" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A440">
+        <v>2019</v>
+      </c>
+      <c r="B440" t="s">
+        <v>220</v>
+      </c>
+      <c r="C440" t="s">
+        <v>220</v>
+      </c>
+      <c r="D440" t="s">
+        <v>34</v>
+      </c>
+      <c r="E440" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="441" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A441">
+        <v>2020</v>
+      </c>
+      <c r="B441" t="s">
+        <v>220</v>
+      </c>
+      <c r="C441" t="s">
+        <v>220</v>
+      </c>
+      <c r="D441" t="s">
+        <v>34</v>
+      </c>
+      <c r="E441" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="442" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A442">
+        <v>2021</v>
+      </c>
+      <c r="B442" t="s">
+        <v>220</v>
+      </c>
+      <c r="C442" t="s">
+        <v>220</v>
+      </c>
+      <c r="D442" t="s">
+        <v>34</v>
+      </c>
+      <c r="E442" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="443" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A443">
+        <v>2022</v>
+      </c>
+      <c r="B443" t="s">
+        <v>220</v>
+      </c>
+      <c r="C443" t="s">
+        <v>220</v>
+      </c>
+      <c r="D443" t="s">
+        <v>34</v>
+      </c>
+      <c r="E443" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="444" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A444">
+        <v>2023</v>
+      </c>
+      <c r="B444" t="s">
+        <v>220</v>
+      </c>
+      <c r="C444" t="s">
+        <v>220</v>
+      </c>
+      <c r="D444" t="s">
+        <v>34</v>
+      </c>
+      <c r="E444" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="445" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A445">
+        <v>2008</v>
+      </c>
+      <c r="B445" t="s">
+        <v>228</v>
+      </c>
+      <c r="C445" t="s">
+        <v>221</v>
+      </c>
+      <c r="D445" t="s">
+        <v>37</v>
+      </c>
+      <c r="E445" t="b">
+        <v>1</v>
+      </c>
+      <c r="G445" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="446" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A446">
+        <v>2009</v>
+      </c>
+      <c r="B446" t="s">
+        <v>228</v>
+      </c>
+      <c r="C446" t="s">
+        <v>221</v>
+      </c>
+      <c r="D446" t="s">
+        <v>37</v>
+      </c>
+      <c r="E446" t="b">
+        <v>1</v>
+      </c>
+      <c r="G446" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="447" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A447">
+        <v>2010</v>
+      </c>
+      <c r="B447" t="s">
+        <v>228</v>
+      </c>
+      <c r="C447" t="s">
+        <v>221</v>
+      </c>
+      <c r="D447" t="s">
+        <v>37</v>
+      </c>
+      <c r="E447" t="b">
+        <v>1</v>
+      </c>
+      <c r="G447" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="448" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A448">
+        <v>2011</v>
+      </c>
+      <c r="B448" t="s">
+        <v>228</v>
+      </c>
+      <c r="C448" t="s">
+        <v>221</v>
+      </c>
+      <c r="D448" t="s">
+        <v>37</v>
+      </c>
+      <c r="E448" t="b">
+        <v>1</v>
+      </c>
+      <c r="G448" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="449" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A449">
+        <v>2012</v>
+      </c>
+      <c r="B449" t="s">
+        <v>228</v>
+      </c>
+      <c r="C449" t="s">
+        <v>223</v>
+      </c>
+      <c r="D449" t="s">
+        <v>37</v>
+      </c>
+      <c r="E449" t="b">
+        <v>1</v>
+      </c>
+      <c r="G449" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="450" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A450">
+        <v>2013</v>
+      </c>
+      <c r="B450" t="s">
+        <v>228</v>
+      </c>
+      <c r="C450" t="s">
+        <v>223</v>
+      </c>
+      <c r="D450" t="s">
+        <v>37</v>
+      </c>
+      <c r="E450" t="b">
+        <v>1</v>
+      </c>
+      <c r="G450" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="451" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A451">
+        <v>2014</v>
+      </c>
+      <c r="B451" t="s">
+        <v>228</v>
+      </c>
+      <c r="C451" t="s">
+        <v>223</v>
+      </c>
+      <c r="D451" t="s">
+        <v>37</v>
+      </c>
+      <c r="E451" t="b">
+        <v>1</v>
+      </c>
+      <c r="G451" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="452" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A452">
+        <v>2015</v>
+      </c>
+      <c r="B452" t="s">
+        <v>228</v>
+      </c>
+      <c r="C452" t="s">
+        <v>223</v>
+      </c>
+      <c r="D452" t="s">
+        <v>37</v>
+      </c>
+      <c r="E452" t="b">
+        <v>1</v>
+      </c>
+      <c r="G452" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="453" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A453">
+        <v>2016</v>
+      </c>
+      <c r="B453" t="s">
+        <v>228</v>
+      </c>
+      <c r="C453" t="s">
+        <v>223</v>
+      </c>
+      <c r="D453" t="s">
+        <v>37</v>
+      </c>
+      <c r="E453" t="b">
+        <v>1</v>
+      </c>
+      <c r="G453" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="454" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A454">
+        <v>2017</v>
+      </c>
+      <c r="B454" t="s">
+        <v>228</v>
+      </c>
+      <c r="C454" t="s">
+        <v>223</v>
+      </c>
+      <c r="D454" t="s">
+        <v>37</v>
+      </c>
+      <c r="E454" t="b">
+        <v>1</v>
+      </c>
+      <c r="G454" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="455" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A455">
+        <v>2018</v>
+      </c>
+      <c r="B455" t="s">
+        <v>228</v>
+      </c>
+      <c r="C455" t="s">
+        <v>225</v>
+      </c>
+      <c r="D455" t="s">
+        <v>34</v>
+      </c>
+      <c r="E455" t="b">
+        <v>1</v>
+      </c>
+      <c r="G455" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="456" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A456">
+        <v>2019</v>
+      </c>
+      <c r="B456" t="s">
+        <v>228</v>
+      </c>
+      <c r="C456" t="s">
+        <v>225</v>
+      </c>
+      <c r="D456" t="s">
+        <v>34</v>
+      </c>
+      <c r="E456" t="b">
+        <v>1</v>
+      </c>
+      <c r="G456" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="457" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A457">
+        <v>2020</v>
+      </c>
+      <c r="B457" t="s">
+        <v>228</v>
+      </c>
+      <c r="C457" t="s">
+        <v>225</v>
+      </c>
+      <c r="D457" t="s">
+        <v>34</v>
+      </c>
+      <c r="E457" t="b">
+        <v>1</v>
+      </c>
+      <c r="G457" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="458" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A458">
+        <v>2021</v>
+      </c>
+      <c r="B458" t="s">
+        <v>228</v>
+      </c>
+      <c r="C458" t="s">
+        <v>225</v>
+      </c>
+      <c r="D458" t="s">
+        <v>34</v>
+      </c>
+      <c r="E458" t="b">
+        <v>1</v>
+      </c>
+      <c r="G458" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="459" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A459">
+        <v>2022</v>
+      </c>
+      <c r="B459" t="s">
+        <v>228</v>
+      </c>
+      <c r="C459" t="s">
+        <v>225</v>
+      </c>
+      <c r="D459" t="s">
+        <v>34</v>
+      </c>
+      <c r="E459" t="b">
+        <v>1</v>
+      </c>
+      <c r="G459" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="460" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A460">
+        <v>2023</v>
+      </c>
+      <c r="B460" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="C460" t="s">
+        <v>225</v>
+      </c>
+      <c r="D460" t="s">
+        <v>34</v>
+      </c>
+      <c r="E460" t="b">
+        <v>1</v>
+      </c>
+      <c r="G460" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="461" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A461">
+        <v>2016</v>
+      </c>
+      <c r="B461" t="s">
+        <v>227</v>
+      </c>
+      <c r="C461" t="s">
+        <v>224</v>
+      </c>
+      <c r="D461" t="s">
+        <v>37</v>
+      </c>
+      <c r="E461" t="b">
+        <v>1</v>
+      </c>
+      <c r="G461" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="462" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A462">
+        <v>2017</v>
+      </c>
+      <c r="B462" t="s">
+        <v>227</v>
+      </c>
+      <c r="C462" t="s">
+        <v>224</v>
+      </c>
+      <c r="D462" t="s">
+        <v>37</v>
+      </c>
+      <c r="E462" t="b">
+        <v>1</v>
+      </c>
+      <c r="G462" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="463" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A463">
+        <v>2018</v>
+      </c>
+      <c r="B463" t="s">
+        <v>227</v>
+      </c>
+      <c r="C463" t="s">
+        <v>226</v>
+      </c>
+      <c r="D463" t="s">
+        <v>34</v>
+      </c>
+      <c r="E463" t="b">
+        <v>1</v>
+      </c>
+      <c r="G463" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="464" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A464">
+        <v>2019</v>
+      </c>
+      <c r="B464" t="s">
+        <v>227</v>
+      </c>
+      <c r="C464" t="s">
+        <v>226</v>
+      </c>
+      <c r="D464" t="s">
+        <v>34</v>
+      </c>
+      <c r="E464" t="b">
+        <v>1</v>
+      </c>
+      <c r="G464" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="465" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A465">
+        <v>2020</v>
+      </c>
+      <c r="B465" t="s">
+        <v>227</v>
+      </c>
+      <c r="C465" t="s">
+        <v>226</v>
+      </c>
+      <c r="D465" t="s">
+        <v>34</v>
+      </c>
+      <c r="E465" t="b">
+        <v>1</v>
+      </c>
+      <c r="G465" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="466" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A466">
+        <v>2021</v>
+      </c>
+      <c r="B466" t="s">
+        <v>227</v>
+      </c>
+      <c r="C466" t="s">
+        <v>226</v>
+      </c>
+      <c r="D466" t="s">
+        <v>34</v>
+      </c>
+      <c r="E466" t="b">
+        <v>1</v>
+      </c>
+      <c r="G466" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="467" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A467">
+        <v>2022</v>
+      </c>
+      <c r="B467" t="s">
+        <v>227</v>
+      </c>
+      <c r="C467" t="s">
+        <v>226</v>
+      </c>
+      <c r="D467" t="s">
+        <v>34</v>
+      </c>
+      <c r="E467" t="b">
+        <v>1</v>
+      </c>
+      <c r="G467" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="468" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A468">
+        <v>2023</v>
+      </c>
+      <c r="B468" t="s">
+        <v>227</v>
+      </c>
+      <c r="C468" t="s">
+        <v>226</v>
+      </c>
+      <c r="D468" t="s">
+        <v>34</v>
+      </c>
+      <c r="E468" t="b">
+        <v>1</v>
+      </c>
+      <c r="G468" t="s">
+        <v>232</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10460,17 +13266,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d5cc9fc5-cf59-440a-a506-890d57680064">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B598B773ED9FC644B8B740EB3205C8DA" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6cfe95817d5870f6c066b2c32ab5fb2a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xmlns:ns3="d5cc9fc5-cf59-440a-a506-890d57680064" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a231614a4bf4996e6f4146316e2aaf8" ns2:_="" ns3:_="">
     <xsd:import namespace="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
@@ -10733,7 +13528,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -10742,24 +13537,18 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA6725D-5CB1-4E78-9F97-F79E79C18DA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d5cc9fc5-cf59-440a-a506-890d57680064"/>
-    <ds:schemaRef ds:uri="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d5cc9fc5-cf59-440a-a506-890d57680064">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B298AB6-2F6D-497E-AD9E-0F97ABEC8463}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10778,10 +13567,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3FAF407-B1B6-4FB8-B534-293B9E1D533A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA6725D-5CB1-4E78-9F97-F79E79C18DA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d5cc9fc5-cf59-440a-a506-890d57680064"/>
+    <ds:schemaRef ds:uri="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added AP Exam taken/passed
</commit_message>
<xml_diff>
--- a/Local Historic Crosswalk.xlsx
+++ b/Local Historic Crosswalk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasontheisen/Documents/Advance Illinois/Historic Report Card/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F81D6B3B-0887-0246-9B8F-C93A20194320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D43A490-C16F-CE42-B7A0-3CDA643084BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2208" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2432" uniqueCount="256">
   <si>
     <t>Year</t>
   </si>
@@ -1303,6 +1303,72 @@
   </si>
   <si>
     <t>COUNTY</t>
+  </si>
+  <si>
+    <t># of GRADE 10 STUDENTS TOOK ONE OR MORE AP EXAMS (SCHOOL)</t>
+  </si>
+  <si>
+    <t># of GRADE 10 STUDENTS PASSED ONE OR MORE AP EXAMS (SCHOOL)</t>
+  </si>
+  <si>
+    <t># of GRADE 11 STUDENTS TOOK ONE OR MORE AP EXAMS (SCHOOL)</t>
+  </si>
+  <si>
+    <t># of GRADE 11 STUDENTS PASSED ONE OR MORE AP EXAMS (SCHOOL)</t>
+  </si>
+  <si>
+    <t># of GRADE 12 STUDENTS TOOK ONE OR MORE AP EXAMS (SCHOOL)</t>
+  </si>
+  <si>
+    <t># of GRADE 12 STUDENTS PASSED ONE OR MORE AP EXAMS (SCHOOL)</t>
+  </si>
+  <si>
+    <t>Number of students who took one ore more AP Exams Grade 10</t>
+  </si>
+  <si>
+    <t>Number of students who passed one ore more AP Exams Grade 10</t>
+  </si>
+  <si>
+    <t>Number of students who took one ore more AP Exams Grade 11</t>
+  </si>
+  <si>
+    <t>Number of students who passed one ore more AP Exams Grade 11</t>
+  </si>
+  <si>
+    <t>Number of students who took one ore more AP Exams Grade 12</t>
+  </si>
+  <si>
+    <t>Number of students who passed one ore more AP Exams Grade 12</t>
+  </si>
+  <si>
+    <t>Number of students who took one ore more AP Exams Grade 9</t>
+  </si>
+  <si>
+    <t>Number of students who passed one ore more AP Exams Grade 9</t>
+  </si>
+  <si>
+    <t>Number of students who took one or more AP Exams Grade 9</t>
+  </si>
+  <si>
+    <t>Number of students who passed one or more AP Exams Grade 9</t>
+  </si>
+  <si>
+    <t>Number of students who passed one or more AP Exams Grade 10</t>
+  </si>
+  <si>
+    <t>Number of students who passed one or more AP Exams Grade 11</t>
+  </si>
+  <si>
+    <t>Number of students who took one or more AP Exams Grade 10</t>
+  </si>
+  <si>
+    <t>Number of students who took one or more AP Exams Grade 11</t>
+  </si>
+  <si>
+    <t>Number of students who took one or more AP Exams Grade 12</t>
+  </si>
+  <si>
+    <t>Number of students who passed one or more AP Exams Grade 12</t>
   </si>
 </sst>
 </file>
@@ -1476,7 +1542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1500,11 +1566,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="71">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1556,6 +1624,64 @@
           <color theme="4" tint="0.39997558519241921"/>
         </right>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2100,73 +2226,89 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}" name="Table1" displayName="Table1" ref="A1:BA17" totalsRowShown="0" dataDxfId="62">
-  <autoFilter ref="A1:BA17" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}" name="Table1" displayName="Table1" ref="A1:BI17" totalsRowShown="0" dataDxfId="70">
+  <autoFilter ref="A1:BI17" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O17">
     <sortCondition ref="A1:A17"/>
   </sortState>
-  <tableColumns count="53">
-    <tableColumn id="1" xr3:uid="{6DA6945B-9D7D-0142-A374-7C4A97BBBBAB}" name="Year" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{1617EDAF-51CD-413F-9022-F6E4C97C233F}" name="RCDTS" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{A67D85A4-5303-744E-B7CD-31ECBC6CE0A7}" name="Type" dataDxfId="59"/>
-    <tableColumn id="13" xr3:uid="{C8F50192-B0A1-D84D-96D9-819955E9CE26}" name="District Type" dataDxfId="58"/>
-    <tableColumn id="14" xr3:uid="{A7661728-A363-9840-8182-CBC0352B14C6}" name="School Type" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{94336B41-A312-184A-9F00-C5E1720E28AF}" name="School Name" dataDxfId="56"/>
-    <tableColumn id="5" xr3:uid="{7516DA0D-E868-1941-B0D3-80B0E523A018}" name="District Name" dataDxfId="55"/>
-    <tableColumn id="10" xr3:uid="{DCD59F4B-C55C-2846-9070-7F8CC6CA2F51}" name="City" dataDxfId="54"/>
-    <tableColumn id="11" xr3:uid="{AB642454-853E-F049-84B7-745455B992F3}" name="County" dataDxfId="53"/>
-    <tableColumn id="9" xr3:uid="{5B5F7B45-CEFB-EE48-90E0-380BD11BD347}" name="Student Enrollment" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{DC5BC21C-5B26-D441-96D3-64D606494C9A}" name="Student Attendance Rate" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{16C5B399-2D53-AF41-815C-1F7C3259622D}" name="Student Chronic Truancy Rate" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{E3173650-9CBD-2046-9561-EC76593F21A4}" name="Chronic Absenteeism" dataDxfId="49"/>
-    <tableColumn id="12" xr3:uid="{A5C89E32-E6C7-354A-AD94-8B9E7BF5BEAF}" name="Total Teacher FTE" dataDxfId="48"/>
-    <tableColumn id="15" xr3:uid="{91CEEB72-10AD-5347-AD91-C2EA26951FFD}" name="Teacher Retention Rate" dataDxfId="47"/>
-    <tableColumn id="16" xr3:uid="{B95926A8-CE9E-5E4C-8517-F53E1DD6BB12}" name="Pupil Teacher Ratio - Elementary" dataDxfId="46"/>
-    <tableColumn id="17" xr3:uid="{66E6EF1B-5F71-724F-BE1B-2EAE768FA6E4}" name="Pupil Teacher Ratio - High School" dataDxfId="45"/>
-    <tableColumn id="18" xr3:uid="{FF7C5CB9-8A3F-654A-AAC2-F90DDD57691C}" name="% Novice Teachers" dataDxfId="44"/>
-    <tableColumn id="21" xr3:uid="{14F53AE3-04FD-0049-9CD6-2E8BE716335E}" name="% Novice Teachers - High Poverty Schools" dataDxfId="43"/>
-    <tableColumn id="22" xr3:uid="{1A89C2C1-D5B1-D84E-AF9A-AFFF73A90C04}" name="% Novice Teachers - Low Poverty Schools" dataDxfId="42"/>
-    <tableColumn id="19" xr3:uid="{31BB3C4C-CD8A-9848-85A3-6A3A4A977857}" name="% 8th Grade Passing Algebra 1" dataDxfId="41"/>
-    <tableColumn id="20" xr3:uid="{7DC2CAA5-3B64-9C42-8E87-31C44668510E}" name="% 9th Grade on Track" dataDxfId="40"/>
-    <tableColumn id="23" xr3:uid="{AD3426F6-72EB-7A4F-BA71-66C2A3294CCF}" name="# 9th Grade on Track" dataDxfId="39"/>
-    <tableColumn id="24" xr3:uid="{7124EEF3-D182-7A4B-A827-DEC5EE0B1591}" name="# CTE Enrollment" dataDxfId="38"/>
-    <tableColumn id="25" xr3:uid="{0206B422-7E9A-AF41-A20D-0A4445D084F7}" name="# CTE Participants" dataDxfId="37"/>
-    <tableColumn id="26" xr3:uid="{74152CBC-6192-FA44-8D72-64E4E7284B17}" name="4-Year Graduation Rate (Perkins)" dataDxfId="36"/>
-    <tableColumn id="27" xr3:uid="{E91D57BE-E786-0E41-A6C9-D40C584A25B7}" name="Postsecondary Placement Rate (Perkins)" dataDxfId="35"/>
-    <tableColumn id="28" xr3:uid="{61C1EAC6-2067-F84E-B17C-A8B628C30DA0}" name="Nontraditional Program Enrollment Rate (Perkins)" dataDxfId="34"/>
-    <tableColumn id="29" xr3:uid="{612816CA-7F21-1C4E-9A0F-5C68D82ADF7D}" name="# Students who took Dual Credit classes Grade 9" dataDxfId="33"/>
-    <tableColumn id="30" xr3:uid="{5753F583-62B9-8A44-A3EC-546C676CE502}" name="# Students who took Dual Credit classes Grade 10" dataDxfId="32"/>
-    <tableColumn id="31" xr3:uid="{99388DA0-03B4-324C-93D0-00C4E7DFFD44}" name="# Students who took Dual Credit classes Grade 11" dataDxfId="31"/>
-    <tableColumn id="32" xr3:uid="{100FC056-2E22-0C4B-9AAC-CCBAF3958BB5}" name="# Students who took Dual Credit classes Grade 12" dataDxfId="30"/>
-    <tableColumn id="33" xr3:uid="{7148123E-CBBF-7A4C-A783-2B28AF22F11E}" name="# Students enrolled in Dual Credit Coursework" dataDxfId="29"/>
-    <tableColumn id="34" xr3:uid="{9282E612-FE85-D14F-B5B4-F790B296E915}" name="% Students enrolled in Dual Credit Coursework" dataDxfId="28"/>
-    <tableColumn id="35" xr3:uid="{62431BD2-7051-FC48-BD9B-525CBF545DDD}" name="# Students who took AP classes Grade 9" dataDxfId="27"/>
-    <tableColumn id="36" xr3:uid="{73C469BE-B611-0145-B886-AAA2CB70EAE8}" name="# Students who took AP classes Grade 10" dataDxfId="26"/>
-    <tableColumn id="37" xr3:uid="{CFE88FEF-98CA-654A-B3B8-05790EA4E553}" name="# Students who took AP classes Grade 11" dataDxfId="25"/>
-    <tableColumn id="38" xr3:uid="{CB531B3F-8204-2644-91D3-88ACB4BFD0A7}" name="# Students who took AP classes Grade 12" dataDxfId="24"/>
-    <tableColumn id="39" xr3:uid="{97ED4799-6B71-FF44-A7E9-0D6FEC826075}" name="# Students who took IB classes Grade 9" dataDxfId="23"/>
-    <tableColumn id="40" xr3:uid="{F30102B8-881A-CA42-88CE-89D1D66A2AFB}" name="# Students who took IB classes Grade 10" dataDxfId="22"/>
-    <tableColumn id="41" xr3:uid="{99E2E959-F950-414B-BBF3-82CF023E0766}" name="# Students who took IB classes Grade 11" dataDxfId="21"/>
-    <tableColumn id="42" xr3:uid="{E9437747-1EEE-D94C-8B2E-5EB4508C3746}" name="# Students who took IB classes Grade 12" dataDxfId="20"/>
-    <tableColumn id="43" xr3:uid="{3CBA554F-964A-B546-B1CB-F3FFBC958E43}" name="# Out-of-Field Teachers" dataDxfId="19"/>
-    <tableColumn id="44" xr3:uid="{C4CCD547-D042-A040-8E97-CD2FA1F749A9}" name="% Out-of-Field Teachers" dataDxfId="18"/>
-    <tableColumn id="45" xr3:uid="{DC129293-5D55-4C48-A979-6304ABE3CAB9}" name="% Teachers with Short-Term or Provisional License" dataDxfId="17"/>
-    <tableColumn id="46" xr3:uid="{69922C1F-B1F6-AA41-8916-728215E1A659}" name="% Teachers with Short-Term or Provisional License - High Poverty Schools" dataDxfId="16"/>
-    <tableColumn id="47" xr3:uid="{CB9F66DB-18B6-4A41-A560-2737C375BEAA}" name="% Teachers with Short-Term or Provisional License - Low Poverty Schools" dataDxfId="15"/>
-    <tableColumn id="48" xr3:uid="{FA593E29-37FA-2F49-B1E2-8A20B24707C0}" name="# Teachers with Short-Term or Provisional License - High Poverty Schools" dataDxfId="14"/>
-    <tableColumn id="49" xr3:uid="{F17AD799-AAF2-CA4B-9052-79526ED68F55}" name="# Teachers with Short-Term or Provisional License - Low Poverty Schools" dataDxfId="13"/>
-    <tableColumn id="50" xr3:uid="{95D43F71-6E78-7545-8A4C-AE8258AA92BA}" name="Teacher Attendance Rate" dataDxfId="12"/>
-    <tableColumn id="51" xr3:uid="{35904462-8ACF-104B-8595-F9EDDB9D005D}" name="Principal Turnover within 6 Years" dataDxfId="11"/>
-    <tableColumn id="52" xr3:uid="{37C54579-1382-4047-B32E-9B6DCF4C6D1A}" name="High School 4-Year Graduation Rate" dataDxfId="10"/>
-    <tableColumn id="53" xr3:uid="{76C7C142-3803-C743-ACB8-2AC253A56510}" name="High School 6-Year Graduation Rate" dataDxfId="9"/>
+  <tableColumns count="61">
+    <tableColumn id="1" xr3:uid="{6DA6945B-9D7D-0142-A374-7C4A97BBBBAB}" name="Year" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{1617EDAF-51CD-413F-9022-F6E4C97C233F}" name="RCDTS" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{A67D85A4-5303-744E-B7CD-31ECBC6CE0A7}" name="Type" dataDxfId="67"/>
+    <tableColumn id="13" xr3:uid="{C8F50192-B0A1-D84D-96D9-819955E9CE26}" name="District Type" dataDxfId="66"/>
+    <tableColumn id="14" xr3:uid="{A7661728-A363-9840-8182-CBC0352B14C6}" name="School Type" dataDxfId="65"/>
+    <tableColumn id="4" xr3:uid="{94336B41-A312-184A-9F00-C5E1720E28AF}" name="School Name" dataDxfId="64"/>
+    <tableColumn id="5" xr3:uid="{7516DA0D-E868-1941-B0D3-80B0E523A018}" name="District Name" dataDxfId="63"/>
+    <tableColumn id="10" xr3:uid="{DCD59F4B-C55C-2846-9070-7F8CC6CA2F51}" name="City" dataDxfId="62"/>
+    <tableColumn id="11" xr3:uid="{AB642454-853E-F049-84B7-745455B992F3}" name="County" dataDxfId="61"/>
+    <tableColumn id="9" xr3:uid="{5B5F7B45-CEFB-EE48-90E0-380BD11BD347}" name="Student Enrollment" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{DC5BC21C-5B26-D441-96D3-64D606494C9A}" name="Student Attendance Rate" dataDxfId="59"/>
+    <tableColumn id="7" xr3:uid="{16C5B399-2D53-AF41-815C-1F7C3259622D}" name="Student Chronic Truancy Rate" dataDxfId="58"/>
+    <tableColumn id="8" xr3:uid="{E3173650-9CBD-2046-9561-EC76593F21A4}" name="Chronic Absenteeism" dataDxfId="57"/>
+    <tableColumn id="12" xr3:uid="{A5C89E32-E6C7-354A-AD94-8B9E7BF5BEAF}" name="Total Teacher FTE" dataDxfId="56"/>
+    <tableColumn id="15" xr3:uid="{91CEEB72-10AD-5347-AD91-C2EA26951FFD}" name="Teacher Retention Rate" dataDxfId="55"/>
+    <tableColumn id="16" xr3:uid="{B95926A8-CE9E-5E4C-8517-F53E1DD6BB12}" name="Pupil Teacher Ratio - Elementary" dataDxfId="54"/>
+    <tableColumn id="17" xr3:uid="{66E6EF1B-5F71-724F-BE1B-2EAE768FA6E4}" name="Pupil Teacher Ratio - High School" dataDxfId="53"/>
+    <tableColumn id="18" xr3:uid="{FF7C5CB9-8A3F-654A-AAC2-F90DDD57691C}" name="% Novice Teachers" dataDxfId="52"/>
+    <tableColumn id="21" xr3:uid="{14F53AE3-04FD-0049-9CD6-2E8BE716335E}" name="% Novice Teachers - High Poverty Schools" dataDxfId="51"/>
+    <tableColumn id="22" xr3:uid="{1A89C2C1-D5B1-D84E-AF9A-AFFF73A90C04}" name="% Novice Teachers - Low Poverty Schools" dataDxfId="50"/>
+    <tableColumn id="19" xr3:uid="{31BB3C4C-CD8A-9848-85A3-6A3A4A977857}" name="% 8th Grade Passing Algebra 1" dataDxfId="49"/>
+    <tableColumn id="20" xr3:uid="{7DC2CAA5-3B64-9C42-8E87-31C44668510E}" name="% 9th Grade on Track" dataDxfId="48"/>
+    <tableColumn id="23" xr3:uid="{AD3426F6-72EB-7A4F-BA71-66C2A3294CCF}" name="# 9th Grade on Track" dataDxfId="47"/>
+    <tableColumn id="24" xr3:uid="{7124EEF3-D182-7A4B-A827-DEC5EE0B1591}" name="# CTE Enrollment" dataDxfId="46"/>
+    <tableColumn id="25" xr3:uid="{0206B422-7E9A-AF41-A20D-0A4445D084F7}" name="# CTE Participants" dataDxfId="45"/>
+    <tableColumn id="26" xr3:uid="{74152CBC-6192-FA44-8D72-64E4E7284B17}" name="4-Year Graduation Rate (Perkins)" dataDxfId="44"/>
+    <tableColumn id="27" xr3:uid="{E91D57BE-E786-0E41-A6C9-D40C584A25B7}" name="Postsecondary Placement Rate (Perkins)" dataDxfId="43"/>
+    <tableColumn id="28" xr3:uid="{61C1EAC6-2067-F84E-B17C-A8B628C30DA0}" name="Nontraditional Program Enrollment Rate (Perkins)" dataDxfId="42"/>
+    <tableColumn id="29" xr3:uid="{612816CA-7F21-1C4E-9A0F-5C68D82ADF7D}" name="# Students who took Dual Credit classes Grade 9" dataDxfId="41"/>
+    <tableColumn id="30" xr3:uid="{5753F583-62B9-8A44-A3EC-546C676CE502}" name="# Students who took Dual Credit classes Grade 10" dataDxfId="40"/>
+    <tableColumn id="31" xr3:uid="{99388DA0-03B4-324C-93D0-00C4E7DFFD44}" name="# Students who took Dual Credit classes Grade 11" dataDxfId="39"/>
+    <tableColumn id="32" xr3:uid="{100FC056-2E22-0C4B-9AAC-CCBAF3958BB5}" name="# Students who took Dual Credit classes Grade 12" dataDxfId="38"/>
+    <tableColumn id="33" xr3:uid="{7148123E-CBBF-7A4C-A783-2B28AF22F11E}" name="# Students enrolled in Dual Credit Coursework" dataDxfId="37"/>
+    <tableColumn id="34" xr3:uid="{9282E612-FE85-D14F-B5B4-F790B296E915}" name="% Students enrolled in Dual Credit Coursework" dataDxfId="36"/>
+    <tableColumn id="35" xr3:uid="{62431BD2-7051-FC48-BD9B-525CBF545DDD}" name="# Students who took AP classes Grade 9" dataDxfId="35"/>
+    <tableColumn id="36" xr3:uid="{73C469BE-B611-0145-B886-AAA2CB70EAE8}" name="# Students who took AP classes Grade 10" dataDxfId="34"/>
+    <tableColumn id="37" xr3:uid="{CFE88FEF-98CA-654A-B3B8-05790EA4E553}" name="# Students who took AP classes Grade 11" dataDxfId="33"/>
+    <tableColumn id="38" xr3:uid="{CB531B3F-8204-2644-91D3-88ACB4BFD0A7}" name="# Students who took AP classes Grade 12" dataDxfId="32"/>
+    <tableColumn id="39" xr3:uid="{97ED4799-6B71-FF44-A7E9-0D6FEC826075}" name="# Students who took IB classes Grade 9" dataDxfId="31"/>
+    <tableColumn id="40" xr3:uid="{F30102B8-881A-CA42-88CE-89D1D66A2AFB}" name="# Students who took IB classes Grade 10" dataDxfId="30"/>
+    <tableColumn id="41" xr3:uid="{99E2E959-F950-414B-BBF3-82CF023E0766}" name="# Students who took IB classes Grade 11" dataDxfId="29"/>
+    <tableColumn id="42" xr3:uid="{E9437747-1EEE-D94C-8B2E-5EB4508C3746}" name="# Students who took IB classes Grade 12" dataDxfId="28"/>
+    <tableColumn id="43" xr3:uid="{3CBA554F-964A-B546-B1CB-F3FFBC958E43}" name="# Out-of-Field Teachers" dataDxfId="27"/>
+    <tableColumn id="44" xr3:uid="{C4CCD547-D042-A040-8E97-CD2FA1F749A9}" name="% Out-of-Field Teachers" dataDxfId="26"/>
+    <tableColumn id="45" xr3:uid="{DC129293-5D55-4C48-A979-6304ABE3CAB9}" name="% Teachers with Short-Term or Provisional License" dataDxfId="25"/>
+    <tableColumn id="46" xr3:uid="{69922C1F-B1F6-AA41-8916-728215E1A659}" name="% Teachers with Short-Term or Provisional License - High Poverty Schools" dataDxfId="24"/>
+    <tableColumn id="47" xr3:uid="{CB9F66DB-18B6-4A41-A560-2737C375BEAA}" name="% Teachers with Short-Term or Provisional License - Low Poverty Schools" dataDxfId="23"/>
+    <tableColumn id="48" xr3:uid="{FA593E29-37FA-2F49-B1E2-8A20B24707C0}" name="# Teachers with Short-Term or Provisional License - High Poverty Schools" dataDxfId="22"/>
+    <tableColumn id="49" xr3:uid="{F17AD799-AAF2-CA4B-9052-79526ED68F55}" name="# Teachers with Short-Term or Provisional License - Low Poverty Schools" dataDxfId="21"/>
+    <tableColumn id="50" xr3:uid="{95D43F71-6E78-7545-8A4C-AE8258AA92BA}" name="Teacher Attendance Rate" dataDxfId="20"/>
+    <tableColumn id="51" xr3:uid="{35904462-8ACF-104B-8595-F9EDDB9D005D}" name="Principal Turnover within 6 Years" dataDxfId="19"/>
+    <tableColumn id="52" xr3:uid="{37C54579-1382-4047-B32E-9B6DCF4C6D1A}" name="High School 4-Year Graduation Rate" dataDxfId="18"/>
+    <tableColumn id="53" xr3:uid="{76C7C142-3803-C743-ACB8-2AC253A56510}" name="High School 6-Year Graduation Rate" dataDxfId="17"/>
+    <tableColumn id="54" xr3:uid="{D57E1850-D7FE-9141-B5FF-8D139A17D39D}" name="Number of students who took one or more AP Exams Grade 9" dataDxfId="16"/>
+    <tableColumn id="55" xr3:uid="{D85884E7-853A-2E46-93D7-579975E2D930}" name="Number of students who passed one or more AP Exams Grade 9" dataDxfId="15"/>
+    <tableColumn id="56" xr3:uid="{24D843C3-F6B3-4A48-8E47-DCCC0C37AB56}" name="Number of students who took one or more AP Exams Grade 10" dataDxfId="14"/>
+    <tableColumn id="57" xr3:uid="{C1215080-ECBF-3A40-951A-7496839DDC04}" name="Number of students who passed one or more AP Exams Grade 10" dataDxfId="13"/>
+    <tableColumn id="58" xr3:uid="{5305A7BA-20A4-B64A-BEE0-7EBE5CA1285E}" name="Number of students who took one or more AP Exams Grade 11" dataDxfId="12">
+      <calculatedColumnFormula>REPLACE(BD2,FIND("10",BD2),2,"11")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="59" xr3:uid="{95397CC1-7B04-4B4A-A1EE-AB2A5546B55E}" name="Number of students who passed one or more AP Exams Grade 11" dataDxfId="11">
+      <calculatedColumnFormula>REPLACE(BE2,FIND("10",BE2),2,"11")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="60" xr3:uid="{09F63790-ADCE-6E4A-A471-0A5D1D8214A2}" name="Number of students who took one or more AP Exams Grade 12" dataDxfId="10">
+      <calculatedColumnFormula>REPLACE(BF2,FIND("11",BF2),2,"12")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="61" xr3:uid="{EF07B6AA-C8A6-FC44-BFD2-653A0B6E2A86}" name="Number of students who passed one or more AP Exams Grade 12" dataDxfId="9">
+      <calculatedColumnFormula>REPLACE(BG2,FIND("11",BG2),2,"12")</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}" name="Table44" displayName="Table44" ref="A1:H468" totalsRowShown="0" dataDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="A1:H468" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}" name="Table44" displayName="Table44" ref="A1:H526" totalsRowShown="0" dataDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A1:H526" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H323">
     <sortCondition ref="B1:B323"/>
   </sortState>
@@ -2814,11 +2956,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BA26"/>
+  <dimension ref="A1:BI26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I22" sqref="I22:I23"/>
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AZ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BD10" activeCellId="1" sqref="A10:A17 BD10:BE17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2870,9 +3012,16 @@
     <col min="51" max="51" width="42.83203125" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="38.5" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="33" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="52.5" bestFit="1" customWidth="1"/>
+    <col min="55" max="56" width="54.5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="55.1640625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="55.1640625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="52.5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="54.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:61" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3032,8 +3181,32 @@
       <c r="BA1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB1" t="s">
+        <v>248</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>249</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>252</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>250</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>253</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>251</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>254</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2008</v>
       </c>
@@ -3089,8 +3262,16 @@
       <c r="AZ2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB2" s="19"/>
+      <c r="BC2" s="19"/>
+      <c r="BD2" s="19"/>
+      <c r="BE2" s="19"/>
+      <c r="BF2" s="19"/>
+      <c r="BG2" s="19"/>
+      <c r="BH2" s="19"/>
+      <c r="BI2" s="19"/>
+    </row>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2009</v>
       </c>
@@ -3146,8 +3327,16 @@
       <c r="AZ3" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB3" s="19"/>
+      <c r="BC3" s="19"/>
+      <c r="BD3" s="19"/>
+      <c r="BE3" s="19"/>
+      <c r="BF3" s="19"/>
+      <c r="BG3" s="19"/>
+      <c r="BH3" s="19"/>
+      <c r="BI3" s="19"/>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2010</v>
       </c>
@@ -3203,8 +3392,16 @@
       <c r="AZ4" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB4" s="19"/>
+      <c r="BC4" s="19"/>
+      <c r="BD4" s="19"/>
+      <c r="BE4" s="19"/>
+      <c r="BF4" s="19"/>
+      <c r="BG4" s="19"/>
+      <c r="BH4" s="19"/>
+      <c r="BI4" s="19"/>
+    </row>
+    <row r="5" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2011</v>
       </c>
@@ -3260,8 +3457,16 @@
       <c r="AZ5" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB5" s="19"/>
+      <c r="BC5" s="19"/>
+      <c r="BD5" s="19"/>
+      <c r="BE5" s="19"/>
+      <c r="BF5" s="19"/>
+      <c r="BG5" s="19"/>
+      <c r="BH5" s="19"/>
+      <c r="BI5" s="19"/>
+    </row>
+    <row r="6" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2012</v>
       </c>
@@ -3317,8 +3522,16 @@
       <c r="AZ6" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB6" s="19"/>
+      <c r="BC6" s="19"/>
+      <c r="BD6" s="19"/>
+      <c r="BE6" s="19"/>
+      <c r="BF6" s="19"/>
+      <c r="BG6" s="19"/>
+      <c r="BH6" s="19"/>
+      <c r="BI6" s="19"/>
+    </row>
+    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2013</v>
       </c>
@@ -3374,8 +3587,16 @@
       <c r="AZ7" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB7" s="19"/>
+      <c r="BC7" s="19"/>
+      <c r="BD7" s="19"/>
+      <c r="BE7" s="19"/>
+      <c r="BF7" s="19"/>
+      <c r="BG7" s="19"/>
+      <c r="BH7" s="19"/>
+      <c r="BI7" s="19"/>
+    </row>
+    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2014</v>
       </c>
@@ -3440,8 +3661,16 @@
       <c r="AZ8" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB8" s="19"/>
+      <c r="BC8" s="19"/>
+      <c r="BD8" s="19"/>
+      <c r="BE8" s="19"/>
+      <c r="BF8" s="19"/>
+      <c r="BG8" s="19"/>
+      <c r="BH8" s="19"/>
+      <c r="BI8" s="19"/>
+    </row>
+    <row r="9" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2015</v>
       </c>
@@ -3509,8 +3738,16 @@
       <c r="AZ9" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB9" s="19"/>
+      <c r="BC9" s="19"/>
+      <c r="BD9" s="19"/>
+      <c r="BE9" s="19"/>
+      <c r="BF9" s="19"/>
+      <c r="BG9" s="19"/>
+      <c r="BH9" s="19"/>
+      <c r="BI9" s="19"/>
+    </row>
+    <row r="10" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2016</v>
       </c>
@@ -3605,8 +3842,30 @@
       <c r="BA10" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB10" s="19"/>
+      <c r="BC10" s="19"/>
+      <c r="BD10" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="BE10" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="BF10" s="19" t="str">
+        <f>REPLACE(BD10,FIND("10",BD10),2,"11")</f>
+        <v># of GRADE 11 STUDENTS TOOK ONE OR MORE AP EXAMS (SCHOOL)</v>
+      </c>
+      <c r="BG10" s="19" t="str">
+        <f>REPLACE(BE10,FIND("10",BE10),2,"11")</f>
+        <v># of GRADE 11 STUDENTS PASSED ONE OR MORE AP EXAMS (SCHOOL)</v>
+      </c>
+      <c r="BH10" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="BI10" s="19" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2017</v>
       </c>
@@ -3701,8 +3960,30 @@
       <c r="BA11" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB11" s="19"/>
+      <c r="BC11" s="19"/>
+      <c r="BD11" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="BE11" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="BF11" s="19" t="str">
+        <f t="shared" ref="BF11:BF17" si="0">REPLACE(BD11,FIND("10",BD11),2,"11")</f>
+        <v># of GRADE 11 STUDENTS TOOK ONE OR MORE AP EXAMS (SCHOOL)</v>
+      </c>
+      <c r="BG11" s="19" t="str">
+        <f t="shared" ref="BG11:BG17" si="1">REPLACE(BE11,FIND("10",BE11),2,"11")</f>
+        <v># of GRADE 11 STUDENTS PASSED ONE OR MORE AP EXAMS (SCHOOL)</v>
+      </c>
+      <c r="BH11" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="BI11" s="19" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -3823,8 +4104,30 @@
       <c r="BA12" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB12" s="19"/>
+      <c r="BC12" s="19"/>
+      <c r="BD12" t="s">
+        <v>240</v>
+      </c>
+      <c r="BE12" t="s">
+        <v>241</v>
+      </c>
+      <c r="BF12" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Number of students who took one ore more AP Exams Grade 11</v>
+      </c>
+      <c r="BG12" s="19" t="str">
+        <f t="shared" si="1"/>
+        <v>Number of students who passed one ore more AP Exams Grade 11</v>
+      </c>
+      <c r="BH12" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="BI12" s="19" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="13" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2019</v>
       </c>
@@ -3954,8 +4257,34 @@
       <c r="BA13" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB13" t="s">
+        <v>246</v>
+      </c>
+      <c r="BC13" t="s">
+        <v>247</v>
+      </c>
+      <c r="BD13" t="s">
+        <v>240</v>
+      </c>
+      <c r="BE13" t="s">
+        <v>241</v>
+      </c>
+      <c r="BF13" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Number of students who took one ore more AP Exams Grade 11</v>
+      </c>
+      <c r="BG13" s="19" t="str">
+        <f t="shared" si="1"/>
+        <v>Number of students who passed one ore more AP Exams Grade 11</v>
+      </c>
+      <c r="BH13" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="BI13" s="19" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2020</v>
       </c>
@@ -4085,8 +4414,34 @@
       <c r="BA14" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB14" t="s">
+        <v>246</v>
+      </c>
+      <c r="BC14" t="s">
+        <v>247</v>
+      </c>
+      <c r="BD14" t="s">
+        <v>240</v>
+      </c>
+      <c r="BE14" t="s">
+        <v>241</v>
+      </c>
+      <c r="BF14" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Number of students who took one ore more AP Exams Grade 11</v>
+      </c>
+      <c r="BG14" s="19" t="str">
+        <f t="shared" si="1"/>
+        <v>Number of students who passed one ore more AP Exams Grade 11</v>
+      </c>
+      <c r="BH14" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="BI14" s="19" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2021</v>
       </c>
@@ -4222,8 +4577,34 @@
       <c r="BA15" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB15" t="s">
+        <v>246</v>
+      </c>
+      <c r="BC15" t="s">
+        <v>247</v>
+      </c>
+      <c r="BD15" t="s">
+        <v>240</v>
+      </c>
+      <c r="BE15" t="s">
+        <v>241</v>
+      </c>
+      <c r="BF15" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Number of students who took one ore more AP Exams Grade 11</v>
+      </c>
+      <c r="BG15" s="19" t="str">
+        <f t="shared" si="1"/>
+        <v>Number of students who passed one ore more AP Exams Grade 11</v>
+      </c>
+      <c r="BH15" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="BI15" s="19" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="16" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2022</v>
       </c>
@@ -4371,8 +4752,34 @@
       <c r="BA16" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB16" t="s">
+        <v>246</v>
+      </c>
+      <c r="BC16" t="s">
+        <v>247</v>
+      </c>
+      <c r="BD16" t="s">
+        <v>240</v>
+      </c>
+      <c r="BE16" t="s">
+        <v>241</v>
+      </c>
+      <c r="BF16" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Number of students who took one ore more AP Exams Grade 11</v>
+      </c>
+      <c r="BG16" s="19" t="str">
+        <f t="shared" si="1"/>
+        <v>Number of students who passed one ore more AP Exams Grade 11</v>
+      </c>
+      <c r="BH16" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="BI16" s="19" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="17" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2023</v>
       </c>
@@ -4523,17 +4930,46 @@
       <c r="BA17" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB17" t="s">
+        <v>246</v>
+      </c>
+      <c r="BC17" t="s">
+        <v>247</v>
+      </c>
+      <c r="BD17" t="s">
+        <v>240</v>
+      </c>
+      <c r="BE17" t="s">
+        <v>241</v>
+      </c>
+      <c r="BF17" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Number of students who took one ore more AP Exams Grade 11</v>
+      </c>
+      <c r="BG17" s="19" t="str">
+        <f t="shared" si="1"/>
+        <v>Number of students who passed one ore more AP Exams Grade 11</v>
+      </c>
+      <c r="BH17" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="BI17" s="19" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="19" spans="1:61" x14ac:dyDescent="0.2">
       <c r="AZ19" s="18"/>
     </row>
-    <row r="26" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:61" x14ac:dyDescent="0.2">
       <c r="AP26" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="BH10:BI17" calculatedColumn="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -4542,12 +4978,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249B090D-D7BB-374A-9D81-FFCE8C0599DD}">
-  <dimension ref="A1:H468"/>
+  <dimension ref="A1:H526"/>
   <sheetViews>
-    <sheetView topLeftCell="A436" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A483" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A162" sqref="A162"/>
-      <selection pane="topRight" activeCell="C446" sqref="C446"/>
+      <selection pane="topRight" activeCell="C506" sqref="C506"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13176,7 +13612,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="465" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A465">
         <v>2020</v>
       </c>
@@ -13196,7 +13632,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="466" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A466">
         <v>2021</v>
       </c>
@@ -13216,7 +13652,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="467" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A467">
         <v>2022</v>
       </c>
@@ -13236,7 +13672,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="468" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A468">
         <v>2023</v>
       </c>
@@ -13255,6 +13691,1108 @@
       <c r="G468" t="s">
         <v>232</v>
       </c>
+    </row>
+    <row r="469" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A469" s="19">
+        <v>2019</v>
+      </c>
+      <c r="B469" t="s">
+        <v>249</v>
+      </c>
+      <c r="C469" t="s">
+        <v>247</v>
+      </c>
+      <c r="D469" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E469" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F469" s="19"/>
+      <c r="H469" s="19"/>
+    </row>
+    <row r="470" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A470" s="19">
+        <v>2020</v>
+      </c>
+      <c r="B470" t="s">
+        <v>249</v>
+      </c>
+      <c r="C470" t="s">
+        <v>247</v>
+      </c>
+      <c r="D470" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E470" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F470" s="19"/>
+      <c r="H470" s="19"/>
+    </row>
+    <row r="471" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A471" s="19">
+        <v>2021</v>
+      </c>
+      <c r="B471" t="s">
+        <v>249</v>
+      </c>
+      <c r="C471" t="s">
+        <v>247</v>
+      </c>
+      <c r="D471" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E471" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F471" s="19"/>
+      <c r="H471" s="19"/>
+    </row>
+    <row r="472" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A472" s="19">
+        <v>2022</v>
+      </c>
+      <c r="B472" t="s">
+        <v>249</v>
+      </c>
+      <c r="C472" t="s">
+        <v>247</v>
+      </c>
+      <c r="D472" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E472" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F472" s="19"/>
+      <c r="H472" s="19"/>
+    </row>
+    <row r="473" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A473" s="19">
+        <v>2023</v>
+      </c>
+      <c r="B473" t="s">
+        <v>249</v>
+      </c>
+      <c r="C473" t="s">
+        <v>247</v>
+      </c>
+      <c r="D473" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E473" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F473" s="19"/>
+      <c r="H473" s="19"/>
+    </row>
+    <row r="474" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A474" s="19">
+        <v>2019</v>
+      </c>
+      <c r="B474" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="C474" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="D474" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E474" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F474" s="19"/>
+      <c r="H474" s="19"/>
+    </row>
+    <row r="475" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A475" s="19">
+        <v>2020</v>
+      </c>
+      <c r="B475" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="C475" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="D475" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E475" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F475" s="19"/>
+      <c r="H475" s="19"/>
+    </row>
+    <row r="476" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A476" s="19">
+        <v>2021</v>
+      </c>
+      <c r="B476" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="C476" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="D476" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E476" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F476" s="19"/>
+      <c r="H476" s="19"/>
+    </row>
+    <row r="477" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A477" s="19">
+        <v>2022</v>
+      </c>
+      <c r="B477" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="C477" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="D477" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E477" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F477" s="19"/>
+      <c r="H477" s="19"/>
+    </row>
+    <row r="478" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A478" s="19">
+        <v>2023</v>
+      </c>
+      <c r="B478" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="C478" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="D478" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E478" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F478" s="19"/>
+      <c r="H478" s="19"/>
+    </row>
+    <row r="479" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A479" s="19">
+        <v>2016</v>
+      </c>
+      <c r="B479" t="s">
+        <v>250</v>
+      </c>
+      <c r="C479" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="D479" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E479" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F479" s="19"/>
+      <c r="H479" s="19"/>
+    </row>
+    <row r="480" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A480" s="19">
+        <v>2017</v>
+      </c>
+      <c r="B480" t="s">
+        <v>250</v>
+      </c>
+      <c r="C480" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="D480" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E480" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F480" s="19"/>
+      <c r="H480" s="19"/>
+    </row>
+    <row r="481" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A481" s="19">
+        <v>2018</v>
+      </c>
+      <c r="B481" t="s">
+        <v>250</v>
+      </c>
+      <c r="C481" t="s">
+        <v>241</v>
+      </c>
+      <c r="D481" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E481" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F481" s="19"/>
+      <c r="H481" s="19"/>
+    </row>
+    <row r="482" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A482" s="19">
+        <v>2019</v>
+      </c>
+      <c r="B482" t="s">
+        <v>250</v>
+      </c>
+      <c r="C482" t="s">
+        <v>241</v>
+      </c>
+      <c r="D482" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E482" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F482" s="19"/>
+      <c r="H482" s="19"/>
+    </row>
+    <row r="483" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A483" s="19">
+        <v>2020</v>
+      </c>
+      <c r="B483" t="s">
+        <v>250</v>
+      </c>
+      <c r="C483" t="s">
+        <v>241</v>
+      </c>
+      <c r="D483" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E483" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F483" s="19"/>
+      <c r="H483" s="19"/>
+    </row>
+    <row r="484" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A484" s="19">
+        <v>2021</v>
+      </c>
+      <c r="B484" t="s">
+        <v>250</v>
+      </c>
+      <c r="C484" t="s">
+        <v>241</v>
+      </c>
+      <c r="D484" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E484" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F484" s="19"/>
+      <c r="H484" s="19"/>
+    </row>
+    <row r="485" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A485" s="19">
+        <v>2022</v>
+      </c>
+      <c r="B485" t="s">
+        <v>250</v>
+      </c>
+      <c r="C485" t="s">
+        <v>241</v>
+      </c>
+      <c r="D485" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E485" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F485" s="19"/>
+      <c r="H485" s="19"/>
+    </row>
+    <row r="486" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A486" s="19">
+        <v>2023</v>
+      </c>
+      <c r="B486" t="s">
+        <v>250</v>
+      </c>
+      <c r="C486" t="s">
+        <v>241</v>
+      </c>
+      <c r="D486" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E486" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F486" s="19"/>
+      <c r="H486" s="19"/>
+    </row>
+    <row r="487" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A487" s="19">
+        <v>2016</v>
+      </c>
+      <c r="B487" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="C487" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="D487" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E487" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F487" s="19"/>
+      <c r="H487" s="19"/>
+    </row>
+    <row r="488" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A488" s="19">
+        <v>2017</v>
+      </c>
+      <c r="B488" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="C488" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="D488" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E488" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F488" s="19"/>
+      <c r="H488" s="19"/>
+    </row>
+    <row r="489" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A489" s="19">
+        <v>2018</v>
+      </c>
+      <c r="B489" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="C489" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="D489" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E489" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F489" s="19"/>
+      <c r="H489" s="19"/>
+    </row>
+    <row r="490" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A490" s="19">
+        <v>2019</v>
+      </c>
+      <c r="B490" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="C490" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="D490" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E490" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F490" s="19"/>
+      <c r="H490" s="19"/>
+    </row>
+    <row r="491" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A491" s="19">
+        <v>2020</v>
+      </c>
+      <c r="B491" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="C491" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="D491" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E491" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F491" s="19"/>
+      <c r="H491" s="19"/>
+    </row>
+    <row r="492" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A492" s="19">
+        <v>2021</v>
+      </c>
+      <c r="B492" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="C492" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="D492" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E492" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F492" s="19"/>
+      <c r="H492" s="19"/>
+    </row>
+    <row r="493" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A493" s="19">
+        <v>2022</v>
+      </c>
+      <c r="B493" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="C493" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="D493" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E493" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F493" s="19"/>
+      <c r="H493" s="19"/>
+    </row>
+    <row r="494" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A494" s="19">
+        <v>2023</v>
+      </c>
+      <c r="B494" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="C494" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="D494" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E494" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F494" s="19"/>
+      <c r="H494" s="19"/>
+    </row>
+    <row r="495" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A495" s="19">
+        <v>2016</v>
+      </c>
+      <c r="B495" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="C495" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="D495" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E495" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F495" s="19"/>
+      <c r="H495" s="19"/>
+    </row>
+    <row r="496" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A496" s="19">
+        <v>2017</v>
+      </c>
+      <c r="B496" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="C496" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="D496" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E496" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F496" s="19"/>
+      <c r="H496" s="19"/>
+    </row>
+    <row r="497" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A497" s="19">
+        <v>2018</v>
+      </c>
+      <c r="B497" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="C497" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="D497" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E497" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F497" s="19"/>
+      <c r="H497" s="19"/>
+    </row>
+    <row r="498" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A498" s="19">
+        <v>2019</v>
+      </c>
+      <c r="B498" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="C498" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="D498" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E498" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F498" s="19"/>
+      <c r="H498" s="19"/>
+    </row>
+    <row r="499" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A499" s="19">
+        <v>2020</v>
+      </c>
+      <c r="B499" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="C499" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="D499" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E499" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F499" s="19"/>
+      <c r="H499" s="19"/>
+    </row>
+    <row r="500" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A500" s="19">
+        <v>2021</v>
+      </c>
+      <c r="B500" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="C500" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="D500" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E500" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F500" s="19"/>
+      <c r="H500" s="19"/>
+    </row>
+    <row r="501" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A501" s="19">
+        <v>2022</v>
+      </c>
+      <c r="B501" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="C501" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="D501" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E501" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F501" s="19"/>
+      <c r="H501" s="19"/>
+    </row>
+    <row r="502" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A502" s="19">
+        <v>2023</v>
+      </c>
+      <c r="B502" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="C502" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="D502" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E502" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F502" s="19"/>
+      <c r="H502" s="19"/>
+    </row>
+    <row r="503" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A503" s="19">
+        <v>2016</v>
+      </c>
+      <c r="B503" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="C503" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="D503" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E503" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F503" s="19"/>
+      <c r="H503" s="19"/>
+    </row>
+    <row r="504" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A504" s="19">
+        <v>2017</v>
+      </c>
+      <c r="B504" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="C504" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="D504" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E504" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F504" s="19"/>
+      <c r="H504" s="19"/>
+    </row>
+    <row r="505" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A505" s="19">
+        <v>2018</v>
+      </c>
+      <c r="B505" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="C505" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D505" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E505" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F505" s="19"/>
+      <c r="H505" s="19"/>
+    </row>
+    <row r="506" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A506" s="19">
+        <v>2019</v>
+      </c>
+      <c r="B506" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="C506" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D506" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E506" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F506" s="19"/>
+      <c r="H506" s="19"/>
+    </row>
+    <row r="507" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A507" s="19">
+        <v>2020</v>
+      </c>
+      <c r="B507" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="C507" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D507" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E507" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F507" s="19"/>
+      <c r="H507" s="19"/>
+    </row>
+    <row r="508" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A508" s="19">
+        <v>2021</v>
+      </c>
+      <c r="B508" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="C508" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D508" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E508" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F508" s="19"/>
+      <c r="H508" s="19"/>
+    </row>
+    <row r="509" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A509" s="19">
+        <v>2022</v>
+      </c>
+      <c r="B509" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="C509" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D509" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E509" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F509" s="19"/>
+      <c r="H509" s="19"/>
+    </row>
+    <row r="510" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A510" s="19">
+        <v>2023</v>
+      </c>
+      <c r="B510" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="C510" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D510" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E510" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F510" s="19"/>
+      <c r="H510" s="19"/>
+    </row>
+    <row r="511" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A511" s="19">
+        <v>2016</v>
+      </c>
+      <c r="B511" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="C511" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="D511" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E511" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F511" s="19"/>
+      <c r="H511" s="19"/>
+    </row>
+    <row r="512" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A512" s="19">
+        <v>2017</v>
+      </c>
+      <c r="B512" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="C512" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="D512" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E512" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F512" s="19"/>
+      <c r="H512" s="19"/>
+    </row>
+    <row r="513" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A513" s="19">
+        <v>2018</v>
+      </c>
+      <c r="B513" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="C513" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="D513" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E513" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F513" s="19"/>
+      <c r="H513" s="19"/>
+    </row>
+    <row r="514" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A514" s="19">
+        <v>2019</v>
+      </c>
+      <c r="B514" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="C514" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="D514" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E514" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F514" s="19"/>
+      <c r="H514" s="19"/>
+    </row>
+    <row r="515" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A515" s="19">
+        <v>2020</v>
+      </c>
+      <c r="B515" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="C515" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="D515" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E515" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F515" s="19"/>
+      <c r="H515" s="19"/>
+    </row>
+    <row r="516" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A516" s="19">
+        <v>2021</v>
+      </c>
+      <c r="B516" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="C516" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="D516" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E516" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F516" s="19"/>
+      <c r="H516" s="19"/>
+    </row>
+    <row r="517" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A517" s="19">
+        <v>2022</v>
+      </c>
+      <c r="B517" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="C517" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="D517" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E517" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F517" s="19"/>
+      <c r="H517" s="19"/>
+    </row>
+    <row r="518" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A518" s="19">
+        <v>2023</v>
+      </c>
+      <c r="B518" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="C518" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="D518" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E518" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F518" s="19"/>
+      <c r="H518" s="19"/>
+    </row>
+    <row r="519" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A519" s="19">
+        <v>2016</v>
+      </c>
+      <c r="B519" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="C519" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="D519" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E519" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F519" s="19"/>
+      <c r="H519" s="19"/>
+    </row>
+    <row r="520" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A520" s="19">
+        <v>2017</v>
+      </c>
+      <c r="B520" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="C520" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="D520" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E520" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F520" s="19"/>
+      <c r="H520" s="19"/>
+    </row>
+    <row r="521" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A521" s="19">
+        <v>2018</v>
+      </c>
+      <c r="B521" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="C521" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="D521" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E521" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F521" s="19"/>
+      <c r="H521" s="19"/>
+    </row>
+    <row r="522" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A522" s="19">
+        <v>2019</v>
+      </c>
+      <c r="B522" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="C522" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="D522" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E522" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F522" s="19"/>
+      <c r="H522" s="19"/>
+    </row>
+    <row r="523" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A523" s="19">
+        <v>2020</v>
+      </c>
+      <c r="B523" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="C523" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="D523" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E523" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F523" s="19"/>
+      <c r="H523" s="19"/>
+    </row>
+    <row r="524" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A524" s="19">
+        <v>2021</v>
+      </c>
+      <c r="B524" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="C524" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="D524" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E524" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F524" s="19"/>
+      <c r="H524" s="19"/>
+    </row>
+    <row r="525" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A525" s="19">
+        <v>2022</v>
+      </c>
+      <c r="B525" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="C525" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="D525" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E525" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F525" s="19"/>
+      <c r="H525" s="19"/>
+    </row>
+    <row r="526" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A526" s="19">
+        <v>2023</v>
+      </c>
+      <c r="B526" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="C526" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="D526" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E526" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F526" s="19"/>
+      <c r="H526" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13266,6 +14804,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d5cc9fc5-cf59-440a-a506-890d57680064">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B598B773ED9FC644B8B740EB3205C8DA" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6cfe95817d5870f6c066b2c32ab5fb2a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xmlns:ns3="d5cc9fc5-cf59-440a-a506-890d57680064" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a231614a4bf4996e6f4146316e2aaf8" ns2:_="" ns3:_="">
     <xsd:import namespace="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
@@ -13528,27 +15086,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA6725D-5CB1-4E78-9F97-F79E79C18DA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="d5cc9fc5-cf59-440a-a506-890d57680064"/>
+    <ds:schemaRef ds:uri="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d5cc9fc5-cf59-440a-a506-890d57680064">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3FAF407-B1B6-4FB8-B534-293B9E1D533A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B298AB6-2F6D-497E-AD9E-0F97ABEC8463}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13565,29 +15128,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3FAF407-B1B6-4FB8-B534-293B9E1D533A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA6725D-5CB1-4E78-9F97-F79E79C18DA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d5cc9fc5-cf59-440a-a506-890d57680064"/>
-    <ds:schemaRef ds:uri="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Community College Remediation and Postsecondary Enrollment data
</commit_message>
<xml_diff>
--- a/Local Historic Crosswalk.xlsx
+++ b/Local Historic Crosswalk.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasontheisen/Documents/Advance Illinois/Historic Report Card/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4044659-AB15-E64C-A056-768AA7658491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{53CC54CE-CF44-B449-B462-B8F40993CAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report Card Metadata" sheetId="3" r:id="rId1"/>
     <sheet name="Name Crosswalk" sheetId="1" r:id="rId2"/>
     <sheet name="Details" sheetId="2" r:id="rId3"/>
-    <sheet name="ISBE Ask-For List" sheetId="4" r:id="rId4"/>
-    <sheet name="Notes" sheetId="5" r:id="rId5"/>
+    <sheet name="Notes" sheetId="5" r:id="rId4"/>
+    <sheet name="ISBE Ask-For List" sheetId="4" r:id="rId5"/>
     <sheet name="Missing Metrics" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3594" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4013" uniqueCount="433">
   <si>
     <t>Year</t>
   </si>
@@ -1784,12 +1784,170 @@
   <si>
     <t>% All students IAR ELA Level 1 - Grade 2</t>
   </si>
+  <si>
+    <t>IAR ELA No Participation Rate</t>
+  </si>
+  <si>
+    <t>IAR Math No Participation Rate</t>
+  </si>
+  <si>
+    <t>Equity Journey Continuum</t>
+  </si>
+  <si>
+    <t>Students taking one or more early college courses</t>
+  </si>
+  <si>
+    <t>K-12</t>
+  </si>
+  <si>
+    <t>% OF GRADUATES ENROLLED IN COMMUNITY COLLEGE REMEDIAL COURSES (SCHOOL)</t>
+  </si>
+  <si>
+    <t>Community College Remediation %</t>
+  </si>
+  <si>
+    <t>Community College Remediation Reading %</t>
+  </si>
+  <si>
+    <t>Community College Remediation Math %</t>
+  </si>
+  <si>
+    <t>Community College Remediation Communication</t>
+  </si>
+  <si>
+    <t>% Community College Remediation</t>
+  </si>
+  <si>
+    <t>% Community College Remediation - Reading</t>
+  </si>
+  <si>
+    <t>% Community College Remediation - Math</t>
+  </si>
+  <si>
+    <t>% Community College Remediation - Communication</t>
+  </si>
+  <si>
+    <t>% Graduates enrolled in a Postsecondary Institution within 12 months</t>
+  </si>
+  <si>
+    <t>% Graduates enrolled in a Postsecondary Institution within 12 months - Pubic Institition</t>
+  </si>
+  <si>
+    <t>% Graduates enrolled in a Postsecondary Institution within 12 months - Private Institution</t>
+  </si>
+  <si>
+    <t>% Graduates enrolled in a Postsecondary Institution within 12 months - Four-year Institution</t>
+  </si>
+  <si>
+    <t>% Graduates enrolled in a Postsecondary Institution within 12 months - Two-year Institution</t>
+  </si>
+  <si>
+    <t>% Graduates enrolled in a Postsecondary Institution within 12 months - Trade/Vocational School</t>
+  </si>
+  <si>
+    <t>% Graduates enrolled in a Postsecondary Institution within 16 months</t>
+  </si>
+  <si>
+    <t>% Graduates enrolled in a Postsecondary Institution within 16 months - Pubic Institition</t>
+  </si>
+  <si>
+    <t>% Graduates enrolled in a Postsecondary Institution within 16 months - Private Institution</t>
+  </si>
+  <si>
+    <t>% Graduates enrolled in a Postsecondary Institution within 16 months - Four-year Institution</t>
+  </si>
+  <si>
+    <t>% Graduates enrolled in a Postsecondary Institution within 16 months - Two-year Institution</t>
+  </si>
+  <si>
+    <t>% Graduates enrolled in a Postsecondary Institution within 16 months - Trade/Vocational School</t>
+  </si>
+  <si>
+    <t>% Graduates enrolled in a Postsecondary Institution within 12 months - Public Institition</t>
+  </si>
+  <si>
+    <t>% Graduates enrolled in a Postsecondary Institution within 16 months - Public Institition</t>
+  </si>
+  <si>
+    <t>% Graduates enrolled in Post Secondary Institution  within 16 months</t>
+  </si>
+  <si>
+    <t>% Graduates enrolled in Post Secondary Institution  within 12 months</t>
+  </si>
+  <si>
+    <t>% GRADUATES ENROLLED IN COLLEGE WITHIN 16 MONTHS - SCHOOL</t>
+  </si>
+  <si>
+    <t>% GRADUATES ENROLLED IN COLLEGE WITHIN 12 MONTHS - SCHOOL</t>
+  </si>
+  <si>
+    <t>student access to school counselors</t>
+  </si>
+  <si>
+    <t>National Comparisons</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>2016-2018</t>
+  </si>
+  <si>
+    <t>All "Coming Soon" metrics</t>
+  </si>
+  <si>
+    <t>2008-2016</t>
+  </si>
+  <si>
+    <t>CTE Enrollment vs. CTE Participation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>Career and Technical Education Enrollment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is a legacy measure that is the number of students who enrolled in at least one course that is state approved as a CTE course in at least one CIP, whether it was assigned by an EFE or not. A student is assigned to the last home school in which he/she was enrolled for the school year. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>Career and Technical Education Participant</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is a Grade 9 to 12 student who has enrolled in at least one CTE course during the school year and has a course outcome of Pass, Fail, or Incomplete</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1849,8 +2007,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1873,6 +2044,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC0E4F5"/>
         <bgColor rgb="FFC0E4F5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -1956,7 +2133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1980,11 +2157,23 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="139">
+  <dxfs count="156">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF6FAF4"/>
+          <bgColor rgb="FFF6FAF4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -2036,6 +2225,118 @@
           <color theme="4" tint="0.39997558519241921"/>
         </right>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3106,163 +3407,190 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}" name="Table1" displayName="Table1" ref="A1:EA17" totalsRowShown="0" dataDxfId="138">
-  <autoFilter ref="A1:EA17" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}" name="Table1" displayName="Table1" ref="A1:EQ17" totalsRowShown="0" dataDxfId="155">
+  <autoFilter ref="A1:EQ17" xr:uid="{B5918521-6A40-A04C-A021-2946602B8D6D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O17">
     <sortCondition ref="A1:A17"/>
   </sortState>
-  <tableColumns count="131">
-    <tableColumn id="1" xr3:uid="{6DA6945B-9D7D-0142-A374-7C4A97BBBBAB}" name="Year" dataDxfId="137"/>
-    <tableColumn id="2" xr3:uid="{1617EDAF-51CD-413F-9022-F6E4C97C233F}" name="RCDTS" dataDxfId="136"/>
-    <tableColumn id="3" xr3:uid="{A67D85A4-5303-744E-B7CD-31ECBC6CE0A7}" name="Type" dataDxfId="135"/>
-    <tableColumn id="13" xr3:uid="{C8F50192-B0A1-D84D-96D9-819955E9CE26}" name="District Type" dataDxfId="134"/>
-    <tableColumn id="14" xr3:uid="{A7661728-A363-9840-8182-CBC0352B14C6}" name="School Type" dataDxfId="133"/>
-    <tableColumn id="4" xr3:uid="{94336B41-A312-184A-9F00-C5E1720E28AF}" name="School Name" dataDxfId="132"/>
-    <tableColumn id="5" xr3:uid="{7516DA0D-E868-1941-B0D3-80B0E523A018}" name="District Name" dataDxfId="131"/>
-    <tableColumn id="10" xr3:uid="{DCD59F4B-C55C-2846-9070-7F8CC6CA2F51}" name="City" dataDxfId="130"/>
-    <tableColumn id="11" xr3:uid="{AB642454-853E-F049-84B7-745455B992F3}" name="County" dataDxfId="129"/>
-    <tableColumn id="9" xr3:uid="{5B5F7B45-CEFB-EE48-90E0-380BD11BD347}" name="Student Enrollment" dataDxfId="128"/>
-    <tableColumn id="6" xr3:uid="{DC5BC21C-5B26-D441-96D3-64D606494C9A}" name="Student Attendance Rate" dataDxfId="127"/>
-    <tableColumn id="7" xr3:uid="{16C5B399-2D53-AF41-815C-1F7C3259622D}" name="Student Chronic Truancy Rate" dataDxfId="126"/>
-    <tableColumn id="8" xr3:uid="{E3173650-9CBD-2046-9561-EC76593F21A4}" name="Chronic Absenteeism" dataDxfId="125"/>
-    <tableColumn id="12" xr3:uid="{A5C89E32-E6C7-354A-AD94-8B9E7BF5BEAF}" name="Total Teacher FTE" dataDxfId="124"/>
-    <tableColumn id="15" xr3:uid="{91CEEB72-10AD-5347-AD91-C2EA26951FFD}" name="Teacher Retention Rate" dataDxfId="123"/>
-    <tableColumn id="16" xr3:uid="{B95926A8-CE9E-5E4C-8517-F53E1DD6BB12}" name="Pupil Teacher Ratio - Elementary" dataDxfId="122"/>
-    <tableColumn id="17" xr3:uid="{66E6EF1B-5F71-724F-BE1B-2EAE768FA6E4}" name="Pupil Teacher Ratio - High School" dataDxfId="121"/>
-    <tableColumn id="18" xr3:uid="{FF7C5CB9-8A3F-654A-AAC2-F90DDD57691C}" name="% Novice Teachers" dataDxfId="120"/>
-    <tableColumn id="21" xr3:uid="{14F53AE3-04FD-0049-9CD6-2E8BE716335E}" name="% Novice Teachers - High Poverty Schools" dataDxfId="119"/>
-    <tableColumn id="22" xr3:uid="{1A89C2C1-D5B1-D84E-AF9A-AFFF73A90C04}" name="% Novice Teachers - Low Poverty Schools" dataDxfId="118"/>
-    <tableColumn id="19" xr3:uid="{31BB3C4C-CD8A-9848-85A3-6A3A4A977857}" name="% 8th Grade Passing Algebra 1" dataDxfId="117"/>
-    <tableColumn id="20" xr3:uid="{7DC2CAA5-3B64-9C42-8E87-31C44668510E}" name="% 9th Grade on Track" dataDxfId="116"/>
-    <tableColumn id="23" xr3:uid="{AD3426F6-72EB-7A4F-BA71-66C2A3294CCF}" name="# 9th Grade on Track" dataDxfId="115"/>
-    <tableColumn id="24" xr3:uid="{7124EEF3-D182-7A4B-A827-DEC5EE0B1591}" name="# CTE Enrollment" dataDxfId="114"/>
-    <tableColumn id="25" xr3:uid="{0206B422-7E9A-AF41-A20D-0A4445D084F7}" name="# CTE Participants" dataDxfId="113"/>
-    <tableColumn id="26" xr3:uid="{74152CBC-6192-FA44-8D72-64E4E7284B17}" name="4-Year Graduation Rate (Perkins)" dataDxfId="112"/>
-    <tableColumn id="27" xr3:uid="{E91D57BE-E786-0E41-A6C9-D40C584A25B7}" name="Postsecondary Placement Rate (Perkins)" dataDxfId="111"/>
-    <tableColumn id="28" xr3:uid="{61C1EAC6-2067-F84E-B17C-A8B628C30DA0}" name="Nontraditional Program Enrollment Rate (Perkins)" dataDxfId="110"/>
-    <tableColumn id="29" xr3:uid="{612816CA-7F21-1C4E-9A0F-5C68D82ADF7D}" name="# Students who took Dual Credit classes Grade 9" dataDxfId="109"/>
-    <tableColumn id="30" xr3:uid="{5753F583-62B9-8A44-A3EC-546C676CE502}" name="# Students who took Dual Credit classes Grade 10" dataDxfId="108"/>
-    <tableColumn id="31" xr3:uid="{99388DA0-03B4-324C-93D0-00C4E7DFFD44}" name="# Students who took Dual Credit classes Grade 11" dataDxfId="107"/>
-    <tableColumn id="32" xr3:uid="{100FC056-2E22-0C4B-9AAC-CCBAF3958BB5}" name="# Students who took Dual Credit classes Grade 12" dataDxfId="106"/>
-    <tableColumn id="33" xr3:uid="{7148123E-CBBF-7A4C-A783-2B28AF22F11E}" name="# Students enrolled in Dual Credit Coursework" dataDxfId="105"/>
-    <tableColumn id="34" xr3:uid="{9282E612-FE85-D14F-B5B4-F790B296E915}" name="% Students enrolled in Dual Credit Coursework" dataDxfId="104"/>
-    <tableColumn id="35" xr3:uid="{62431BD2-7051-FC48-BD9B-525CBF545DDD}" name="# Students who took AP classes Grade 9" dataDxfId="103"/>
-    <tableColumn id="36" xr3:uid="{73C469BE-B611-0145-B886-AAA2CB70EAE8}" name="# Students who took AP classes Grade 10" dataDxfId="102"/>
-    <tableColumn id="37" xr3:uid="{CFE88FEF-98CA-654A-B3B8-05790EA4E553}" name="# Students who took AP classes Grade 11" dataDxfId="101"/>
-    <tableColumn id="38" xr3:uid="{CB531B3F-8204-2644-91D3-88ACB4BFD0A7}" name="# Students who took AP classes Grade 12" dataDxfId="100"/>
-    <tableColumn id="39" xr3:uid="{97ED4799-6B71-FF44-A7E9-0D6FEC826075}" name="# Students who took IB classes Grade 9" dataDxfId="99"/>
-    <tableColumn id="40" xr3:uid="{F30102B8-881A-CA42-88CE-89D1D66A2AFB}" name="# Students who took IB classes Grade 10" dataDxfId="98"/>
-    <tableColumn id="41" xr3:uid="{99E2E959-F950-414B-BBF3-82CF023E0766}" name="# Students who took IB classes Grade 11" dataDxfId="97"/>
-    <tableColumn id="42" xr3:uid="{E9437747-1EEE-D94C-8B2E-5EB4508C3746}" name="# Students who took IB classes Grade 12" dataDxfId="96"/>
-    <tableColumn id="43" xr3:uid="{3CBA554F-964A-B546-B1CB-F3FFBC958E43}" name="# Out-of-Field Teachers" dataDxfId="95"/>
-    <tableColumn id="44" xr3:uid="{C4CCD547-D042-A040-8E97-CD2FA1F749A9}" name="% Out-of-Field Teachers" dataDxfId="94"/>
+  <tableColumns count="147">
+    <tableColumn id="1" xr3:uid="{6DA6945B-9D7D-0142-A374-7C4A97BBBBAB}" name="Year" dataDxfId="154"/>
+    <tableColumn id="2" xr3:uid="{1617EDAF-51CD-413F-9022-F6E4C97C233F}" name="RCDTS" dataDxfId="153"/>
+    <tableColumn id="3" xr3:uid="{A67D85A4-5303-744E-B7CD-31ECBC6CE0A7}" name="Type" dataDxfId="152"/>
+    <tableColumn id="13" xr3:uid="{C8F50192-B0A1-D84D-96D9-819955E9CE26}" name="District Type" dataDxfId="151"/>
+    <tableColumn id="14" xr3:uid="{A7661728-A363-9840-8182-CBC0352B14C6}" name="School Type" dataDxfId="150"/>
+    <tableColumn id="4" xr3:uid="{94336B41-A312-184A-9F00-C5E1720E28AF}" name="School Name" dataDxfId="149"/>
+    <tableColumn id="5" xr3:uid="{7516DA0D-E868-1941-B0D3-80B0E523A018}" name="District Name" dataDxfId="148"/>
+    <tableColumn id="10" xr3:uid="{DCD59F4B-C55C-2846-9070-7F8CC6CA2F51}" name="City" dataDxfId="147"/>
+    <tableColumn id="11" xr3:uid="{AB642454-853E-F049-84B7-745455B992F3}" name="County" dataDxfId="146"/>
+    <tableColumn id="9" xr3:uid="{5B5F7B45-CEFB-EE48-90E0-380BD11BD347}" name="Student Enrollment" dataDxfId="145"/>
+    <tableColumn id="6" xr3:uid="{DC5BC21C-5B26-D441-96D3-64D606494C9A}" name="Student Attendance Rate" dataDxfId="144"/>
+    <tableColumn id="7" xr3:uid="{16C5B399-2D53-AF41-815C-1F7C3259622D}" name="Student Chronic Truancy Rate" dataDxfId="143"/>
+    <tableColumn id="8" xr3:uid="{E3173650-9CBD-2046-9561-EC76593F21A4}" name="Chronic Absenteeism" dataDxfId="142"/>
+    <tableColumn id="12" xr3:uid="{A5C89E32-E6C7-354A-AD94-8B9E7BF5BEAF}" name="Total Teacher FTE" dataDxfId="141"/>
+    <tableColumn id="15" xr3:uid="{91CEEB72-10AD-5347-AD91-C2EA26951FFD}" name="Teacher Retention Rate" dataDxfId="140"/>
+    <tableColumn id="16" xr3:uid="{B95926A8-CE9E-5E4C-8517-F53E1DD6BB12}" name="Pupil Teacher Ratio - Elementary" dataDxfId="139"/>
+    <tableColumn id="17" xr3:uid="{66E6EF1B-5F71-724F-BE1B-2EAE768FA6E4}" name="Pupil Teacher Ratio - High School" dataDxfId="138"/>
+    <tableColumn id="18" xr3:uid="{FF7C5CB9-8A3F-654A-AAC2-F90DDD57691C}" name="% Novice Teachers" dataDxfId="137"/>
+    <tableColumn id="21" xr3:uid="{14F53AE3-04FD-0049-9CD6-2E8BE716335E}" name="% Novice Teachers - High Poverty Schools" dataDxfId="136"/>
+    <tableColumn id="22" xr3:uid="{1A89C2C1-D5B1-D84E-AF9A-AFFF73A90C04}" name="% Novice Teachers - Low Poverty Schools" dataDxfId="135"/>
+    <tableColumn id="19" xr3:uid="{31BB3C4C-CD8A-9848-85A3-6A3A4A977857}" name="% 8th Grade Passing Algebra 1" dataDxfId="134"/>
+    <tableColumn id="20" xr3:uid="{7DC2CAA5-3B64-9C42-8E87-31C44668510E}" name="% 9th Grade on Track" dataDxfId="133"/>
+    <tableColumn id="23" xr3:uid="{AD3426F6-72EB-7A4F-BA71-66C2A3294CCF}" name="# 9th Grade on Track" dataDxfId="132"/>
+    <tableColumn id="24" xr3:uid="{7124EEF3-D182-7A4B-A827-DEC5EE0B1591}" name="# CTE Enrollment" dataDxfId="131"/>
+    <tableColumn id="25" xr3:uid="{0206B422-7E9A-AF41-A20D-0A4445D084F7}" name="# CTE Participants" dataDxfId="130"/>
+    <tableColumn id="26" xr3:uid="{74152CBC-6192-FA44-8D72-64E4E7284B17}" name="4-Year Graduation Rate (Perkins)" dataDxfId="129"/>
+    <tableColumn id="27" xr3:uid="{E91D57BE-E786-0E41-A6C9-D40C584A25B7}" name="Postsecondary Placement Rate (Perkins)" dataDxfId="128"/>
+    <tableColumn id="28" xr3:uid="{61C1EAC6-2067-F84E-B17C-A8B628C30DA0}" name="Nontraditional Program Enrollment Rate (Perkins)" dataDxfId="127"/>
+    <tableColumn id="29" xr3:uid="{612816CA-7F21-1C4E-9A0F-5C68D82ADF7D}" name="# Students who took Dual Credit classes Grade 9" dataDxfId="126"/>
+    <tableColumn id="30" xr3:uid="{5753F583-62B9-8A44-A3EC-546C676CE502}" name="# Students who took Dual Credit classes Grade 10" dataDxfId="125"/>
+    <tableColumn id="31" xr3:uid="{99388DA0-03B4-324C-93D0-00C4E7DFFD44}" name="# Students who took Dual Credit classes Grade 11" dataDxfId="124"/>
+    <tableColumn id="32" xr3:uid="{100FC056-2E22-0C4B-9AAC-CCBAF3958BB5}" name="# Students who took Dual Credit classes Grade 12" dataDxfId="123"/>
+    <tableColumn id="33" xr3:uid="{7148123E-CBBF-7A4C-A783-2B28AF22F11E}" name="# Students enrolled in Dual Credit Coursework" dataDxfId="122"/>
+    <tableColumn id="34" xr3:uid="{9282E612-FE85-D14F-B5B4-F790B296E915}" name="% Students enrolled in Dual Credit Coursework" dataDxfId="121"/>
+    <tableColumn id="35" xr3:uid="{62431BD2-7051-FC48-BD9B-525CBF545DDD}" name="# Students who took AP classes Grade 9" dataDxfId="120"/>
+    <tableColumn id="36" xr3:uid="{73C469BE-B611-0145-B886-AAA2CB70EAE8}" name="# Students who took AP classes Grade 10" dataDxfId="119"/>
+    <tableColumn id="37" xr3:uid="{CFE88FEF-98CA-654A-B3B8-05790EA4E553}" name="# Students who took AP classes Grade 11" dataDxfId="118"/>
+    <tableColumn id="38" xr3:uid="{CB531B3F-8204-2644-91D3-88ACB4BFD0A7}" name="# Students who took AP classes Grade 12" dataDxfId="117"/>
+    <tableColumn id="39" xr3:uid="{97ED4799-6B71-FF44-A7E9-0D6FEC826075}" name="# Students who took IB classes Grade 9" dataDxfId="116"/>
+    <tableColumn id="40" xr3:uid="{F30102B8-881A-CA42-88CE-89D1D66A2AFB}" name="# Students who took IB classes Grade 10" dataDxfId="115"/>
+    <tableColumn id="41" xr3:uid="{99E2E959-F950-414B-BBF3-82CF023E0766}" name="# Students who took IB classes Grade 11" dataDxfId="114"/>
+    <tableColumn id="42" xr3:uid="{E9437747-1EEE-D94C-8B2E-5EB4508C3746}" name="# Students who took IB classes Grade 12" dataDxfId="113"/>
+    <tableColumn id="43" xr3:uid="{3CBA554F-964A-B546-B1CB-F3FFBC958E43}" name="# Out-of-Field Teachers" dataDxfId="112"/>
+    <tableColumn id="44" xr3:uid="{C4CCD547-D042-A040-8E97-CD2FA1F749A9}" name="% Out-of-Field Teachers" dataDxfId="111"/>
     <tableColumn id="62" xr3:uid="{5293548B-85DC-4D43-B151-9861D89C3752}" name="# Out-of-Field Teachers - High Poverty Schools"/>
     <tableColumn id="63" xr3:uid="{D2C92466-3D16-2D4B-A12B-9A8ABB3ED364}" name="% Out-of-Field Teachers - High Poverty Schools"/>
-    <tableColumn id="64" xr3:uid="{0F0B2BE2-813C-4144-812C-BE2D5CAF20F8}" name="# Out-of-Field Teachers - Low Poverty Schools" dataDxfId="93"/>
-    <tableColumn id="65" xr3:uid="{FFA97492-5178-024F-ABCD-F128D0C3C118}" name="% Out-of-Field Teachers - Low Poverty Schools" dataDxfId="92"/>
-    <tableColumn id="45" xr3:uid="{DC129293-5D55-4C48-A979-6304ABE3CAB9}" name="% Teachers with Short-Term or Provisional License" dataDxfId="91"/>
-    <tableColumn id="46" xr3:uid="{69922C1F-B1F6-AA41-8916-728215E1A659}" name="% Teachers with Short-Term or Provisional License - High Poverty Schools" dataDxfId="90"/>
-    <tableColumn id="47" xr3:uid="{CB9F66DB-18B6-4A41-A560-2737C375BEAA}" name="% Teachers with Short-Term or Provisional License - Low Poverty Schools" dataDxfId="89"/>
-    <tableColumn id="48" xr3:uid="{FA593E29-37FA-2F49-B1E2-8A20B24707C0}" name="# Teachers with Short-Term or Provisional License - High Poverty Schools" dataDxfId="88"/>
-    <tableColumn id="49" xr3:uid="{F17AD799-AAF2-CA4B-9052-79526ED68F55}" name="# Teachers with Short-Term or Provisional License - Low Poverty Schools" dataDxfId="87"/>
-    <tableColumn id="50" xr3:uid="{95D43F71-6E78-7545-8A4C-AE8258AA92BA}" name="Teacher Attendance Rate" dataDxfId="86"/>
-    <tableColumn id="51" xr3:uid="{35904462-8ACF-104B-8595-F9EDDB9D005D}" name="Principal Turnover within 6 Years" dataDxfId="85"/>
-    <tableColumn id="52" xr3:uid="{37C54579-1382-4047-B32E-9B6DCF4C6D1A}" name="High School 4-Year Graduation Rate" dataDxfId="84"/>
-    <tableColumn id="53" xr3:uid="{76C7C142-3803-C743-ACB8-2AC253A56510}" name="High School 6-Year Graduation Rate" dataDxfId="83"/>
-    <tableColumn id="54" xr3:uid="{D57E1850-D7FE-9141-B5FF-8D139A17D39D}" name="Number of students who took one or more AP Exams Grade 9" dataDxfId="82"/>
-    <tableColumn id="55" xr3:uid="{D85884E7-853A-2E46-93D7-579975E2D930}" name="Number of students who passed one or more AP Exams Grade 9" dataDxfId="81"/>
-    <tableColumn id="56" xr3:uid="{24D843C3-F6B3-4A48-8E47-DCCC0C37AB56}" name="Number of students who took one or more AP Exams Grade 10" dataDxfId="80"/>
-    <tableColumn id="57" xr3:uid="{C1215080-ECBF-3A40-951A-7496839DDC04}" name="Number of students who passed one or more AP Exams Grade 10" dataDxfId="79"/>
-    <tableColumn id="58" xr3:uid="{5305A7BA-20A4-B64A-BEE0-7EBE5CA1285E}" name="Number of students who took one or more AP Exams Grade 11" dataDxfId="78"/>
-    <tableColumn id="59" xr3:uid="{95397CC1-7B04-4B4A-A1EE-AB2A5546B55E}" name="Number of students who passed one or more AP Exams Grade 11" dataDxfId="77"/>
-    <tableColumn id="60" xr3:uid="{09F63790-ADCE-6E4A-A471-0A5D1D8214A2}" name="Number of students who took one or more AP Exams Grade 12" dataDxfId="76"/>
-    <tableColumn id="61" xr3:uid="{EF07B6AA-C8A6-FC44-BFD2-653A0B6E2A86}" name="Number of students who passed one or more AP Exams Grade 12" dataDxfId="75"/>
-    <tableColumn id="66" xr3:uid="{AC007116-4637-644E-AF02-A7AB5D5EADD6}" name="% All students IAR ELA Level 1 - Grade 3" dataDxfId="74"/>
-    <tableColumn id="67" xr3:uid="{6DAFBA42-AD9C-E14A-96FB-288D8BCA99E7}" name="% All students IAR ELA Level 2 - Grade 3" dataDxfId="73"/>
-    <tableColumn id="68" xr3:uid="{2E7A55B0-50B2-1348-9EF5-E0436300315C}" name="% All students IAR ELA Level 3 - Grade 3" dataDxfId="72"/>
-    <tableColumn id="69" xr3:uid="{3B2446EE-A403-8149-8093-69085337F1D6}" name="% All students IAR ELA Level 4 - Grade 3" dataDxfId="71"/>
-    <tableColumn id="70" xr3:uid="{13CB50EE-75B6-AD43-9ED6-31F97F3DFE85}" name="% All students IAR ELA Level 5 - Grade 3" dataDxfId="70"/>
-    <tableColumn id="71" xr3:uid="{FB4CBEC1-BD67-ED47-BD98-9A65971E4BA9}" name="% All students IAR Mathematics Level 1 - Grade 3" dataDxfId="69"/>
-    <tableColumn id="72" xr3:uid="{BAF1E93D-139D-B94F-9700-0FD86F22AF28}" name="% All students IAR Mathematics Level 2 - Grade 3" dataDxfId="68"/>
-    <tableColumn id="73" xr3:uid="{7CD72569-ABF3-4646-B51A-2145BED1C25D}" name="% All students IAR Mathematics Level 3 - Grade 3" dataDxfId="67"/>
-    <tableColumn id="74" xr3:uid="{D6FD88CB-214D-6E43-946E-6311DA9131CC}" name="% All students IAR Mathematics Level 4 - Grade 3" dataDxfId="66"/>
-    <tableColumn id="75" xr3:uid="{9A177942-E27F-614F-B30D-3C3E30D447EE}" name="% All students IAR Mathematics Level 5 - Grade 3" dataDxfId="65"/>
-    <tableColumn id="76" xr3:uid="{F27CFC65-3F0D-7345-AC77-D090538A32D7}" name="% All students IAR ELA Level 1 - Grade 4" dataDxfId="64"/>
-    <tableColumn id="77" xr3:uid="{B4CD64F1-783A-0D4E-BB22-9AC26FC31535}" name="% All students IAR ELA Level 2 - Grade 4" dataDxfId="63"/>
-    <tableColumn id="78" xr3:uid="{3DDE4D53-B2E8-844E-B0CB-563F26DCCBAF}" name="% All students IAR ELA Level 3 - Grade 4" dataDxfId="62"/>
-    <tableColumn id="79" xr3:uid="{B4F28FE8-5C67-AA4A-961F-4637D4DA5263}" name="% All students IAR ELA Level 4 - Grade 4" dataDxfId="61"/>
-    <tableColumn id="80" xr3:uid="{3B600242-98E2-1D4E-9DAA-FDA6A4D0CAE7}" name="% All students IAR ELA Level 5 - Grade 4" dataDxfId="60"/>
-    <tableColumn id="81" xr3:uid="{93D0B95A-07C7-CA42-ADA3-F494E1E89CC6}" name="% All students IAR Mathematics Level 1 - Grade 4" dataDxfId="59"/>
-    <tableColumn id="82" xr3:uid="{DA3B88D8-9F1B-0D43-A00A-0E00A0E101E4}" name="% All students IAR Mathematics Level 2 - Grade 4" dataDxfId="58"/>
-    <tableColumn id="83" xr3:uid="{CFB9A658-C262-A24D-BDBC-A2FA6764B041}" name="% All students IAR Mathematics Level 3 - Grade 4" dataDxfId="57"/>
-    <tableColumn id="84" xr3:uid="{170D49FE-6CD9-2349-8C42-D35123081DAA}" name="% All students IAR Mathematics Level 4 - Grade 4" dataDxfId="56"/>
-    <tableColumn id="85" xr3:uid="{90D4AF95-5666-AA4E-896A-BEFE87C9CA9A}" name="% All students IAR Mathematics Level 5 - Grade 4" dataDxfId="55"/>
-    <tableColumn id="86" xr3:uid="{F01BCEF8-4268-804D-B91E-4DF5945E471F}" name="% All students IAR ELA Level 1 - Grade 5" dataDxfId="54"/>
-    <tableColumn id="87" xr3:uid="{3D948EEB-557F-D548-A8E8-483E928D37C0}" name="% All students IAR ELA Level 2 - Grade 5" dataDxfId="53"/>
-    <tableColumn id="88" xr3:uid="{046CB80A-00D6-5548-8953-4988F3849A8E}" name="% All students IAR ELA Level 3 - Grade 5" dataDxfId="52"/>
-    <tableColumn id="89" xr3:uid="{FD0B5F84-667C-7C4C-965B-B019DF711FFA}" name="% All students IAR ELA Level 4 - Grade 5" dataDxfId="51"/>
-    <tableColumn id="90" xr3:uid="{B280A1EC-2EEE-B94B-BB08-C9C8B4E61414}" name="% All students IAR ELA Level 5 - Grade 5" dataDxfId="50"/>
-    <tableColumn id="91" xr3:uid="{623688F4-27B9-6747-877A-5CD58CD88AD3}" name="% All students IAR Mathematics Level 1 - Grade 5" dataDxfId="49"/>
-    <tableColumn id="92" xr3:uid="{7B942C5F-3AA9-8D48-A248-FA33E13B784D}" name="% All students IAR Mathematics Level 2 - Grade 5" dataDxfId="48"/>
-    <tableColumn id="93" xr3:uid="{19970012-6DDA-3F4F-8C3E-18848326B806}" name="% All students IAR Mathematics Level 3 - Grade 5" dataDxfId="47"/>
-    <tableColumn id="94" xr3:uid="{580D40AB-E7AD-FE44-8761-A7AF851155D2}" name="% All students IAR Mathematics Level 4 - Grade 5" dataDxfId="46"/>
-    <tableColumn id="95" xr3:uid="{979CB1A3-9B4D-B140-A5C9-511186C63C1F}" name="% All students IAR Mathematics Level 5 - Grade 5" dataDxfId="45"/>
-    <tableColumn id="96" xr3:uid="{62252DFA-08F6-744C-9EF9-CFAAE16CF3EF}" name="% All students IAR ELA Level 1 - Grade 6" dataDxfId="44"/>
-    <tableColumn id="97" xr3:uid="{2BFED3F3-04A5-C141-97FF-8BFEAC349211}" name="% All students IAR ELA Level 2 - Grade 6" dataDxfId="43"/>
-    <tableColumn id="98" xr3:uid="{57BF687F-8D34-A241-92C4-151F13501BDA}" name="% All students IAR ELA Level 3 - Grade 6" dataDxfId="42"/>
-    <tableColumn id="99" xr3:uid="{0B1FAB00-E606-9A48-8F9B-1695CDA4141D}" name="% All students IAR ELA Level 4 - Grade 6" dataDxfId="41"/>
-    <tableColumn id="100" xr3:uid="{7CB31A98-CDE5-204A-B623-3FFD055EE8F7}" name="% All students IAR ELA Level 5 - Grade 6" dataDxfId="40"/>
-    <tableColumn id="101" xr3:uid="{905AE3BB-8EC2-2941-B07D-D10CA53C067C}" name="% All students IAR Mathematics Level 1 - Grade 6" dataDxfId="39"/>
-    <tableColumn id="102" xr3:uid="{A0E6A805-C151-3043-8AD6-9ECFC583B49D}" name="% All students IAR Mathematics Level 2 - Grade 6" dataDxfId="38"/>
-    <tableColumn id="103" xr3:uid="{8D82CF0D-C030-684A-8F41-EBF7273C86DC}" name="% All students IAR Mathematics Level 3 - Grade 6" dataDxfId="37"/>
-    <tableColumn id="104" xr3:uid="{8E92DDD0-DE8C-3A48-80BC-0CE584B61CDE}" name="% All students IAR Mathematics Level 4 - Grade 6" dataDxfId="36"/>
-    <tableColumn id="105" xr3:uid="{746F5E03-2EF7-6A45-957C-6217D5777E5C}" name="% All students IAR Mathematics Level 5 - Grade 6" dataDxfId="35"/>
-    <tableColumn id="106" xr3:uid="{1853EBFD-EE25-454A-A5C2-26503987C863}" name="% All students IAR ELA Level 1 - Grade 7" dataDxfId="34"/>
-    <tableColumn id="107" xr3:uid="{FF34E160-7F90-B249-B977-3F31414D9339}" name="% All students IAR ELA Level 2 - Grade 7" dataDxfId="33"/>
-    <tableColumn id="108" xr3:uid="{F5F03D9E-403D-6D47-9C82-225F85BA0BED}" name="% All students IAR ELA Level 3 - Grade 7" dataDxfId="32"/>
-    <tableColumn id="109" xr3:uid="{3E5AB0C7-8DDF-DA4D-BA96-0BD2DFA7F3CE}" name="% All students IAR ELA Level 4 - Grade 7" dataDxfId="31"/>
-    <tableColumn id="110" xr3:uid="{4623F40F-2BA1-2D44-926D-6E0E9E6F3FB6}" name="% All students IAR ELA Level 5 - Grade 7" dataDxfId="30"/>
-    <tableColumn id="111" xr3:uid="{4DD0BB9E-1366-0E41-9087-DACC5328CE35}" name="% All students IAR Mathematics Level 1 - Grade 7" dataDxfId="29"/>
-    <tableColumn id="112" xr3:uid="{51FA4D64-56A2-E740-9159-D9240599CA42}" name="% All students IAR Mathematics Level 2 - Grade 7" dataDxfId="28"/>
-    <tableColumn id="113" xr3:uid="{C31DA806-5B12-EC4F-A04D-3047FA120396}" name="% All students IAR Mathematics Level 3 - Grade 7" dataDxfId="27"/>
-    <tableColumn id="114" xr3:uid="{42BEADD7-CFCC-364A-A1C0-ED82BE268096}" name="% All students IAR Mathematics Level 4 - Grade 7" dataDxfId="26"/>
-    <tableColumn id="115" xr3:uid="{50F32122-C218-2848-9B5E-7B3FCF3F89E2}" name="% All students IAR Mathematics Level 5 - Grade 7" dataDxfId="25"/>
-    <tableColumn id="116" xr3:uid="{E359B9F7-D5AD-E349-A55F-38877DA01441}" name="% All students IAR ELA Level 1 - Grade 8" dataDxfId="24"/>
-    <tableColumn id="117" xr3:uid="{FD9292BF-E7B0-CD42-B60B-371D6D7EED97}" name="% All students IAR ELA Level 2 - Grade 8" dataDxfId="23"/>
-    <tableColumn id="118" xr3:uid="{3ECE2E11-420D-7A46-97EB-6D24DB8D1332}" name="% All students IAR ELA Level 3 - Grade 8" dataDxfId="22"/>
-    <tableColumn id="119" xr3:uid="{14FBB02E-019C-AF4C-9180-F1B3FA3CEC25}" name="% All students IAR ELA Level 4 - Grade 8" dataDxfId="21"/>
-    <tableColumn id="120" xr3:uid="{10A0A9E8-635A-854D-A028-98D894FEFFF2}" name="% All students IAR ELA Level 5 - Grade 8" dataDxfId="20"/>
-    <tableColumn id="121" xr3:uid="{F06B2FE3-9314-EC48-B76D-D29D98F93819}" name="% All students IAR Mathematics Level 1 - Grade 8" dataDxfId="19"/>
-    <tableColumn id="122" xr3:uid="{651BBD41-9898-A245-B250-1A0421718DFD}" name="% All students IAR Mathematics Level 2 - Grade 8" dataDxfId="18"/>
-    <tableColumn id="123" xr3:uid="{2D222852-7268-B148-94DE-2955439FC0D9}" name="% All students IAR Mathematics Level 3 - Grade 8" dataDxfId="17"/>
-    <tableColumn id="124" xr3:uid="{C55FA655-B4FA-B34D-BF96-7A4F914BC92D}" name="% All students IAR Mathematics Level 4 - Grade 8" dataDxfId="16"/>
-    <tableColumn id="125" xr3:uid="{70713A34-CC75-9A40-A064-F7B004C6C343}" name="% All students IAR Mathematics Level 5 - Grade 8" dataDxfId="15"/>
-    <tableColumn id="126" xr3:uid="{7E050A4E-1F41-9A40-B006-6ECAFD6B4D58}" name="# Students IAR Math Participation" dataDxfId="14"/>
-    <tableColumn id="127" xr3:uid="{A948F730-D175-A44A-9DFB-6527B8339E63}" name="% Students IAR Math Participation" dataDxfId="13"/>
-    <tableColumn id="128" xr3:uid="{5E037E5B-E65C-BE42-9FC4-08954641058A}" name="# Students IAR ELA Participation" dataDxfId="12"/>
-    <tableColumn id="129" xr3:uid="{26522368-F055-4447-AE58-9C126D1EA1C7}" name="% Students IAR ELA Participation" dataDxfId="11"/>
-    <tableColumn id="130" xr3:uid="{9B2AEA67-E6CC-CB45-83A8-8C23034BE63D}" name="IAR ELA No Participation Rate - Total" dataDxfId="10"/>
-    <tableColumn id="131" xr3:uid="{625AFF90-E4E5-034B-A879-E2B5760AC282}" name="IAR Math No Participation Rate - Total" dataDxfId="9"/>
+    <tableColumn id="64" xr3:uid="{0F0B2BE2-813C-4144-812C-BE2D5CAF20F8}" name="# Out-of-Field Teachers - Low Poverty Schools" dataDxfId="110"/>
+    <tableColumn id="65" xr3:uid="{FFA97492-5178-024F-ABCD-F128D0C3C118}" name="% Out-of-Field Teachers - Low Poverty Schools" dataDxfId="109"/>
+    <tableColumn id="45" xr3:uid="{DC129293-5D55-4C48-A979-6304ABE3CAB9}" name="% Teachers with Short-Term or Provisional License" dataDxfId="108"/>
+    <tableColumn id="46" xr3:uid="{69922C1F-B1F6-AA41-8916-728215E1A659}" name="% Teachers with Short-Term or Provisional License - High Poverty Schools" dataDxfId="107"/>
+    <tableColumn id="47" xr3:uid="{CB9F66DB-18B6-4A41-A560-2737C375BEAA}" name="% Teachers with Short-Term or Provisional License - Low Poverty Schools" dataDxfId="106"/>
+    <tableColumn id="48" xr3:uid="{FA593E29-37FA-2F49-B1E2-8A20B24707C0}" name="# Teachers with Short-Term or Provisional License - High Poverty Schools" dataDxfId="105"/>
+    <tableColumn id="49" xr3:uid="{F17AD799-AAF2-CA4B-9052-79526ED68F55}" name="# Teachers with Short-Term or Provisional License - Low Poverty Schools" dataDxfId="104"/>
+    <tableColumn id="50" xr3:uid="{95D43F71-6E78-7545-8A4C-AE8258AA92BA}" name="Teacher Attendance Rate" dataDxfId="103"/>
+    <tableColumn id="51" xr3:uid="{35904462-8ACF-104B-8595-F9EDDB9D005D}" name="Principal Turnover within 6 Years" dataDxfId="102"/>
+    <tableColumn id="52" xr3:uid="{37C54579-1382-4047-B32E-9B6DCF4C6D1A}" name="High School 4-Year Graduation Rate" dataDxfId="101"/>
+    <tableColumn id="53" xr3:uid="{76C7C142-3803-C743-ACB8-2AC253A56510}" name="High School 6-Year Graduation Rate" dataDxfId="100"/>
+    <tableColumn id="54" xr3:uid="{D57E1850-D7FE-9141-B5FF-8D139A17D39D}" name="Number of students who took one or more AP Exams Grade 9" dataDxfId="99"/>
+    <tableColumn id="55" xr3:uid="{D85884E7-853A-2E46-93D7-579975E2D930}" name="Number of students who passed one or more AP Exams Grade 9" dataDxfId="98"/>
+    <tableColumn id="56" xr3:uid="{24D843C3-F6B3-4A48-8E47-DCCC0C37AB56}" name="Number of students who took one or more AP Exams Grade 10" dataDxfId="97"/>
+    <tableColumn id="57" xr3:uid="{C1215080-ECBF-3A40-951A-7496839DDC04}" name="Number of students who passed one or more AP Exams Grade 10" dataDxfId="96"/>
+    <tableColumn id="58" xr3:uid="{5305A7BA-20A4-B64A-BEE0-7EBE5CA1285E}" name="Number of students who took one or more AP Exams Grade 11" dataDxfId="95"/>
+    <tableColumn id="59" xr3:uid="{95397CC1-7B04-4B4A-A1EE-AB2A5546B55E}" name="Number of students who passed one or more AP Exams Grade 11" dataDxfId="94"/>
+    <tableColumn id="60" xr3:uid="{09F63790-ADCE-6E4A-A471-0A5D1D8214A2}" name="Number of students who took one or more AP Exams Grade 12" dataDxfId="93"/>
+    <tableColumn id="61" xr3:uid="{EF07B6AA-C8A6-FC44-BFD2-653A0B6E2A86}" name="Number of students who passed one or more AP Exams Grade 12" dataDxfId="92"/>
+    <tableColumn id="66" xr3:uid="{AC007116-4637-644E-AF02-A7AB5D5EADD6}" name="% All students IAR ELA Level 1 - Grade 3" dataDxfId="91"/>
+    <tableColumn id="67" xr3:uid="{6DAFBA42-AD9C-E14A-96FB-288D8BCA99E7}" name="% All students IAR ELA Level 2 - Grade 3" dataDxfId="90"/>
+    <tableColumn id="68" xr3:uid="{2E7A55B0-50B2-1348-9EF5-E0436300315C}" name="% All students IAR ELA Level 3 - Grade 3" dataDxfId="89"/>
+    <tableColumn id="69" xr3:uid="{3B2446EE-A403-8149-8093-69085337F1D6}" name="% All students IAR ELA Level 4 - Grade 3" dataDxfId="88"/>
+    <tableColumn id="70" xr3:uid="{13CB50EE-75B6-AD43-9ED6-31F97F3DFE85}" name="% All students IAR ELA Level 5 - Grade 3" dataDxfId="87"/>
+    <tableColumn id="71" xr3:uid="{FB4CBEC1-BD67-ED47-BD98-9A65971E4BA9}" name="% All students IAR Mathematics Level 1 - Grade 3" dataDxfId="86"/>
+    <tableColumn id="72" xr3:uid="{BAF1E93D-139D-B94F-9700-0FD86F22AF28}" name="% All students IAR Mathematics Level 2 - Grade 3" dataDxfId="85"/>
+    <tableColumn id="73" xr3:uid="{7CD72569-ABF3-4646-B51A-2145BED1C25D}" name="% All students IAR Mathematics Level 3 - Grade 3" dataDxfId="84"/>
+    <tableColumn id="74" xr3:uid="{D6FD88CB-214D-6E43-946E-6311DA9131CC}" name="% All students IAR Mathematics Level 4 - Grade 3" dataDxfId="83"/>
+    <tableColumn id="75" xr3:uid="{9A177942-E27F-614F-B30D-3C3E30D447EE}" name="% All students IAR Mathematics Level 5 - Grade 3" dataDxfId="82"/>
+    <tableColumn id="76" xr3:uid="{F27CFC65-3F0D-7345-AC77-D090538A32D7}" name="% All students IAR ELA Level 1 - Grade 4" dataDxfId="81"/>
+    <tableColumn id="77" xr3:uid="{B4CD64F1-783A-0D4E-BB22-9AC26FC31535}" name="% All students IAR ELA Level 2 - Grade 4" dataDxfId="80"/>
+    <tableColumn id="78" xr3:uid="{3DDE4D53-B2E8-844E-B0CB-563F26DCCBAF}" name="% All students IAR ELA Level 3 - Grade 4" dataDxfId="79"/>
+    <tableColumn id="79" xr3:uid="{B4F28FE8-5C67-AA4A-961F-4637D4DA5263}" name="% All students IAR ELA Level 4 - Grade 4" dataDxfId="78"/>
+    <tableColumn id="80" xr3:uid="{3B600242-98E2-1D4E-9DAA-FDA6A4D0CAE7}" name="% All students IAR ELA Level 5 - Grade 4" dataDxfId="77"/>
+    <tableColumn id="81" xr3:uid="{93D0B95A-07C7-CA42-ADA3-F494E1E89CC6}" name="% All students IAR Mathematics Level 1 - Grade 4" dataDxfId="76"/>
+    <tableColumn id="82" xr3:uid="{DA3B88D8-9F1B-0D43-A00A-0E00A0E101E4}" name="% All students IAR Mathematics Level 2 - Grade 4" dataDxfId="75"/>
+    <tableColumn id="83" xr3:uid="{CFB9A658-C262-A24D-BDBC-A2FA6764B041}" name="% All students IAR Mathematics Level 3 - Grade 4" dataDxfId="74"/>
+    <tableColumn id="84" xr3:uid="{170D49FE-6CD9-2349-8C42-D35123081DAA}" name="% All students IAR Mathematics Level 4 - Grade 4" dataDxfId="73"/>
+    <tableColumn id="85" xr3:uid="{90D4AF95-5666-AA4E-896A-BEFE87C9CA9A}" name="% All students IAR Mathematics Level 5 - Grade 4" dataDxfId="72"/>
+    <tableColumn id="86" xr3:uid="{F01BCEF8-4268-804D-B91E-4DF5945E471F}" name="% All students IAR ELA Level 1 - Grade 5" dataDxfId="71"/>
+    <tableColumn id="87" xr3:uid="{3D948EEB-557F-D548-A8E8-483E928D37C0}" name="% All students IAR ELA Level 2 - Grade 5" dataDxfId="70"/>
+    <tableColumn id="88" xr3:uid="{046CB80A-00D6-5548-8953-4988F3849A8E}" name="% All students IAR ELA Level 3 - Grade 5" dataDxfId="69"/>
+    <tableColumn id="89" xr3:uid="{FD0B5F84-667C-7C4C-965B-B019DF711FFA}" name="% All students IAR ELA Level 4 - Grade 5" dataDxfId="68"/>
+    <tableColumn id="90" xr3:uid="{B280A1EC-2EEE-B94B-BB08-C9C8B4E61414}" name="% All students IAR ELA Level 5 - Grade 5" dataDxfId="67"/>
+    <tableColumn id="91" xr3:uid="{623688F4-27B9-6747-877A-5CD58CD88AD3}" name="% All students IAR Mathematics Level 1 - Grade 5" dataDxfId="66"/>
+    <tableColumn id="92" xr3:uid="{7B942C5F-3AA9-8D48-A248-FA33E13B784D}" name="% All students IAR Mathematics Level 2 - Grade 5" dataDxfId="65"/>
+    <tableColumn id="93" xr3:uid="{19970012-6DDA-3F4F-8C3E-18848326B806}" name="% All students IAR Mathematics Level 3 - Grade 5" dataDxfId="64"/>
+    <tableColumn id="94" xr3:uid="{580D40AB-E7AD-FE44-8761-A7AF851155D2}" name="% All students IAR Mathematics Level 4 - Grade 5" dataDxfId="63"/>
+    <tableColumn id="95" xr3:uid="{979CB1A3-9B4D-B140-A5C9-511186C63C1F}" name="% All students IAR Mathematics Level 5 - Grade 5" dataDxfId="62"/>
+    <tableColumn id="96" xr3:uid="{62252DFA-08F6-744C-9EF9-CFAAE16CF3EF}" name="% All students IAR ELA Level 1 - Grade 6" dataDxfId="61"/>
+    <tableColumn id="97" xr3:uid="{2BFED3F3-04A5-C141-97FF-8BFEAC349211}" name="% All students IAR ELA Level 2 - Grade 6" dataDxfId="60"/>
+    <tableColumn id="98" xr3:uid="{57BF687F-8D34-A241-92C4-151F13501BDA}" name="% All students IAR ELA Level 3 - Grade 6" dataDxfId="59"/>
+    <tableColumn id="99" xr3:uid="{0B1FAB00-E606-9A48-8F9B-1695CDA4141D}" name="% All students IAR ELA Level 4 - Grade 6" dataDxfId="58"/>
+    <tableColumn id="100" xr3:uid="{7CB31A98-CDE5-204A-B623-3FFD055EE8F7}" name="% All students IAR ELA Level 5 - Grade 6" dataDxfId="57"/>
+    <tableColumn id="101" xr3:uid="{905AE3BB-8EC2-2941-B07D-D10CA53C067C}" name="% All students IAR Mathematics Level 1 - Grade 6" dataDxfId="56"/>
+    <tableColumn id="102" xr3:uid="{A0E6A805-C151-3043-8AD6-9ECFC583B49D}" name="% All students IAR Mathematics Level 2 - Grade 6" dataDxfId="55"/>
+    <tableColumn id="103" xr3:uid="{8D82CF0D-C030-684A-8F41-EBF7273C86DC}" name="% All students IAR Mathematics Level 3 - Grade 6" dataDxfId="54"/>
+    <tableColumn id="104" xr3:uid="{8E92DDD0-DE8C-3A48-80BC-0CE584B61CDE}" name="% All students IAR Mathematics Level 4 - Grade 6" dataDxfId="53"/>
+    <tableColumn id="105" xr3:uid="{746F5E03-2EF7-6A45-957C-6217D5777E5C}" name="% All students IAR Mathematics Level 5 - Grade 6" dataDxfId="52"/>
+    <tableColumn id="106" xr3:uid="{1853EBFD-EE25-454A-A5C2-26503987C863}" name="% All students IAR ELA Level 1 - Grade 7" dataDxfId="51"/>
+    <tableColumn id="107" xr3:uid="{FF34E160-7F90-B249-B977-3F31414D9339}" name="% All students IAR ELA Level 2 - Grade 7" dataDxfId="50"/>
+    <tableColumn id="108" xr3:uid="{F5F03D9E-403D-6D47-9C82-225F85BA0BED}" name="% All students IAR ELA Level 3 - Grade 7" dataDxfId="49"/>
+    <tableColumn id="109" xr3:uid="{3E5AB0C7-8DDF-DA4D-BA96-0BD2DFA7F3CE}" name="% All students IAR ELA Level 4 - Grade 7" dataDxfId="48"/>
+    <tableColumn id="110" xr3:uid="{4623F40F-2BA1-2D44-926D-6E0E9E6F3FB6}" name="% All students IAR ELA Level 5 - Grade 7" dataDxfId="47"/>
+    <tableColumn id="111" xr3:uid="{4DD0BB9E-1366-0E41-9087-DACC5328CE35}" name="% All students IAR Mathematics Level 1 - Grade 7" dataDxfId="46"/>
+    <tableColumn id="112" xr3:uid="{51FA4D64-56A2-E740-9159-D9240599CA42}" name="% All students IAR Mathematics Level 2 - Grade 7" dataDxfId="45"/>
+    <tableColumn id="113" xr3:uid="{C31DA806-5B12-EC4F-A04D-3047FA120396}" name="% All students IAR Mathematics Level 3 - Grade 7" dataDxfId="44"/>
+    <tableColumn id="114" xr3:uid="{42BEADD7-CFCC-364A-A1C0-ED82BE268096}" name="% All students IAR Mathematics Level 4 - Grade 7" dataDxfId="43"/>
+    <tableColumn id="115" xr3:uid="{50F32122-C218-2848-9B5E-7B3FCF3F89E2}" name="% All students IAR Mathematics Level 5 - Grade 7" dataDxfId="42"/>
+    <tableColumn id="116" xr3:uid="{E359B9F7-D5AD-E349-A55F-38877DA01441}" name="% All students IAR ELA Level 1 - Grade 8" dataDxfId="41"/>
+    <tableColumn id="117" xr3:uid="{FD9292BF-E7B0-CD42-B60B-371D6D7EED97}" name="% All students IAR ELA Level 2 - Grade 8" dataDxfId="40"/>
+    <tableColumn id="118" xr3:uid="{3ECE2E11-420D-7A46-97EB-6D24DB8D1332}" name="% All students IAR ELA Level 3 - Grade 8" dataDxfId="39"/>
+    <tableColumn id="119" xr3:uid="{14FBB02E-019C-AF4C-9180-F1B3FA3CEC25}" name="% All students IAR ELA Level 4 - Grade 8" dataDxfId="38"/>
+    <tableColumn id="120" xr3:uid="{10A0A9E8-635A-854D-A028-98D894FEFFF2}" name="% All students IAR ELA Level 5 - Grade 8" dataDxfId="37"/>
+    <tableColumn id="121" xr3:uid="{F06B2FE3-9314-EC48-B76D-D29D98F93819}" name="% All students IAR Mathematics Level 1 - Grade 8" dataDxfId="36"/>
+    <tableColumn id="122" xr3:uid="{651BBD41-9898-A245-B250-1A0421718DFD}" name="% All students IAR Mathematics Level 2 - Grade 8" dataDxfId="35"/>
+    <tableColumn id="123" xr3:uid="{2D222852-7268-B148-94DE-2955439FC0D9}" name="% All students IAR Mathematics Level 3 - Grade 8" dataDxfId="34"/>
+    <tableColumn id="124" xr3:uid="{C55FA655-B4FA-B34D-BF96-7A4F914BC92D}" name="% All students IAR Mathematics Level 4 - Grade 8" dataDxfId="33"/>
+    <tableColumn id="125" xr3:uid="{70713A34-CC75-9A40-A064-F7B004C6C343}" name="% All students IAR Mathematics Level 5 - Grade 8" dataDxfId="32"/>
+    <tableColumn id="126" xr3:uid="{7E050A4E-1F41-9A40-B006-6ECAFD6B4D58}" name="# Students IAR Math Participation" dataDxfId="31"/>
+    <tableColumn id="127" xr3:uid="{A948F730-D175-A44A-9DFB-6527B8339E63}" name="% Students IAR Math Participation" dataDxfId="30"/>
+    <tableColumn id="128" xr3:uid="{5E037E5B-E65C-BE42-9FC4-08954641058A}" name="# Students IAR ELA Participation" dataDxfId="29"/>
+    <tableColumn id="129" xr3:uid="{26522368-F055-4447-AE58-9C126D1EA1C7}" name="% Students IAR ELA Participation" dataDxfId="28"/>
+    <tableColumn id="130" xr3:uid="{9B2AEA67-E6CC-CB45-83A8-8C23034BE63D}" name="IAR ELA No Participation Rate" dataDxfId="27"/>
+    <tableColumn id="131" xr3:uid="{625AFF90-E4E5-034B-A879-E2B5760AC282}" name="IAR Math No Participation Rate" dataDxfId="26"/>
+    <tableColumn id="132" xr3:uid="{29B89C6C-9339-404A-AF82-DB0D3A222F3F}" name="% Community College Remediation" dataDxfId="25"/>
+    <tableColumn id="133" xr3:uid="{DBC9D35A-12A7-024D-AD84-BAE3D1E852F5}" name="% Community College Remediation - Reading" dataDxfId="24"/>
+    <tableColumn id="134" xr3:uid="{F16A3308-5B9F-5C49-BC36-E58E6F759587}" name="% Community College Remediation - Math" dataDxfId="23"/>
+    <tableColumn id="135" xr3:uid="{EBD68FC6-33A5-0449-9DDE-ED4341B71BBC}" name="% Community College Remediation - Communication" dataDxfId="22"/>
+    <tableColumn id="136" xr3:uid="{7677EA77-55C0-6340-A86D-25BCFB0B1AD7}" name="% Graduates enrolled in a Postsecondary Institution within 12 months" dataDxfId="21"/>
+    <tableColumn id="137" xr3:uid="{754A2BDC-3313-CE40-9F3F-2BD573EA75EB}" name="% Graduates enrolled in a Postsecondary Institution within 12 months - Public Institition" dataDxfId="20"/>
+    <tableColumn id="138" xr3:uid="{B198F225-9C72-564B-AD78-59AB07AFA5D8}" name="% Graduates enrolled in a Postsecondary Institution within 12 months - Private Institution" dataDxfId="19"/>
+    <tableColumn id="139" xr3:uid="{874B7093-79B7-984C-936B-FE7084604594}" name="% Graduates enrolled in a Postsecondary Institution within 12 months - Four-year Institution" dataDxfId="18"/>
+    <tableColumn id="140" xr3:uid="{B4DF4D71-019B-8A46-9A8B-5654791E6C34}" name="% Graduates enrolled in a Postsecondary Institution within 12 months - Two-year Institution" dataDxfId="17"/>
+    <tableColumn id="141" xr3:uid="{189D99CA-793F-634D-A81E-7155132D48C2}" name="% Graduates enrolled in a Postsecondary Institution within 12 months - Trade/Vocational School" dataDxfId="16"/>
+    <tableColumn id="142" xr3:uid="{57A98670-CF80-EA41-844D-B0365140F834}" name="% Graduates enrolled in a Postsecondary Institution within 16 months" dataDxfId="15"/>
+    <tableColumn id="143" xr3:uid="{CEA01699-9998-2B44-999D-252443994649}" name="% Graduates enrolled in a Postsecondary Institution within 16 months - Public Institition" dataDxfId="14"/>
+    <tableColumn id="144" xr3:uid="{772E6547-222F-3E4B-9068-1C3A9D1A53C8}" name="% Graduates enrolled in a Postsecondary Institution within 16 months - Private Institution" dataDxfId="13"/>
+    <tableColumn id="145" xr3:uid="{86412A3B-196A-4841-9A44-312EF6D68C3E}" name="% Graduates enrolled in a Postsecondary Institution within 16 months - Four-year Institution" dataDxfId="12"/>
+    <tableColumn id="146" xr3:uid="{E38AABD2-67F1-964D-BED3-9330423809BA}" name="% Graduates enrolled in a Postsecondary Institution within 16 months - Two-year Institution" dataDxfId="11"/>
+    <tableColumn id="147" xr3:uid="{0C630235-9E1C-A045-9C59-D9DCEAF08337}" name="% Graduates enrolled in a Postsecondary Institution within 16 months - Trade/Vocational School" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}" name="Table44" displayName="Table44" ref="A1:H794" totalsRowShown="0" dataDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="A1:H794" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}" name="Table44" displayName="Table44" ref="A1:H890" totalsRowShown="0" dataDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="A1:H890" xr:uid="{AD1B13A2-FA47-5D4B-9EA5-39ACC7EE5058}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H323">
     <sortCondition ref="B1:B323"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{CF003222-4DDE-BB47-A657-1775812A7CF9}" name="Year" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{75198FC7-15E7-C749-9856-FF87007012FD}" name="Metric" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{250849D7-E98C-6047-AD29-C748E7E94296}" name="Original Metric" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{2B055042-83EA-3F40-9F97-2E2C80BE4FCE}" name="Sheet" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{FCF3CEDF-90EF-DD4A-BD7C-2C3BB2D372C6}" name="Disaggregated" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{E905735F-4B71-1A4E-AA00-10B4AAD2B5F6}" name="Disaggregation Details" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{CF003222-4DDE-BB47-A657-1775812A7CF9}" name="Year" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{75198FC7-15E7-C749-9856-FF87007012FD}" name="Metric" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{250849D7-E98C-6047-AD29-C748E7E94296}" name="Original Metric" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{2B055042-83EA-3F40-9F97-2E2C80BE4FCE}" name="Sheet" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{FCF3CEDF-90EF-DD4A-BD7C-2C3BB2D372C6}" name="Disaggregated" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{E905735F-4B71-1A4E-AA00-10B4AAD2B5F6}" name="Disaggregation Details" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{6FC8DE02-1AAB-8248-8E52-B299C7FFB44A}" name="Disaggregation Format"/>
-    <tableColumn id="6" xr3:uid="{89643796-F484-D048-862D-B85A1B6BB907}" name="Special Format" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{89643796-F484-D048-862D-B85A1B6BB907}" name="Special Format" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F1FC7976-8703-F741-A840-3B88EF6176BE}" name="Table5" displayName="Table5" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6" xr:uid="{F1FC7976-8703-F741-A840-3B88EF6176BE}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{A8B448A4-30B1-C440-902C-9B91549BC0DA}" name="Metric"/>
+    <tableColumn id="2" xr3:uid="{BECACC40-0E74-FD4D-AC89-15309A97E5C1}" name="Years"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3898,11 +4226,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:EA26"/>
+  <dimension ref="A1:EQ26"/>
   <sheetViews>
-    <sheetView zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AR33" sqref="AR33"/>
+    <sheetView zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="BB1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BE9" sqref="BE9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3962,9 +4290,26 @@
     <col min="63" max="63" width="55.1640625" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="52.5" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="54.5" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="68" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="36.83203125" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="59" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="73.6640625" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="74.83203125" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="76.83203125" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="76.33203125" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="79.6640625" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="59" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="73.6640625" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="74.83203125" bestFit="1" customWidth="1"/>
+    <col min="145" max="145" width="76.83203125" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="76.33203125" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="79.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:131" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:147" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4353,13 +4698,61 @@
         <v>326</v>
       </c>
       <c r="DZ1" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="EA1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="2" spans="1:131" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+      <c r="EB1" t="s">
+        <v>403</v>
+      </c>
+      <c r="EC1" t="s">
+        <v>404</v>
+      </c>
+      <c r="ED1" t="s">
+        <v>405</v>
+      </c>
+      <c r="EE1" t="s">
+        <v>406</v>
+      </c>
+      <c r="EF1" t="s">
+        <v>407</v>
+      </c>
+      <c r="EG1" t="s">
+        <v>419</v>
+      </c>
+      <c r="EH1" t="s">
+        <v>409</v>
+      </c>
+      <c r="EI1" t="s">
+        <v>410</v>
+      </c>
+      <c r="EJ1" t="s">
+        <v>411</v>
+      </c>
+      <c r="EK1" t="s">
+        <v>412</v>
+      </c>
+      <c r="EL1" t="s">
+        <v>413</v>
+      </c>
+      <c r="EM1" t="s">
+        <v>420</v>
+      </c>
+      <c r="EN1" t="s">
+        <v>415</v>
+      </c>
+      <c r="EO1" t="s">
+        <v>416</v>
+      </c>
+      <c r="EP1" t="s">
+        <v>417</v>
+      </c>
+      <c r="EQ1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="2" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2008</v>
       </c>
@@ -4416,7 +4809,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:131" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2009</v>
       </c>
@@ -4473,7 +4866,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:131" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2010</v>
       </c>
@@ -4530,7 +4923,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="5" spans="1:131" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2011</v>
       </c>
@@ -4587,7 +4980,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:131" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2012</v>
       </c>
@@ -4644,7 +5037,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="7" spans="1:131" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2013</v>
       </c>
@@ -4701,7 +5094,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="8" spans="1:131" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2014</v>
       </c>
@@ -4766,8 +5159,14 @@
       <c r="BD8" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="9" spans="1:131" x14ac:dyDescent="0.2">
+      <c r="EF8" t="s">
+        <v>424</v>
+      </c>
+      <c r="EL8" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="9" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2015</v>
       </c>
@@ -4835,8 +5234,14 @@
       <c r="BD9" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="10" spans="1:131" x14ac:dyDescent="0.2">
+      <c r="EF9" t="s">
+        <v>424</v>
+      </c>
+      <c r="EL9" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="10" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2016</v>
       </c>
@@ -4949,8 +5354,17 @@
       <c r="BM10" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="11" spans="1:131" x14ac:dyDescent="0.2">
+      <c r="EB10" t="s">
+        <v>398</v>
+      </c>
+      <c r="EF10" t="s">
+        <v>424</v>
+      </c>
+      <c r="EL10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="11" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2017</v>
       </c>
@@ -5063,8 +5477,17 @@
       <c r="BM11" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="12" spans="1:131" x14ac:dyDescent="0.2">
+      <c r="EB11" t="s">
+        <v>398</v>
+      </c>
+      <c r="EF11" t="s">
+        <v>424</v>
+      </c>
+      <c r="EL11" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="12" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -5203,8 +5626,26 @@
       <c r="BM12" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="13" spans="1:131" x14ac:dyDescent="0.2">
+      <c r="EB12" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC12" t="s">
+        <v>400</v>
+      </c>
+      <c r="ED12" t="s">
+        <v>401</v>
+      </c>
+      <c r="EE12" t="s">
+        <v>402</v>
+      </c>
+      <c r="EF12" t="s">
+        <v>422</v>
+      </c>
+      <c r="EL12" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="13" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2019</v>
       </c>
@@ -5550,8 +5991,56 @@
       <c r="DY13" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="14" spans="1:131" x14ac:dyDescent="0.2">
+      <c r="EB13" t="s">
+        <v>403</v>
+      </c>
+      <c r="EC13" t="s">
+        <v>404</v>
+      </c>
+      <c r="ED13" t="s">
+        <v>405</v>
+      </c>
+      <c r="EE13" t="s">
+        <v>406</v>
+      </c>
+      <c r="EF13" t="s">
+        <v>407</v>
+      </c>
+      <c r="EG13" t="s">
+        <v>408</v>
+      </c>
+      <c r="EH13" t="s">
+        <v>409</v>
+      </c>
+      <c r="EI13" t="s">
+        <v>410</v>
+      </c>
+      <c r="EJ13" t="s">
+        <v>411</v>
+      </c>
+      <c r="EK13" t="s">
+        <v>412</v>
+      </c>
+      <c r="EL13" t="s">
+        <v>413</v>
+      </c>
+      <c r="EM13" t="s">
+        <v>414</v>
+      </c>
+      <c r="EN13" t="s">
+        <v>415</v>
+      </c>
+      <c r="EO13" t="s">
+        <v>416</v>
+      </c>
+      <c r="EP13" t="s">
+        <v>417</v>
+      </c>
+      <c r="EQ13" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="14" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2020</v>
       </c>
@@ -5705,8 +6194,56 @@
       <c r="BM14" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="15" spans="1:131" x14ac:dyDescent="0.2">
+      <c r="EB14" t="s">
+        <v>403</v>
+      </c>
+      <c r="EC14" t="s">
+        <v>404</v>
+      </c>
+      <c r="ED14" t="s">
+        <v>405</v>
+      </c>
+      <c r="EE14" t="s">
+        <v>406</v>
+      </c>
+      <c r="EF14" t="s">
+        <v>407</v>
+      </c>
+      <c r="EG14" t="s">
+        <v>419</v>
+      </c>
+      <c r="EH14" t="s">
+        <v>409</v>
+      </c>
+      <c r="EI14" t="s">
+        <v>410</v>
+      </c>
+      <c r="EJ14" t="s">
+        <v>411</v>
+      </c>
+      <c r="EK14" t="s">
+        <v>412</v>
+      </c>
+      <c r="EL14" t="s">
+        <v>413</v>
+      </c>
+      <c r="EM14" t="s">
+        <v>420</v>
+      </c>
+      <c r="EN14" t="s">
+        <v>415</v>
+      </c>
+      <c r="EO14" t="s">
+        <v>416</v>
+      </c>
+      <c r="EP14" t="s">
+        <v>417</v>
+      </c>
+      <c r="EQ14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="15" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2021</v>
       </c>
@@ -6058,8 +6595,56 @@
       <c r="DY15" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="16" spans="1:131" x14ac:dyDescent="0.2">
+      <c r="EB15" t="s">
+        <v>403</v>
+      </c>
+      <c r="EC15" t="s">
+        <v>404</v>
+      </c>
+      <c r="ED15" t="s">
+        <v>405</v>
+      </c>
+      <c r="EE15" t="s">
+        <v>406</v>
+      </c>
+      <c r="EF15" t="s">
+        <v>407</v>
+      </c>
+      <c r="EG15" t="s">
+        <v>419</v>
+      </c>
+      <c r="EH15" t="s">
+        <v>409</v>
+      </c>
+      <c r="EI15" t="s">
+        <v>410</v>
+      </c>
+      <c r="EJ15" t="s">
+        <v>411</v>
+      </c>
+      <c r="EK15" t="s">
+        <v>412</v>
+      </c>
+      <c r="EL15" t="s">
+        <v>413</v>
+      </c>
+      <c r="EM15" t="s">
+        <v>420</v>
+      </c>
+      <c r="EN15" t="s">
+        <v>415</v>
+      </c>
+      <c r="EO15" t="s">
+        <v>416</v>
+      </c>
+      <c r="EP15" t="s">
+        <v>417</v>
+      </c>
+      <c r="EQ15" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="16" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2022</v>
       </c>
@@ -6429,8 +7014,56 @@
       <c r="EA16" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="17" spans="1:131" x14ac:dyDescent="0.2">
+      <c r="EB16" t="s">
+        <v>403</v>
+      </c>
+      <c r="EC16" t="s">
+        <v>404</v>
+      </c>
+      <c r="ED16" t="s">
+        <v>405</v>
+      </c>
+      <c r="EE16" t="s">
+        <v>406</v>
+      </c>
+      <c r="EF16" t="s">
+        <v>407</v>
+      </c>
+      <c r="EG16" t="s">
+        <v>419</v>
+      </c>
+      <c r="EH16" t="s">
+        <v>409</v>
+      </c>
+      <c r="EI16" t="s">
+        <v>410</v>
+      </c>
+      <c r="EJ16" t="s">
+        <v>411</v>
+      </c>
+      <c r="EK16" t="s">
+        <v>412</v>
+      </c>
+      <c r="EL16" t="s">
+        <v>413</v>
+      </c>
+      <c r="EM16" t="s">
+        <v>420</v>
+      </c>
+      <c r="EN16" t="s">
+        <v>415</v>
+      </c>
+      <c r="EO16" t="s">
+        <v>416</v>
+      </c>
+      <c r="EP16" t="s">
+        <v>417</v>
+      </c>
+      <c r="EQ16" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="17" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2023</v>
       </c>
@@ -6815,11 +7448,59 @@
       <c r="EA17" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="19" spans="1:131" x14ac:dyDescent="0.2">
+      <c r="EB17" t="s">
+        <v>403</v>
+      </c>
+      <c r="EC17" t="s">
+        <v>404</v>
+      </c>
+      <c r="ED17" t="s">
+        <v>405</v>
+      </c>
+      <c r="EE17" t="s">
+        <v>406</v>
+      </c>
+      <c r="EF17" t="s">
+        <v>407</v>
+      </c>
+      <c r="EG17" t="s">
+        <v>419</v>
+      </c>
+      <c r="EH17" t="s">
+        <v>409</v>
+      </c>
+      <c r="EI17" t="s">
+        <v>410</v>
+      </c>
+      <c r="EJ17" t="s">
+        <v>411</v>
+      </c>
+      <c r="EK17" t="s">
+        <v>412</v>
+      </c>
+      <c r="EL17" t="s">
+        <v>413</v>
+      </c>
+      <c r="EM17" t="s">
+        <v>420</v>
+      </c>
+      <c r="EN17" t="s">
+        <v>415</v>
+      </c>
+      <c r="EO17" t="s">
+        <v>416</v>
+      </c>
+      <c r="EP17" t="s">
+        <v>417</v>
+      </c>
+      <c r="EQ17" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="19" spans="1:147" x14ac:dyDescent="0.2">
       <c r="BD19" s="18"/>
     </row>
-    <row r="26" spans="1:131" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:147" x14ac:dyDescent="0.2">
       <c r="AP26" s="16"/>
     </row>
   </sheetData>
@@ -6834,12 +7515,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249B090D-D7BB-374A-9D81-FFCE8C0599DD}">
-  <dimension ref="A1:H794"/>
+  <dimension ref="A1:H890"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A773" zoomScale="200" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A792" zoomScale="161" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A162" sqref="A162"/>
-      <selection pane="topRight" activeCell="B787" sqref="B787"/>
+      <selection pane="topRight" activeCell="C885" sqref="C885"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22051,7 +22732,7 @@
         <v>2022</v>
       </c>
       <c r="B791" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="C791" t="s">
         <v>387</v>
@@ -22071,7 +22752,7 @@
         <v>2023</v>
       </c>
       <c r="B792" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="C792" t="s">
         <v>387</v>
@@ -22091,7 +22772,7 @@
         <v>2022</v>
       </c>
       <c r="B793" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="C793" t="s">
         <v>388</v>
@@ -22111,7 +22792,7 @@
         <v>2023</v>
       </c>
       <c r="B794" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="C794" t="s">
         <v>388</v>
@@ -22124,6 +22805,1638 @@
       </c>
       <c r="G794" t="s">
         <v>391</v>
+      </c>
+    </row>
+    <row r="795" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A795">
+        <v>2016</v>
+      </c>
+      <c r="B795" t="s">
+        <v>398</v>
+      </c>
+      <c r="C795" t="s">
+        <v>403</v>
+      </c>
+      <c r="D795" t="s">
+        <v>34</v>
+      </c>
+      <c r="E795" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="796" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A796">
+        <v>2017</v>
+      </c>
+      <c r="B796" t="s">
+        <v>398</v>
+      </c>
+      <c r="C796" t="s">
+        <v>403</v>
+      </c>
+      <c r="D796" t="s">
+        <v>34</v>
+      </c>
+      <c r="E796" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="797" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A797">
+        <v>2018</v>
+      </c>
+      <c r="B797" t="s">
+        <v>399</v>
+      </c>
+      <c r="C797" t="s">
+        <v>403</v>
+      </c>
+      <c r="D797" t="s">
+        <v>34</v>
+      </c>
+      <c r="E797" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="798" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A798">
+        <v>2019</v>
+      </c>
+      <c r="B798" t="s">
+        <v>403</v>
+      </c>
+      <c r="C798" t="s">
+        <v>403</v>
+      </c>
+      <c r="D798" t="s">
+        <v>34</v>
+      </c>
+      <c r="E798" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="799" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A799">
+        <v>2020</v>
+      </c>
+      <c r="B799" t="s">
+        <v>403</v>
+      </c>
+      <c r="C799" t="s">
+        <v>403</v>
+      </c>
+      <c r="D799" t="s">
+        <v>34</v>
+      </c>
+      <c r="E799" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="800" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A800">
+        <v>2021</v>
+      </c>
+      <c r="B800" t="s">
+        <v>403</v>
+      </c>
+      <c r="C800" t="s">
+        <v>403</v>
+      </c>
+      <c r="D800" t="s">
+        <v>34</v>
+      </c>
+      <c r="E800" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="801" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A801">
+        <v>2022</v>
+      </c>
+      <c r="B801" t="s">
+        <v>403</v>
+      </c>
+      <c r="C801" t="s">
+        <v>403</v>
+      </c>
+      <c r="D801" t="s">
+        <v>34</v>
+      </c>
+      <c r="E801" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="802" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A802">
+        <v>2023</v>
+      </c>
+      <c r="B802" t="s">
+        <v>403</v>
+      </c>
+      <c r="C802" t="s">
+        <v>403</v>
+      </c>
+      <c r="D802" t="s">
+        <v>34</v>
+      </c>
+      <c r="E802" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="803" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A803">
+        <v>2018</v>
+      </c>
+      <c r="B803" t="s">
+        <v>400</v>
+      </c>
+      <c r="C803" t="s">
+        <v>404</v>
+      </c>
+      <c r="D803" t="s">
+        <v>34</v>
+      </c>
+      <c r="E803" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="804" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A804">
+        <v>2019</v>
+      </c>
+      <c r="B804" t="s">
+        <v>404</v>
+      </c>
+      <c r="C804" t="s">
+        <v>404</v>
+      </c>
+      <c r="D804" t="s">
+        <v>34</v>
+      </c>
+      <c r="E804" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="805" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A805">
+        <v>2020</v>
+      </c>
+      <c r="B805" t="s">
+        <v>404</v>
+      </c>
+      <c r="C805" t="s">
+        <v>404</v>
+      </c>
+      <c r="D805" t="s">
+        <v>34</v>
+      </c>
+      <c r="E805" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="806" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A806">
+        <v>2021</v>
+      </c>
+      <c r="B806" t="s">
+        <v>404</v>
+      </c>
+      <c r="C806" t="s">
+        <v>404</v>
+      </c>
+      <c r="D806" t="s">
+        <v>34</v>
+      </c>
+      <c r="E806" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="807" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A807">
+        <v>2022</v>
+      </c>
+      <c r="B807" t="s">
+        <v>404</v>
+      </c>
+      <c r="C807" t="s">
+        <v>404</v>
+      </c>
+      <c r="D807" t="s">
+        <v>34</v>
+      </c>
+      <c r="E807" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="808" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A808">
+        <v>2023</v>
+      </c>
+      <c r="B808" t="s">
+        <v>404</v>
+      </c>
+      <c r="C808" t="s">
+        <v>404</v>
+      </c>
+      <c r="D808" t="s">
+        <v>34</v>
+      </c>
+      <c r="E808" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="809" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A809">
+        <v>2018</v>
+      </c>
+      <c r="B809" t="s">
+        <v>401</v>
+      </c>
+      <c r="C809" t="s">
+        <v>405</v>
+      </c>
+      <c r="D809" t="s">
+        <v>34</v>
+      </c>
+      <c r="E809" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="810" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A810">
+        <v>2019</v>
+      </c>
+      <c r="B810" t="s">
+        <v>405</v>
+      </c>
+      <c r="C810" t="s">
+        <v>405</v>
+      </c>
+      <c r="D810" t="s">
+        <v>34</v>
+      </c>
+      <c r="E810" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="811" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A811">
+        <v>2020</v>
+      </c>
+      <c r="B811" t="s">
+        <v>405</v>
+      </c>
+      <c r="C811" t="s">
+        <v>405</v>
+      </c>
+      <c r="D811" t="s">
+        <v>34</v>
+      </c>
+      <c r="E811" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="812" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A812">
+        <v>2021</v>
+      </c>
+      <c r="B812" t="s">
+        <v>405</v>
+      </c>
+      <c r="C812" t="s">
+        <v>405</v>
+      </c>
+      <c r="D812" t="s">
+        <v>34</v>
+      </c>
+      <c r="E812" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="813" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A813">
+        <v>2022</v>
+      </c>
+      <c r="B813" t="s">
+        <v>405</v>
+      </c>
+      <c r="C813" t="s">
+        <v>405</v>
+      </c>
+      <c r="D813" t="s">
+        <v>34</v>
+      </c>
+      <c r="E813" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="814" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A814">
+        <v>2023</v>
+      </c>
+      <c r="B814" t="s">
+        <v>405</v>
+      </c>
+      <c r="C814" t="s">
+        <v>405</v>
+      </c>
+      <c r="D814" t="s">
+        <v>34</v>
+      </c>
+      <c r="E814" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="815" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A815">
+        <v>2018</v>
+      </c>
+      <c r="B815" t="s">
+        <v>402</v>
+      </c>
+      <c r="C815" t="s">
+        <v>406</v>
+      </c>
+      <c r="D815" t="s">
+        <v>34</v>
+      </c>
+      <c r="E815" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="816" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A816">
+        <v>2019</v>
+      </c>
+      <c r="B816" t="s">
+        <v>406</v>
+      </c>
+      <c r="C816" t="s">
+        <v>406</v>
+      </c>
+      <c r="D816" t="s">
+        <v>34</v>
+      </c>
+      <c r="E816" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="817" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A817">
+        <v>2020</v>
+      </c>
+      <c r="B817" t="s">
+        <v>406</v>
+      </c>
+      <c r="C817" t="s">
+        <v>406</v>
+      </c>
+      <c r="D817" t="s">
+        <v>34</v>
+      </c>
+      <c r="E817" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="818" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A818">
+        <v>2021</v>
+      </c>
+      <c r="B818" t="s">
+        <v>406</v>
+      </c>
+      <c r="C818" t="s">
+        <v>406</v>
+      </c>
+      <c r="D818" t="s">
+        <v>34</v>
+      </c>
+      <c r="E818" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="819" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A819">
+        <v>2022</v>
+      </c>
+      <c r="B819" t="s">
+        <v>406</v>
+      </c>
+      <c r="C819" t="s">
+        <v>406</v>
+      </c>
+      <c r="D819" t="s">
+        <v>34</v>
+      </c>
+      <c r="E819" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="820" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A820">
+        <v>2023</v>
+      </c>
+      <c r="B820" t="s">
+        <v>406</v>
+      </c>
+      <c r="C820" t="s">
+        <v>406</v>
+      </c>
+      <c r="D820" t="s">
+        <v>34</v>
+      </c>
+      <c r="E820" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="821" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A821" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B821" t="s">
+        <v>407</v>
+      </c>
+      <c r="C821" t="s">
+        <v>407</v>
+      </c>
+      <c r="D821" t="s">
+        <v>34</v>
+      </c>
+      <c r="E821" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="822" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A822" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B822" t="s">
+        <v>407</v>
+      </c>
+      <c r="C822" t="s">
+        <v>407</v>
+      </c>
+      <c r="D822" t="s">
+        <v>34</v>
+      </c>
+      <c r="E822" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="823" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A823" s="7">
+        <v>2021</v>
+      </c>
+      <c r="B823" t="s">
+        <v>407</v>
+      </c>
+      <c r="C823" t="s">
+        <v>407</v>
+      </c>
+      <c r="D823" t="s">
+        <v>34</v>
+      </c>
+      <c r="E823" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="824" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A824" s="7">
+        <v>2022</v>
+      </c>
+      <c r="B824" t="s">
+        <v>407</v>
+      </c>
+      <c r="C824" t="s">
+        <v>407</v>
+      </c>
+      <c r="D824" t="s">
+        <v>34</v>
+      </c>
+      <c r="E824" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="825" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A825" s="7">
+        <v>2023</v>
+      </c>
+      <c r="B825" t="s">
+        <v>407</v>
+      </c>
+      <c r="C825" t="s">
+        <v>407</v>
+      </c>
+      <c r="D825" t="s">
+        <v>34</v>
+      </c>
+      <c r="E825" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="826" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A826" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B826" t="s">
+        <v>408</v>
+      </c>
+      <c r="C826" t="s">
+        <v>408</v>
+      </c>
+      <c r="D826" t="s">
+        <v>34</v>
+      </c>
+      <c r="E826" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="827" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A827" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B827" t="s">
+        <v>419</v>
+      </c>
+      <c r="C827" t="s">
+        <v>419</v>
+      </c>
+      <c r="D827" t="s">
+        <v>34</v>
+      </c>
+      <c r="E827" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="828" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A828" s="7">
+        <v>2021</v>
+      </c>
+      <c r="B828" t="s">
+        <v>419</v>
+      </c>
+      <c r="C828" t="s">
+        <v>419</v>
+      </c>
+      <c r="D828" t="s">
+        <v>34</v>
+      </c>
+      <c r="E828" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="829" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A829" s="7">
+        <v>2022</v>
+      </c>
+      <c r="B829" t="s">
+        <v>419</v>
+      </c>
+      <c r="C829" t="s">
+        <v>419</v>
+      </c>
+      <c r="D829" t="s">
+        <v>34</v>
+      </c>
+      <c r="E829" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="830" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A830" s="7">
+        <v>2023</v>
+      </c>
+      <c r="B830" t="s">
+        <v>419</v>
+      </c>
+      <c r="C830" t="s">
+        <v>419</v>
+      </c>
+      <c r="D830" t="s">
+        <v>34</v>
+      </c>
+      <c r="E830" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="831" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A831" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B831" t="s">
+        <v>409</v>
+      </c>
+      <c r="C831" t="s">
+        <v>409</v>
+      </c>
+      <c r="D831" t="s">
+        <v>34</v>
+      </c>
+      <c r="E831" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="832" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A832" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B832" t="s">
+        <v>409</v>
+      </c>
+      <c r="C832" t="s">
+        <v>409</v>
+      </c>
+      <c r="D832" t="s">
+        <v>34</v>
+      </c>
+      <c r="E832" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="833" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A833" s="7">
+        <v>2021</v>
+      </c>
+      <c r="B833" t="s">
+        <v>409</v>
+      </c>
+      <c r="C833" t="s">
+        <v>409</v>
+      </c>
+      <c r="D833" t="s">
+        <v>34</v>
+      </c>
+      <c r="E833" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="834" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A834" s="7">
+        <v>2022</v>
+      </c>
+      <c r="B834" t="s">
+        <v>409</v>
+      </c>
+      <c r="C834" t="s">
+        <v>409</v>
+      </c>
+      <c r="D834" t="s">
+        <v>34</v>
+      </c>
+      <c r="E834" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="835" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A835" s="7">
+        <v>2023</v>
+      </c>
+      <c r="B835" t="s">
+        <v>409</v>
+      </c>
+      <c r="C835" t="s">
+        <v>409</v>
+      </c>
+      <c r="D835" t="s">
+        <v>34</v>
+      </c>
+      <c r="E835" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="836" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A836" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B836" t="s">
+        <v>410</v>
+      </c>
+      <c r="C836" t="s">
+        <v>410</v>
+      </c>
+      <c r="D836" t="s">
+        <v>34</v>
+      </c>
+      <c r="E836" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="837" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A837" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B837" t="s">
+        <v>410</v>
+      </c>
+      <c r="C837" t="s">
+        <v>410</v>
+      </c>
+      <c r="D837" t="s">
+        <v>34</v>
+      </c>
+      <c r="E837" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="838" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A838" s="7">
+        <v>2021</v>
+      </c>
+      <c r="B838" t="s">
+        <v>410</v>
+      </c>
+      <c r="C838" t="s">
+        <v>410</v>
+      </c>
+      <c r="D838" t="s">
+        <v>34</v>
+      </c>
+      <c r="E838" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="839" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A839" s="7">
+        <v>2022</v>
+      </c>
+      <c r="B839" t="s">
+        <v>410</v>
+      </c>
+      <c r="C839" t="s">
+        <v>410</v>
+      </c>
+      <c r="D839" t="s">
+        <v>34</v>
+      </c>
+      <c r="E839" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="840" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A840" s="7">
+        <v>2023</v>
+      </c>
+      <c r="B840" t="s">
+        <v>410</v>
+      </c>
+      <c r="C840" t="s">
+        <v>410</v>
+      </c>
+      <c r="D840" t="s">
+        <v>34</v>
+      </c>
+      <c r="E840" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="841" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A841" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B841" t="s">
+        <v>411</v>
+      </c>
+      <c r="C841" t="s">
+        <v>411</v>
+      </c>
+      <c r="D841" t="s">
+        <v>34</v>
+      </c>
+      <c r="E841" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="842" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A842" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B842" t="s">
+        <v>411</v>
+      </c>
+      <c r="C842" t="s">
+        <v>411</v>
+      </c>
+      <c r="D842" t="s">
+        <v>34</v>
+      </c>
+      <c r="E842" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="843" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A843" s="7">
+        <v>2021</v>
+      </c>
+      <c r="B843" t="s">
+        <v>411</v>
+      </c>
+      <c r="C843" t="s">
+        <v>411</v>
+      </c>
+      <c r="D843" t="s">
+        <v>34</v>
+      </c>
+      <c r="E843" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="844" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A844" s="7">
+        <v>2022</v>
+      </c>
+      <c r="B844" t="s">
+        <v>411</v>
+      </c>
+      <c r="C844" t="s">
+        <v>411</v>
+      </c>
+      <c r="D844" t="s">
+        <v>34</v>
+      </c>
+      <c r="E844" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="845" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A845" s="7">
+        <v>2023</v>
+      </c>
+      <c r="B845" t="s">
+        <v>411</v>
+      </c>
+      <c r="C845" t="s">
+        <v>411</v>
+      </c>
+      <c r="D845" t="s">
+        <v>34</v>
+      </c>
+      <c r="E845" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="846" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A846" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B846" t="s">
+        <v>412</v>
+      </c>
+      <c r="C846" t="s">
+        <v>412</v>
+      </c>
+      <c r="D846" t="s">
+        <v>34</v>
+      </c>
+      <c r="E846" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="847" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A847" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B847" t="s">
+        <v>412</v>
+      </c>
+      <c r="C847" t="s">
+        <v>412</v>
+      </c>
+      <c r="D847" t="s">
+        <v>34</v>
+      </c>
+      <c r="E847" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="848" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A848" s="7">
+        <v>2021</v>
+      </c>
+      <c r="B848" t="s">
+        <v>412</v>
+      </c>
+      <c r="C848" t="s">
+        <v>412</v>
+      </c>
+      <c r="D848" t="s">
+        <v>34</v>
+      </c>
+      <c r="E848" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="849" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A849" s="7">
+        <v>2022</v>
+      </c>
+      <c r="B849" t="s">
+        <v>412</v>
+      </c>
+      <c r="C849" t="s">
+        <v>412</v>
+      </c>
+      <c r="D849" t="s">
+        <v>34</v>
+      </c>
+      <c r="E849" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="850" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A850" s="7">
+        <v>2023</v>
+      </c>
+      <c r="B850" t="s">
+        <v>412</v>
+      </c>
+      <c r="C850" t="s">
+        <v>412</v>
+      </c>
+      <c r="D850" t="s">
+        <v>34</v>
+      </c>
+      <c r="E850" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="851" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A851" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B851" t="s">
+        <v>413</v>
+      </c>
+      <c r="C851" t="s">
+        <v>413</v>
+      </c>
+      <c r="D851" t="s">
+        <v>34</v>
+      </c>
+      <c r="E851" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="852" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A852" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B852" t="s">
+        <v>413</v>
+      </c>
+      <c r="C852" t="s">
+        <v>413</v>
+      </c>
+      <c r="D852" t="s">
+        <v>34</v>
+      </c>
+      <c r="E852" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="853" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A853" s="7">
+        <v>2021</v>
+      </c>
+      <c r="B853" t="s">
+        <v>413</v>
+      </c>
+      <c r="C853" t="s">
+        <v>413</v>
+      </c>
+      <c r="D853" t="s">
+        <v>34</v>
+      </c>
+      <c r="E853" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="854" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A854" s="7">
+        <v>2022</v>
+      </c>
+      <c r="B854" t="s">
+        <v>413</v>
+      </c>
+      <c r="C854" t="s">
+        <v>413</v>
+      </c>
+      <c r="D854" t="s">
+        <v>34</v>
+      </c>
+      <c r="E854" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="855" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A855" s="7">
+        <v>2023</v>
+      </c>
+      <c r="B855" t="s">
+        <v>413</v>
+      </c>
+      <c r="C855" t="s">
+        <v>413</v>
+      </c>
+      <c r="D855" t="s">
+        <v>34</v>
+      </c>
+      <c r="E855" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="856" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A856" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B856" t="s">
+        <v>414</v>
+      </c>
+      <c r="C856" t="s">
+        <v>414</v>
+      </c>
+      <c r="D856" t="s">
+        <v>34</v>
+      </c>
+      <c r="E856" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="857" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A857" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B857" t="s">
+        <v>420</v>
+      </c>
+      <c r="C857" t="s">
+        <v>420</v>
+      </c>
+      <c r="D857" t="s">
+        <v>34</v>
+      </c>
+      <c r="E857" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="858" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A858" s="7">
+        <v>2021</v>
+      </c>
+      <c r="B858" t="s">
+        <v>420</v>
+      </c>
+      <c r="C858" t="s">
+        <v>420</v>
+      </c>
+      <c r="D858" t="s">
+        <v>34</v>
+      </c>
+      <c r="E858" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="859" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A859" s="7">
+        <v>2022</v>
+      </c>
+      <c r="B859" t="s">
+        <v>420</v>
+      </c>
+      <c r="C859" t="s">
+        <v>420</v>
+      </c>
+      <c r="D859" t="s">
+        <v>34</v>
+      </c>
+      <c r="E859" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="860" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A860" s="7">
+        <v>2023</v>
+      </c>
+      <c r="B860" t="s">
+        <v>420</v>
+      </c>
+      <c r="C860" t="s">
+        <v>420</v>
+      </c>
+      <c r="D860" t="s">
+        <v>34</v>
+      </c>
+      <c r="E860" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="861" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A861" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B861" t="s">
+        <v>415</v>
+      </c>
+      <c r="C861" t="s">
+        <v>415</v>
+      </c>
+      <c r="D861" t="s">
+        <v>34</v>
+      </c>
+      <c r="E861" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="862" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A862" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B862" t="s">
+        <v>415</v>
+      </c>
+      <c r="C862" t="s">
+        <v>415</v>
+      </c>
+      <c r="D862" t="s">
+        <v>34</v>
+      </c>
+      <c r="E862" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="863" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A863" s="7">
+        <v>2021</v>
+      </c>
+      <c r="B863" t="s">
+        <v>415</v>
+      </c>
+      <c r="C863" t="s">
+        <v>415</v>
+      </c>
+      <c r="D863" t="s">
+        <v>34</v>
+      </c>
+      <c r="E863" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="864" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A864" s="7">
+        <v>2022</v>
+      </c>
+      <c r="B864" t="s">
+        <v>415</v>
+      </c>
+      <c r="C864" t="s">
+        <v>415</v>
+      </c>
+      <c r="D864" t="s">
+        <v>34</v>
+      </c>
+      <c r="E864" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="865" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A865" s="7">
+        <v>2023</v>
+      </c>
+      <c r="B865" t="s">
+        <v>415</v>
+      </c>
+      <c r="C865" t="s">
+        <v>415</v>
+      </c>
+      <c r="D865" t="s">
+        <v>34</v>
+      </c>
+      <c r="E865" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="866" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A866" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B866" t="s">
+        <v>416</v>
+      </c>
+      <c r="C866" t="s">
+        <v>416</v>
+      </c>
+      <c r="D866" t="s">
+        <v>34</v>
+      </c>
+      <c r="E866" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="867" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A867" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B867" t="s">
+        <v>416</v>
+      </c>
+      <c r="C867" t="s">
+        <v>416</v>
+      </c>
+      <c r="D867" t="s">
+        <v>34</v>
+      </c>
+      <c r="E867" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="868" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A868" s="7">
+        <v>2021</v>
+      </c>
+      <c r="B868" t="s">
+        <v>416</v>
+      </c>
+      <c r="C868" t="s">
+        <v>416</v>
+      </c>
+      <c r="D868" t="s">
+        <v>34</v>
+      </c>
+      <c r="E868" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="869" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A869" s="7">
+        <v>2022</v>
+      </c>
+      <c r="B869" t="s">
+        <v>416</v>
+      </c>
+      <c r="C869" t="s">
+        <v>416</v>
+      </c>
+      <c r="D869" t="s">
+        <v>34</v>
+      </c>
+      <c r="E869" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="870" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A870" s="7">
+        <v>2023</v>
+      </c>
+      <c r="B870" t="s">
+        <v>416</v>
+      </c>
+      <c r="C870" t="s">
+        <v>416</v>
+      </c>
+      <c r="D870" t="s">
+        <v>34</v>
+      </c>
+      <c r="E870" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="871" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A871" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B871" t="s">
+        <v>417</v>
+      </c>
+      <c r="C871" t="s">
+        <v>417</v>
+      </c>
+      <c r="D871" t="s">
+        <v>34</v>
+      </c>
+      <c r="E871" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="872" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A872" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B872" t="s">
+        <v>417</v>
+      </c>
+      <c r="C872" t="s">
+        <v>417</v>
+      </c>
+      <c r="D872" t="s">
+        <v>34</v>
+      </c>
+      <c r="E872" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="873" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A873" s="7">
+        <v>2021</v>
+      </c>
+      <c r="B873" t="s">
+        <v>417</v>
+      </c>
+      <c r="C873" t="s">
+        <v>417</v>
+      </c>
+      <c r="D873" t="s">
+        <v>34</v>
+      </c>
+      <c r="E873" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="874" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A874" s="7">
+        <v>2022</v>
+      </c>
+      <c r="B874" t="s">
+        <v>417</v>
+      </c>
+      <c r="C874" t="s">
+        <v>417</v>
+      </c>
+      <c r="D874" t="s">
+        <v>34</v>
+      </c>
+      <c r="E874" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="875" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A875" s="7">
+        <v>2023</v>
+      </c>
+      <c r="B875" t="s">
+        <v>417</v>
+      </c>
+      <c r="C875" t="s">
+        <v>417</v>
+      </c>
+      <c r="D875" t="s">
+        <v>34</v>
+      </c>
+      <c r="E875" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="876" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A876" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B876" t="s">
+        <v>418</v>
+      </c>
+      <c r="C876" t="s">
+        <v>418</v>
+      </c>
+      <c r="D876" t="s">
+        <v>34</v>
+      </c>
+      <c r="E876" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="877" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A877" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B877" t="s">
+        <v>418</v>
+      </c>
+      <c r="C877" t="s">
+        <v>418</v>
+      </c>
+      <c r="D877" t="s">
+        <v>34</v>
+      </c>
+      <c r="E877" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="878" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A878" s="7">
+        <v>2021</v>
+      </c>
+      <c r="B878" t="s">
+        <v>418</v>
+      </c>
+      <c r="C878" t="s">
+        <v>418</v>
+      </c>
+      <c r="D878" t="s">
+        <v>34</v>
+      </c>
+      <c r="E878" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="879" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A879" s="7">
+        <v>2022</v>
+      </c>
+      <c r="B879" t="s">
+        <v>418</v>
+      </c>
+      <c r="C879" t="s">
+        <v>418</v>
+      </c>
+      <c r="D879" t="s">
+        <v>34</v>
+      </c>
+      <c r="E879" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="880" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A880" s="8">
+        <v>2023</v>
+      </c>
+      <c r="B880" t="s">
+        <v>418</v>
+      </c>
+      <c r="C880" t="s">
+        <v>418</v>
+      </c>
+      <c r="D880" t="s">
+        <v>34</v>
+      </c>
+      <c r="E880" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="881" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A881">
+        <v>2018</v>
+      </c>
+      <c r="B881" t="s">
+        <v>407</v>
+      </c>
+      <c r="C881" t="s">
+        <v>422</v>
+      </c>
+      <c r="D881" t="s">
+        <v>34</v>
+      </c>
+      <c r="E881" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="882" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A882">
+        <v>2018</v>
+      </c>
+      <c r="B882" t="s">
+        <v>413</v>
+      </c>
+      <c r="C882" t="s">
+        <v>421</v>
+      </c>
+      <c r="D882" t="s">
+        <v>34</v>
+      </c>
+      <c r="E882" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="883" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A883">
+        <v>2014</v>
+      </c>
+      <c r="B883" t="s">
+        <v>407</v>
+      </c>
+      <c r="C883" t="s">
+        <v>424</v>
+      </c>
+      <c r="D883" t="s">
+        <v>34</v>
+      </c>
+      <c r="E883" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="884" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A884">
+        <v>2015</v>
+      </c>
+      <c r="B884" t="s">
+        <v>407</v>
+      </c>
+      <c r="C884" t="s">
+        <v>424</v>
+      </c>
+      <c r="D884" t="s">
+        <v>34</v>
+      </c>
+      <c r="E884" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="885" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A885">
+        <v>2016</v>
+      </c>
+      <c r="B885" t="s">
+        <v>407</v>
+      </c>
+      <c r="C885" t="s">
+        <v>424</v>
+      </c>
+      <c r="D885" t="s">
+        <v>34</v>
+      </c>
+      <c r="E885" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="886" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A886">
+        <v>2017</v>
+      </c>
+      <c r="B886" t="s">
+        <v>407</v>
+      </c>
+      <c r="C886" t="s">
+        <v>424</v>
+      </c>
+      <c r="D886" t="s">
+        <v>34</v>
+      </c>
+      <c r="E886" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="887" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A887">
+        <v>2014</v>
+      </c>
+      <c r="B887" t="s">
+        <v>413</v>
+      </c>
+      <c r="C887" t="s">
+        <v>423</v>
+      </c>
+      <c r="D887" t="s">
+        <v>34</v>
+      </c>
+      <c r="E887" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="888" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A888">
+        <v>2015</v>
+      </c>
+      <c r="B888" t="s">
+        <v>413</v>
+      </c>
+      <c r="C888" t="s">
+        <v>423</v>
+      </c>
+      <c r="D888" t="s">
+        <v>34</v>
+      </c>
+      <c r="E888" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="889" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A889">
+        <v>2016</v>
+      </c>
+      <c r="B889" t="s">
+        <v>413</v>
+      </c>
+      <c r="C889" t="s">
+        <v>423</v>
+      </c>
+      <c r="D889" t="s">
+        <v>34</v>
+      </c>
+      <c r="E889" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="890" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A890">
+        <v>2017</v>
+      </c>
+      <c r="B890" t="s">
+        <v>413</v>
+      </c>
+      <c r="C890" t="s">
+        <v>423</v>
+      </c>
+      <c r="D890" t="s">
+        <v>34</v>
+      </c>
+      <c r="E890" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -22137,35 +24450,107 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8521E5FD-ABD7-A144-B5B7-B0A36A8953CC}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB1C15B-5597-114F-BDFB-8D8FF2D17734}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="38.83203125" customWidth="1"/>
+    <col min="2" max="2" width="63.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="128" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>431</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB1C15B-5597-114F-BDFB-8D8FF2D17734}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8521E5FD-ABD7-A144-B5B7-B0A36A8953CC}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="157" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="59" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B2">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B3" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B4" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B6" t="s">
+        <v>430</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6016504-2F1C-6243-97B3-0CBED110888D}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="209" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22190,32 +24575,41 @@
         <v>262</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>396</v>
+      </c>
+      <c r="B4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>425</v>
+      </c>
+      <c r="B5" t="s">
+        <v>426</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>#REF!="In Progress"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d5cc9fc5-cf59-440a-a506-890d57680064">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B598B773ED9FC644B8B740EB3205C8DA" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6cfe95817d5870f6c066b2c32ab5fb2a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xmlns:ns3="d5cc9fc5-cf59-440a-a506-890d57680064" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a231614a4bf4996e6f4146316e2aaf8" ns2:_="" ns3:_="">
     <xsd:import namespace="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
@@ -22478,32 +24872,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA6725D-5CB1-4E78-9F97-F79E79C18DA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="d5cc9fc5-cf59-440a-a506-890d57680064"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d5cc9fc5-cf59-440a-a506-890d57680064">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3FAF407-B1B6-4FB8-B534-293B9E1D533A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B298AB6-2F6D-497E-AD9E-0F97ABEC8463}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22520,4 +24909,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA6725D-5CB1-4E78-9F97-F79E79C18DA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d5cc9fc5-cf59-440a-a506-890d57680064"/>
+    <ds:schemaRef ds:uri="49e1d5e2-6a7b-461e-a08d-88c8bb8c4019"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3FAF407-B1B6-4FB8-B534-293B9E1D533A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>